<commit_message>
New File PP Regression1
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C1386-E7DC-432E-A5E2-8CED9797A221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF38F44-339B-4399-92F8-0DD0A259C22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alipay" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="326">
   <si>
     <t>CancellationFlag</t>
   </si>
@@ -508,40 +508,112 @@
     <t>\UploadExcel\JsonTemplates\CreditCardNewCustomer.json</t>
   </si>
   <si>
+    <t>20240702112604</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f41281569</t>
+  </si>
+  <si>
+    <t>20240702112604Test</t>
+  </si>
+  <si>
+    <t>20240702112604Auto</t>
+  </si>
+  <si>
+    <t>20240702112604@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e111a</t>
+  </si>
+  <si>
+    <t>e0c5210c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213165 for AS order 20240702112604</t>
+  </si>
+  <si>
+    <t>3213165</t>
+  </si>
+  <si>
+    <t>0000000135548858</t>
+  </si>
+  <si>
+    <t>0000000135550648</t>
+  </si>
+  <si>
+    <t>0000000135545948</t>
+  </si>
+  <si>
+    <t>20240701164345</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f29527164</t>
+  </si>
+  <si>
+    <t>20240701162813Test</t>
+  </si>
+  <si>
+    <t>20240701162813Auto</t>
+  </si>
+  <si>
+    <t>20240701162813@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e352a</t>
+  </si>
+  <si>
+    <t>e0c2155c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213146 for AS order 20240701164345</t>
+  </si>
+  <si>
+    <t>3213146</t>
+  </si>
+  <si>
+    <t>0000000135545558</t>
+  </si>
+  <si>
+    <t>0000000135548831</t>
+  </si>
+  <si>
+    <t>0000000135545561</t>
+  </si>
+  <si>
     <t>Alipay_CN</t>
   </si>
   <si>
-    <t>20240514120817</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f51469381</t>
-  </si>
-  <si>
-    <t>20240514120817Test</t>
-  </si>
-  <si>
-    <t>20240514120817Auto</t>
-  </si>
-  <si>
-    <t>20240514120817@Wiley.com</t>
-  </si>
-  <si>
-    <t>df1e950b-a1d7-45bf-acab-42f7ed3e282a</t>
-  </si>
-  <si>
-    <t>e0c6155c-ba2c-401d-b2a6-3fb3a59b3c00</t>
-  </si>
-  <si>
-    <t>Created Viax order 3211968 for AS order 20240514120817</t>
-  </si>
-  <si>
-    <t>3211968</t>
-  </si>
-  <si>
-    <t>0000000135364759</t>
-  </si>
-  <si>
-    <t>0000000135363232</t>
+    <t>20240701164842</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f37815148</t>
+  </si>
+  <si>
+    <t>20240701164842Test</t>
+  </si>
+  <si>
+    <t>20240701164842Auto</t>
+  </si>
+  <si>
+    <t>20240701164842@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e874a</t>
+  </si>
+  <si>
+    <t>e0c1685c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213147 for AS order 20240701164842</t>
+  </si>
+  <si>
+    <t>3213147</t>
+  </si>
+  <si>
+    <t>0000000135552204</t>
+  </si>
+  <si>
+    <t>0000000135545565</t>
   </si>
   <si>
     <t>Issue In Idoc or No Idoc Found</t>
@@ -550,25 +622,79 @@
     <t>AlipayExisting_CN</t>
   </si>
   <si>
-    <t>20240514122419</t>
-  </si>
-  <si>
-    <t>11ca99f1-8a00-4cb3-123e-222f72455517</t>
-  </si>
-  <si>
-    <t>df1e950b-a1d7-45bf-acab-42f7ed3e844a</t>
-  </si>
-  <si>
-    <t>e0c6325c-ba2c-401d-b2a6-3fb3a59b3c00</t>
-  </si>
-  <si>
-    <t>Created Viax order 3211969 for AS order 20240514122419</t>
-  </si>
-  <si>
-    <t>3211969</t>
-  </si>
-  <si>
-    <t>0000000135365558</t>
+    <t>20240701170549</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f40230129</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e599a</t>
+  </si>
+  <si>
+    <t>e0c2579c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213151 for AS order 20240701170549</t>
+  </si>
+  <si>
+    <t>0000000135550525</t>
+  </si>
+  <si>
+    <t>20240701171741</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f87863139</t>
+  </si>
+  <si>
+    <t>20240701171741Test</t>
+  </si>
+  <si>
+    <t>20240701171741Auto</t>
+  </si>
+  <si>
+    <t>20240701171741@Wiley.com</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e205a</t>
+  </si>
+  <si>
+    <t>e0c4172c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213152 for AS order 20240701171741</t>
+  </si>
+  <si>
+    <t>3213152</t>
+  </si>
+  <si>
+    <t>0000000135545585</t>
+  </si>
+  <si>
+    <t>0000000135545584</t>
+  </si>
+  <si>
+    <t>0000000135545586</t>
+  </si>
+  <si>
+    <t>20240701173354</t>
+  </si>
+  <si>
+    <t>11ca99f1-8a00-4cb3-123e-222f11482632</t>
+  </si>
+  <si>
+    <t>df1e950b-a1d7-45bf-acab-42f7ed3e140a</t>
+  </si>
+  <si>
+    <t>e0c6549c-ba2c-401d-b2a6-3fb3a59b3c00</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213153 for AS order 20240701173354</t>
+  </si>
+  <si>
+    <t>3213153</t>
+  </si>
+  <si>
+    <t>0000000135552217</t>
   </si>
   <si>
     <t>VIAXEnvironment</t>
@@ -601,10 +727,7 @@
     <t>c597beef-e45f-4cc7-b34c-0df812e2ef25</t>
   </si>
   <si>
-    <t>Created Viax order 7232464 for PriceProposal 24ef2382-783b-4808-9127-af8e42410407</t>
-  </si>
-  <si>
-    <t>7232464</t>
+    <t>Created Viax order 7236048 for PriceProposal 24ef6375-783b-4808-9127-af8e42410759</t>
   </si>
   <si>
     <t>PriceDetermined</t>
@@ -618,7 +741,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef2382-783b-4808-9127-af8e42410407",
+      "submissionId": "24ef6375-783b-4808-9127-af8e42410759",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -674,7 +797,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232464 for PriceProposal 24ef2382-783b-4808-9127-af8e42410407","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232464","priceProposal":{"uid":"667a5a0c-7a58-4c33-bbaf-8e3139c03af0","biId":"7232464","wAsSubmissionId":"24ef2382-783b-4808-9127-af8e42410407","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:47:56.585Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2382-783b-4808-9127-af8e42410407","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:47:57.061Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2382-783b-4808-9127-af8e42410407","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2382-783b-4808-9127-af8e42410407","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236048 for PriceProposal 24ef6375-783b-4808-9127-af8e42410759","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236048","priceProposal":{"uid":"6683cf65-573c-43d8-8366-e7429cbbd385","biId":"7236048","wAsSubmissionId":"24ef6375-783b-4808-9127-af8e42410759","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:01.653Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6375-783b-4808-9127-af8e42410759","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:02.178Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6375-783b-4808-9127-af8e42410759","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6375-783b-4808-9127-af8e42410759","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Promotional discount</t>
@@ -683,10 +806,10 @@
     <t>Promotional</t>
   </si>
   <si>
-    <t>Created Viax order 7232465 for PriceProposal 24ef2252-783b-4808-9127-af8e42410292</t>
-  </si>
-  <si>
-    <t>7232465</t>
+    <t>Created Viax order 7236049 for PriceProposal 24ef5688-783b-4808-9127-af8e42410761</t>
+  </si>
+  <si>
+    <t>7236049</t>
   </si>
   <si>
     <t>{
@@ -694,7 +817,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef2252-783b-4808-9127-af8e42410292",
+      "submissionId": "24ef5688-783b-4808-9127-af8e42410761",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -750,7 +873,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232465 for PriceProposal 24ef2252-783b-4808-9127-af8e42410292","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232465","priceProposal":{"uid":"667a5a10-96a4-4890-9772-c42c3b93a60f","biId":"7232465","wAsSubmissionId":"24ef2252-783b-4808-9127-af8e42410292","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:00.461Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2252-783b-4808-9127-af8e42410292","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:00.905Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2252-783b-4808-9127-af8e42410292","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2252-783b-4808-9127-af8e42410292","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236049 for PriceProposal 24ef5688-783b-4808-9127-af8e42410761","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236049","priceProposal":{"uid":"6683cf69-f057-44e3-b4ca-a517a48adb51","biId":"7236049","wAsSubmissionId":"24ef5688-783b-4808-9127-af8e42410761","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:05.710Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef5688-783b-4808-9127-af8e42410761","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:06.140Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5688-783b-4808-9127-af8e42410761","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef5688-783b-4808-9127-af8e42410761","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Institutional discount</t>
@@ -759,10 +882,10 @@
     <t>Institutional</t>
   </si>
   <si>
-    <t>Created Viax order 7232466 for PriceProposal 24ef4871-783b-4808-9127-af8e42410757</t>
-  </si>
-  <si>
-    <t>7232466</t>
+    <t>Created Viax order 7236050 for PriceProposal 24ef1093-783b-4808-9127-af8e42410467</t>
+  </si>
+  <si>
+    <t>7236050</t>
   </si>
   <si>
     <t>{
@@ -770,7 +893,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef4871-783b-4808-9127-af8e42410757",
+      "submissionId": "24ef1093-783b-4808-9127-af8e42410467",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -824,7 +947,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232466 for PriceProposal 24ef4871-783b-4808-9127-af8e42410757","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232466","priceProposal":{"uid":"667a5a16-12ac-4bf9-aa9e-06153c566ef4","biId":"7232466","wAsSubmissionId":"24ef4871-783b-4808-9127-af8e42410757","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:06.161Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4871-783b-4808-9127-af8e42410757","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-16","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:06.808Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4871-783b-4808-9127-af8e42410757","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef4871-783b-4808-9127-af8e42410757","wAsSubmissionDate":"2024-04-16","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236050 for PriceProposal 24ef1093-783b-4808-9127-af8e42410467","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236050","priceProposal":{"uid":"6683cf73-b182-4a96-a00b-becc0dcb413f","biId":"7236050","wAsSubmissionId":"24ef1093-783b-4808-9127-af8e42410467","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:15.755Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef1093-783b-4808-9127-af8e42410467","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-16","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:16.318Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1093-783b-4808-9127-af8e42410467","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1093-783b-4808-9127-af8e42410467","wAsSubmissionDate":"2024-04-16","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Editorial discount</t>
@@ -833,10 +956,10 @@
     <t>Editorial</t>
   </si>
   <si>
-    <t>Created Viax order 7232469 for PriceProposal 24ef9384-783b-4808-9127-af8e42410953</t>
-  </si>
-  <si>
-    <t>7232469</t>
+    <t>Created Viax order 7236051 for PriceProposal 24ef8267-783b-4808-9127-af8e42410133</t>
+  </si>
+  <si>
+    <t>7236051</t>
   </si>
   <si>
     <t>{
@@ -844,7 +967,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef9384-783b-4808-9127-af8e42410953",
+      "submissionId": "24ef8267-783b-4808-9127-af8e42410133",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -899,7 +1022,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232469 for PriceProposal 24ef9384-783b-4808-9127-af8e42410953","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232469","priceProposal":{"uid":"667a5a1a-ba34-4e46-87ca-344cc5b77e3f","biId":"7232469","wAsSubmissionId":"24ef9384-783b-4808-9127-af8e42410953","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:10.144Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef9384-783b-4808-9127-af8e42410953","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:10.556Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":0,"tax":0,"total":0,"discountAmount":640,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":null,"sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef9384-783b-4808-9127-af8e42410953","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef9384-783b-4808-9127-af8e42410953","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236051 for PriceProposal 24ef8267-783b-4808-9127-af8e42410133","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236051","priceProposal":{"uid":"6683cf79-051a-43f3-8398-c576c15bd46b","biId":"7236051","wAsSubmissionId":"24ef8267-783b-4808-9127-af8e42410133","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:21.179Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8267-783b-4808-9127-af8e42410133","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:22.352Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":0,"tax":0,"total":0,"discountAmount":640,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":null,"sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":640,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef8267-783b-4808-9127-af8e42410133","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8267-783b-4808-9127-af8e42410133","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Referral discount</t>
@@ -911,10 +1034,10 @@
     <t>1b28a8b9-067b-4ce9-b981-e8eabe16e0a7</t>
   </si>
   <si>
-    <t>Created Viax order 7232470 for PriceProposal 24ef9445-783b-4808-9127-af8e42410318</t>
-  </si>
-  <si>
-    <t>7232470</t>
+    <t>Created Viax order 7236052 for PriceProposal 24ef1284-783b-4808-9127-af8e42410880</t>
+  </si>
+  <si>
+    <t>7236052</t>
   </si>
   <si>
     <t>{
@@ -922,7 +1045,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef9445-783b-4808-9127-af8e42410318",
+      "submissionId": "24ef1284-783b-4808-9127-af8e42410880",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "1b28a8b9-067b-4ce9-b981-e8eabe16e0a7",
@@ -977,7 +1100,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232470 for PriceProposal 24ef9445-783b-4808-9127-af8e42410318","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232470","priceProposal":{"uid":"667a5a1d-267a-47f2-b3c6-1d54ee5437ff","biId":"7232470","wAsSubmissionId":"24ef9445-783b-4808-9127-af8e42410318","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:13.879Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef9445-783b-4808-9127-af8e42410318","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Have a goood day(*&amp;^%$#.","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:14.231Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsReferringJournalRef":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalEISSN":"14390272","wAsEditorialOfficeEmail":null},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":3450,"price":3450,"subtotal":3450,"tax":0,"total":3450,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Have a goood day(*&amp;^%$#.","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9445-783b-4808-9127-af8e42410318","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef9445-783b-4808-9127-af8e42410318","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"14390272","wAsFlipDate":"2022-09-21","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":null}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236052 for PriceProposal 24ef1284-783b-4808-9127-af8e42410880","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236052","priceProposal":{"uid":"6683cf7f-ba01-4774-961e-a86318934155","biId":"7236052","wAsSubmissionId":"24ef1284-783b-4808-9127-af8e42410880","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:27.208Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef1284-783b-4808-9127-af8e42410880","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Have a goood day(*&amp;^%$#.","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:27.649Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsReferringJournalRef":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalEISSN":"14390272","wAsEditorialOfficeEmail":null},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":3450,"price":3450,"subtotal":3450,"tax":0,"total":3450,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Have a goood day(*&amp;^%$#.","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1284-783b-4808-9127-af8e42410880","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1284-783b-4808-9127-af8e42410880","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"14390272","wAsFlipDate":"2022-09-21","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":null}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Geographical discount</t>
@@ -989,10 +1112,10 @@
     <t>b6d18dc5-3811-4b21-81f0-a01997c20001</t>
   </si>
   <si>
-    <t>Created Viax order 7232471 for PriceProposal 24ef5994-783b-4808-9127-af8e42410929</t>
-  </si>
-  <si>
-    <t>7232471</t>
+    <t>Created Viax order 7236053 for PriceProposal 24ef2470-783b-4808-9127-af8e42410841</t>
+  </si>
+  <si>
+    <t>7236053</t>
   </si>
   <si>
     <t>{
@@ -1000,7 +1123,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef5994-783b-4808-9127-af8e42410929",
+      "submissionId": "24ef2470-783b-4808-9127-af8e42410841",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "b6d18dc5-3811-4b21-81f0-a01997c20001",
@@ -1055,7 +1178,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232471 for PriceProposal 24ef5994-783b-4808-9127-af8e42410929","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232471","priceProposal":{"uid":"667a5a21-8b2c-4c43-b6c0-59eaeb0068ab","biId":"7232471","wAsSubmissionId":"24ef5994-783b-4808-9127-af8e42410929","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:17.362Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5994-783b-4808-9127-af8e42410929","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"EMTW5R","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:17.733Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":150,"subtotal":0,"tax":0,"total":0,"discountAmount":150,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"EMTW5R","discountType":"EditorialDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":"EDITORIAL","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"EMTW5R","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"OPINION","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":60,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"EMTW5R","biiSalable":{"maId":"24ef5994-783b-4808-9127-af8e42410929","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef5994-783b-4808-9127-af8e42410929","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236053 for PriceProposal 24ef2470-783b-4808-9127-af8e42410841","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236053","priceProposal":{"uid":"6683cf83-efcf-4761-b4d1-b2b28a9a5c65","biId":"7236053","wAsSubmissionId":"24ef2470-783b-4808-9127-af8e42410841","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:31.910Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef2470-783b-4808-9127-af8e42410841","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"EMTW5R","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:32.359Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":150,"subtotal":0,"tax":0,"total":0,"discountAmount":150,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"EMTW5R","discountType":"EditorialDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":"EDITORIAL","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"EMTW5R","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"OPINION","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":60,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":150,"discountPercentage":100,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":150,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"EMTW5R","biiSalable":{"maId":"24ef2470-783b-4808-9127-af8e42410841","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2470-783b-4808-9127-af8e42410841","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Article type discount</t>
@@ -1064,10 +1187,10 @@
     <t>ArticleType</t>
   </si>
   <si>
-    <t>Created Viax order 7232472 for PriceProposal 24ef6001-783b-4808-9127-af8e42410199</t>
-  </si>
-  <si>
-    <t>7232472</t>
+    <t>Created Viax order 7236054 for PriceProposal 24ef2890-783b-4808-9127-af8e42410382</t>
+  </si>
+  <si>
+    <t>7236054</t>
   </si>
   <si>
     <t>{
@@ -1075,7 +1198,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef6001-783b-4808-9127-af8e42410199",
+      "submissionId": "24ef2890-783b-4808-9127-af8e42410382",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1129,7 +1252,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232472 for PriceProposal 24ef6001-783b-4808-9127-af8e42410199","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232472","priceProposal":{"uid":"667a5a25-4ea3-4407-b07b-a6a26dfff3d6","biId":"7232472","wAsSubmissionId":"24ef6001-783b-4808-9127-af8e42410199","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:21.136Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6001-783b-4808-9127-af8e42410199","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:21.604Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6001-783b-4808-9127-af8e42410199","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6001-783b-4808-9127-af8e42410199","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236054 for PriceProposal 24ef2890-783b-4808-9127-af8e42410382","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236054","priceProposal":{"uid":"6683cf89-af29-4923-b59a-423f8149493b","biId":"7236054","wAsSubmissionId":"24ef2890-783b-4808-9127-af8e42410382","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:37.032Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef2890-783b-4808-9127-af8e42410382","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:37.482Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2890-783b-4808-9127-af8e42410382","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2890-783b-4808-9127-af8e42410382","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Stacked Institutional discount</t>
@@ -1138,13 +1261,10 @@
     <t>Stacked</t>
   </si>
   <si>
-    <t>Created Viax order 7232473 for PriceProposal 24ef3284-783b-4808-9127-af8e42410374</t>
-  </si>
-  <si>
-    <t>7232473</t>
-  </si>
-  <si>
-    <t>DataCorrectionRequired</t>
+    <t>Created Viax order 7236055 for PriceProposal 24ef8508-783b-4808-9127-af8e42410878</t>
+  </si>
+  <si>
+    <t>7236055</t>
   </si>
   <si>
     <t>{
@@ -1152,10 +1272,10 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef3284-783b-4808-9127-af8e42410374",
+      "submissionId": "24ef8508-783b-4808-9127-af8e42410878",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
-      "journalId": "1b28a8b9-067b-4ce9-b981-e8eabe16e0a7",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
@@ -1206,7 +1326,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232473 for PriceProposal 24ef3284-783b-4808-9127-af8e42410374","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232473","priceProposal":{"uid":"667a5a28-6885-42a7-97b1-e20c7bb01b0f","biId":"7232473","wAsSubmissionId":"24ef3284-783b-4808-9127-af8e42410374","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-06-25T05:48:24.653Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef3284-783b-4808-9127-af8e42410374","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:25.298Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"500","errorMessage":"Price calculation error. {}","fieldPath":"","fieldValue":""}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3284-783b-4808-9127-af8e42410374","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef3284-783b-4808-9127-af8e42410374","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"AND","maName":"Andrologia","wAsJournalUuid":"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"14390272","wAsFlipDate":"2022-09-21","wAsJournalTitle":"Andrologia","wAsJournalGroupCode":"AND","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":null}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236055 for PriceProposal 24ef8508-783b-4808-9127-af8e42410878","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236055","priceProposal":{"uid":"6683cf8d-4bec-43e0-9933-a9fd65e2b505","biId":"7236055","wAsSubmissionId":"24ef8508-783b-4808-9127-af8e42410878","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:41.183Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8508-783b-4808-9127-af8e42410878","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:41.799Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":2471,"price":617.75,"subtotal":0,"tax":0,"total":0,"discountAmount":617.75,"discountPercentage":100,"currencyCode":"GBP","allDiscounts":[{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":617.75,"discountPercentage":39.76851477134763,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O LAWRENCE BERKELEY NATIONAL LABORATORY","discountType":"Institutional","discountAmount":617.75,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8508-783b-4808-9127-af8e42410878","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8508-783b-4808-9127-af8e42410878","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with multiple Society and Promotional discounts</t>
@@ -1215,10 +1335,10 @@
     <t>SocietyPromo</t>
   </si>
   <si>
-    <t>Created Viax order 7232474 for PriceProposal 24ef2978-783b-4808-9127-af8e42410206</t>
-  </si>
-  <si>
-    <t>7232474</t>
+    <t>Created Viax order 7236056 for PriceProposal 24ef6804-783b-4808-9127-af8e42410110</t>
+  </si>
+  <si>
+    <t>7236056</t>
   </si>
   <si>
     <t>{
@@ -1226,7 +1346,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef2978-783b-4808-9127-af8e42410206",
+      "submissionId": "24ef6804-783b-4808-9127-af8e42410110",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1284,7 +1404,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232474 for PriceProposal 24ef2978-783b-4808-9127-af8e42410206","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232474","priceProposal":{"uid":"667a5a2b-1908-4bf7-ade8-ade6f377dcf6","biId":"7232474","wAsSubmissionId":"24ef2978-783b-4808-9127-af8e42410206","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:27.342Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2978-783b-4808-9127-af8e42410206","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-17","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:27.780Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2978-783b-4808-9127-af8e42410206","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2978-783b-4808-9127-af8e42410206","wAsSubmissionDate":"2024-04-17","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236056 for PriceProposal 24ef6804-783b-4808-9127-af8e42410110","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236056","priceProposal":{"uid":"6683cf91-da42-4e15-80c0-c0d121be7217","biId":"7236056","wAsSubmissionId":"24ef6804-783b-4808-9127-af8e42410110","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:45.584Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6804-783b-4808-9127-af8e42410110","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-17","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:46.112Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6804-783b-4808-9127-af8e42410110","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6804-783b-4808-9127-af8e42410110","wAsSubmissionDate":"2024-04-17","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with same discount Geographical Editorial and Society discounts</t>
@@ -1293,33 +1413,35 @@
     <t>GeoEditSociety</t>
   </si>
   <si>
-    <t>Error in Response</t>
+    <t>Created Viax order 7236057 for PriceProposal 24ef1931-783b-4808-9127-af8e42410691</t>
+  </si>
+  <si>
+    <t>7236057</t>
   </si>
   <si>
     <t>{
   "query": "mutation testFn( $data: Object) { testFunction(input: { name: \"receive-price-proposal-from-kafka\" data: { apiversion: \"1.0.1\" tenant: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" id: \"51014872-8dfd-11ed-a1eb-0242ac120002\" type: \"priceproposal.requested\" source: \"urn:appcat:cmh-eeolink\" specversion: \"1.0\" subject: \"0d961334-8e06-4973-9c4a-5524ebd33f55\" time: \"2019-08-24T14:15:22Z\" datacontenttype: \"application/json\" data: $data } } ) { status data }}",
   "variables": {
     "data": {
-      "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "5168a602-3307-4503-8576-aa709dd0d368",
+      "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
+      "submissionId": "24ef1931-783b-4808-9127-af8e42410691",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
-      "journalId": "3a634d93-aea6-4ba1-9cd2-08ec458c273b",
+      "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
-      "baseArticleType": "OPINION",
-      "displayArticleType": "OPINION",
-      "submissionDate": "2024-04-23",
+      "baseArticleType": "EDUCATION",
+      "displayArticleType": "Research Article (ABC)",
+      "submissionDate": "2024-04-17",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
       "isManualOverrideRequired": false,
       "manualOverrideInstructions": "string",
       "societyCodes": [
-        "MAU25"
+        "EANM9"
       ],
       "promoCodes": [],
       "discountCodes": [],
-      "editorialDiscountCode": "BES25",
       "authors": [
         {
           "role": "Corresponding Author",
@@ -1340,8 +1462,8 @@
                 }
               ],
               "addressLocality": "Aix en Provence",
-              "countryCode": "PE",
-              "country": "PE",
+              "countryCode": "BO",
+              "country": "BO",
               "institution": "Grant Institute",
               "department": "School of GeoSciences",
               "stateProvince": "New Jersey",
@@ -1358,7 +1480,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"FAILURE","errors":["Price proposal already created."],"errorCode":"P040","errorValue":"5168a602-3307-4503-8576-aa709dd0d368"}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236057 for PriceProposal 24ef1931-783b-4808-9127-af8e42410691","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236057","priceProposal":{"uid":"6683cf95-047f-4903-a1eb-be436fa537fb","biId":"7236057","wAsSubmissionId":"24ef1931-783b-4808-9127-af8e42410691","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:49.814Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef1931-783b-4808-9127-af8e42410691","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-17","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM9"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"BO","country":"BO","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:50.183Z"}},"wAsCountryCode":"BO","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":400,"tax":0,"total":400,"discountAmount":400,"discountPercentage":50,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"BO","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"BO","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1931-783b-4808-9127-af8e42410691","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1931-783b-4808-9127-af8e42410691","wAsSubmissionDate":"2024-04-17","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Society Promotional Geographical Editorial Article type and Referral discounts</t>
@@ -1367,10 +1489,10 @@
     <t>All</t>
   </si>
   <si>
-    <t>Created Viax order 7232475 for PriceProposal 24ef6713-783b-4808-9127-af8e42410444</t>
-  </si>
-  <si>
-    <t>7232475</t>
+    <t>Created Viax order 7236058 for PriceProposal 24ef4032-783b-4808-9127-af8e42410900</t>
+  </si>
+  <si>
+    <t>7236058</t>
   </si>
   <si>
     <t>{
@@ -1378,7 +1500,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef6713-783b-4808-9127-af8e42410444",
+      "submissionId": "24ef4032-783b-4808-9127-af8e42410900",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1438,7 +1560,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232475 for PriceProposal 24ef6713-783b-4808-9127-af8e42410444","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232475","priceProposal":{"uid":"667a5a30-ae6a-4d2b-b3aa-3080c4fa087d","biId":"7232475","wAsSubmissionId":"24ef6713-783b-4808-9127-af8e42410444","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:32.827Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6713-783b-4808-9127-af8e42410444","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:33.220Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":20,"tax":0,"total":20,"discountAmount":180,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef6713-783b-4808-9127-af8e42410444","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef6713-783b-4808-9127-af8e42410444","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236058 for PriceProposal 24ef4032-783b-4808-9127-af8e42410900","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236058","priceProposal":{"uid":"6683cf99-7481-4ed4-a663-49b344350c10","biId":"7236058","wAsSubmissionId":"24ef4032-783b-4808-9127-af8e42410900","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:53.476Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4032-783b-4808-9127-af8e42410900","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-04-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:54.050Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":20,"tax":0,"total":20,"discountAmount":180,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef4032-783b-4808-9127-af8e42410900","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef4032-783b-4808-9127-af8e42410900","wAsSubmissionDate":"2024-04-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Multiple Insitutional discounts</t>
@@ -1447,10 +1569,10 @@
     <t>MultiInsti</t>
   </si>
   <si>
-    <t>Created Viax order 7232476 for PriceProposal 24ef3433-783b-4808-9127-af8e42410418</t>
-  </si>
-  <si>
-    <t>7232476</t>
+    <t>Created Viax order 7236059 for PriceProposal 24ef5056-783b-4808-9127-af8e42410812</t>
+  </si>
+  <si>
+    <t>7236059</t>
   </si>
   <si>
     <t>{
@@ -1458,7 +1580,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef3433-783b-4808-9127-af8e42410418",
+      "submissionId": "24ef5056-783b-4808-9127-af8e42410812",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1514,7 +1636,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232476 for PriceProposal 24ef3433-783b-4808-9127-af8e42410418","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232476","priceProposal":{"uid":"667a5a34-ac1d-4fa8-af2b-b067699e3eac","biId":"7232476","wAsSubmissionId":"24ef3433-783b-4808-9127-af8e42410418","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:36.277Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef3433-783b-4808-9127-af8e42410418","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-10","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:36.693Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3433-783b-4808-9127-af8e42410418","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef3433-783b-4808-9127-af8e42410418","wAsSubmissionDate":"2024-04-10","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236059 for PriceProposal 24ef5056-783b-4808-9127-af8e42410812","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236059","priceProposal":{"uid":"6683cf9d-2dd8-469a-92c6-7568ca3b3e0d","biId":"7236059","wAsSubmissionId":"24ef5056-783b-4808-9127-af8e42410812","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T09:59:57.034Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5056-783b-4808-9127-af8e42410812","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-10","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T09:59:57.411Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5056-783b-4808-9127-af8e42410812","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef5056-783b-4808-9127-af8e42410812","wAsSubmissionDate":"2024-04-10","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Funder details</t>
@@ -1523,10 +1645,10 @@
     <t>FunderPaid</t>
   </si>
   <si>
-    <t>Created Viax order 7232477 for PriceProposal 24ef3174-783b-4808-9127-af8e42410867</t>
-  </si>
-  <si>
-    <t>7232477</t>
+    <t>Created Viax order 7236060 for PriceProposal 24ef2720-783b-4808-9127-af8e42410157</t>
+  </si>
+  <si>
+    <t>7236060</t>
   </si>
   <si>
     <t>{
@@ -1534,7 +1656,7 @@
   "variables": {
     "data": {
       "requestId": "4a48d9c8-6b6d-4583-b9ac-1836890cb988",
-      "submissionId": "24ef3174-783b-4808-9127-af8e42410867",
+      "submissionId": "24ef2720-783b-4808-9127-af8e42410157",
       "edRefCode": "CAM4-2024-04-1853",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1621,7 +1743,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232477 for PriceProposal 24ef3174-783b-4808-9127-af8e42410867","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232477","priceProposal":{"uid":"667a5a37-a35f-4a00-958b-f98eeb214022","biId":"7232477","wAsSubmissionId":"24ef3174-783b-4808-9127-af8e42410867","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-06-25T05:48:39.830Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef3174-783b-4808-9127-af8e42410867","edRefCode":"CAM4-2024-04-1853","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]},{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:40.361Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null},{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3174-783b-4808-9127-af8e42410867","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-1853","wAsSubmissionId":"24ef3174-783b-4808-9127-af8e42410867","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236060 for PriceProposal 24ef2720-783b-4808-9127-af8e42410157","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236060","priceProposal":{"uid":"6683cfa0-2b4a-4ab0-a74d-f5c4b120f9a7","biId":"7236060","wAsSubmissionId":"24ef2720-783b-4808-9127-af8e42410157","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-02T10:00:00.727Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef2720-783b-4808-9127-af8e42410157","edRefCode":"CAM4-2024-04-1853","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-03-21","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]},{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:01.661Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null},{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2720-783b-4808-9127-af8e42410157","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-1853","wAsSubmissionId":"24ef2720-783b-4808-9127-af8e42410157","wAsSubmissionDate":"2024-03-21","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Invalid Promotional discount code</t>
@@ -1630,10 +1752,13 @@
     <t>InvalidPromo</t>
   </si>
   <si>
-    <t>Created Viax order 7232478 for PriceProposal 24ef1792-783b-4808-9127-af8e42410236</t>
-  </si>
-  <si>
-    <t>7232478</t>
+    <t>Created Viax order 7236061 for PriceProposal 24ef9151-783b-4808-9127-af8e42410275</t>
+  </si>
+  <si>
+    <t>7236061</t>
+  </si>
+  <si>
+    <t>DataCorrectionRequired</t>
   </si>
   <si>
     <t>{
@@ -1641,7 +1766,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef1792-783b-4808-9127-af8e42410236",
+      "submissionId": "24ef9151-783b-4808-9127-af8e42410275",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1697,7 +1822,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232478 for PriceProposal 24ef1792-783b-4808-9127-af8e42410236","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232478","priceProposal":{"uid":"667a5a3b-f9ef-4783-a4c3-5d9a1a5262ff","biId":"7232478","wAsSubmissionId":"24ef1792-783b-4808-9127-af8e42410236","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-06-25T05:48:43.436Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef1792-783b-4808-9127-af8e42410236","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:43.900Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef1792-783b-4808-9127-af8e42410236","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef1792-783b-4808-9127-af8e42410236","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236061 for PriceProposal 24ef9151-783b-4808-9127-af8e42410275","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236061","priceProposal":{"uid":"6683cfae-af87-4170-bb8b-4558efc43967","biId":"7236061","wAsSubmissionId":"24ef9151-783b-4808-9127-af8e42410275","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-07-02T10:00:14.406Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9151-783b-4808-9127-af8e42410275","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:14.908Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9151-783b-4808-9127-af8e42410275","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef9151-783b-4808-9127-af8e42410275","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
   <si>
     <t>Create PP with Manual override required value as Yes</t>
@@ -1706,10 +1831,10 @@
     <t>ManualOverride</t>
   </si>
   <si>
-    <t>Created Viax order 7232479 for PriceProposal 24ef7384-783b-4808-9127-af8e42410372</t>
-  </si>
-  <si>
-    <t>7232479</t>
+    <t>Created Viax order 7236065 for PriceProposal 24ef8820-783b-4808-9127-af8e42410282</t>
+  </si>
+  <si>
+    <t>7236065</t>
   </si>
   <si>
     <t>ManualOverrideRequired</t>
@@ -1720,7 +1845,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef7384-783b-4808-9127-af8e42410372",
+      "submissionId": "24ef8820-783b-4808-9127-af8e42410282",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -1776,7 +1901,7 @@
 }</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7232479 for PriceProposal 24ef7384-783b-4808-9127-af8e42410372","version":"1.4.0-qa2.36","viaxPriceProposalId":"7232479","priceProposal":{"uid":"667a5a3f-d986-45c5-9431-16b78578fd96","biId":"7232479","wAsSubmissionId":"24ef7384-783b-4808-9127-af8e42410372","bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-06-25T05:48:47.964Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7384-783b-4808-9127-af8e42410372","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-06-25T05:48:48.381Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7384-783b-4808-9127-af8e42410372","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef7384-783b-4808-9127-af8e42410372","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7236065 for PriceProposal 24ef8820-783b-4808-9127-af8e42410282","version":"1.4.1-qa2.39","viaxPriceProposalId":"7236065","priceProposal":{"uid":"6683cfb2-23d1-4598-80ff-c6baeacc9e26","biId":"7236065","wAsSubmissionId":"24ef8820-783b-4808-9127-af8e42410282","bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-07-02T10:00:18.794Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8820-783b-4808-9127-af8e42410282","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-02T10:00:19.315Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8820-783b-4808-9127-af8e42410282","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef8820-783b-4808-9127-af8e42410282","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1931,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1851,20 +1976,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1881,7 +1994,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1898,8 +2011,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3127,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3138,7 +3249,7 @@
     <col min="3" max="3" width="27.90625" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.26953125" customWidth="1"/>
     <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
@@ -3357,10 +3468,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3491,34 +3602,34 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>160</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>161</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>162</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>163</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>164</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>165</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>166</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>167</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>168</v>
-      </c>
-      <c r="K2" t="s">
-        <v>169</v>
       </c>
       <c r="L2" t="s">
         <v>42</v>
@@ -3529,14 +3640,32 @@
       <c r="N2" t="s">
         <v>43</v>
       </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
       <c r="P2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" t="s">
         <v>170</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>171</v>
       </c>
-      <c r="R2" t="s">
-        <v>172</v>
+      <c r="W2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -3544,52 +3673,273 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
         <v>173</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>174</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>175</v>
       </c>
-      <c r="E3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="H3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L3" t="s">
         <v>42</v>
       </c>
       <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>182</v>
+      </c>
+      <c r="R3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K4" t="s">
+        <v>193</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>195</v>
+      </c>
+      <c r="R4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I5" t="s">
+        <v>201</v>
+      </c>
+      <c r="J5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K5">
+        <v>3213151</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N5" t="s">
         <v>56</v>
       </c>
-      <c r="P3" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>171</v>
-      </c>
-      <c r="R3" t="s">
-        <v>172</v>
+      <c r="P5" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>195</v>
+      </c>
+      <c r="R5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" t="s">
+        <v>211</v>
+      </c>
+      <c r="K6" t="s">
+        <v>212</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>214</v>
+      </c>
+      <c r="R6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J7" t="s">
+        <v>220</v>
+      </c>
+      <c r="K7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>214</v>
+      </c>
+      <c r="R7" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3605,8 +3955,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3628,31 +3978,31 @@
         <v>79</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>30</v>
@@ -3666,31 +4016,31 @@
         <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>194</v>
+        <v>233</v>
+      </c>
+      <c r="G2">
+        <v>7236048</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J2" t="s">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="K2" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3701,31 +4051,31 @@
         <v>154</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>197</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>194</v>
+        <v>241</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J3" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="K3" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -3736,31 +4086,31 @@
         <v>154</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>203</v>
+        <v>244</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F4" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>194</v>
+        <v>247</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J4" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="K4" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -3771,31 +4121,31 @@
         <v>154</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="E5" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="G5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>194</v>
+        <v>253</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J5" t="s">
-        <v>213</v>
+        <v>254</v>
       </c>
       <c r="K5" t="s">
-        <v>214</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -3806,31 +4156,31 @@
         <v>154</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>215</v>
+        <v>256</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>216</v>
+        <v>257</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>259</v>
       </c>
       <c r="G6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>194</v>
+        <v>260</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J6" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="K6" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -3841,31 +4191,31 @@
         <v>154</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>222</v>
+        <v>263</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>265</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>266</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>194</v>
+        <v>267</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J7" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
       <c r="K7" t="s">
-        <v>228</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3876,31 +4226,31 @@
         <v>154</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>229</v>
+        <v>270</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>230</v>
+        <v>271</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>231</v>
+        <v>272</v>
       </c>
       <c r="G8" t="s">
-        <v>232</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>194</v>
+        <v>273</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J8" t="s">
-        <v>233</v>
+        <v>274</v>
       </c>
       <c r="K8" t="s">
-        <v>234</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -3911,31 +4261,31 @@
         <v>154</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" t="s">
+        <v>279</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" t="s">
-        <v>237</v>
-      </c>
-      <c r="G9" t="s">
-        <v>238</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="J9" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="K9" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -3946,31 +4296,31 @@
         <v>154</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="G10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>194</v>
+        <v>285</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
+        <v>286</v>
       </c>
       <c r="K10" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -3981,25 +4331,31 @@
         <v>154</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>194</v>
+        <v>232</v>
+      </c>
+      <c r="F11" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J11" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -4010,31 +4366,31 @@
         <v>154</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>254</v>
+        <v>295</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
-        <v>255</v>
+        <v>296</v>
       </c>
       <c r="G12" t="s">
-        <v>256</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>194</v>
+        <v>297</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J12" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="K12" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -4045,31 +4401,31 @@
         <v>154</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F13" t="s">
-        <v>261</v>
+        <v>302</v>
       </c>
       <c r="G13" t="s">
-        <v>262</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>194</v>
+        <v>303</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J13" t="s">
-        <v>263</v>
+        <v>304</v>
       </c>
       <c r="K13" t="s">
-        <v>264</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -4080,31 +4436,31 @@
         <v>154</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>266</v>
+        <v>307</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F14" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="G14" t="s">
-        <v>268</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>194</v>
+        <v>309</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J14" t="s">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="K14" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -4115,31 +4471,31 @@
         <v>154</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F15" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="G15" t="s">
-        <v>274</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>194</v>
+        <v>315</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J15" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="K15" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -4150,31 +4506,31 @@
         <v>154</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="G16" t="s">
-        <v>280</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>194</v>
+        <v>322</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="J16" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="K16" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New File PP Regression13
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -3210,12 +3210,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Created Viax order 7239708 for PriceProposal 24ef2446-866b-4808-9127-af8e42410746</t>
+          <t>Created Viax order 7239973 for PriceProposal 24ef2132-664b-4808-9127-af8e42410984</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7239708</t>
+          <t>7239973</t>
         </is>
       </c>
       <c r="H2" s="13" t="inlineStr">
@@ -3235,7 +3235,7 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef2446-866b-4808-9127-af8e42410746",
+      "submissionId": "24ef2132-664b-4808-9127-af8e42410984",
       "edRefCode": "ACN3-2023-06-0432",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
@@ -3293,7 +3293,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7239708 for PriceProposal 24ef2446-866b-4808-9127-af8e42410746","version":"1.4.1-qa2.43","viaxPriceProposalId":"7239708","priceProposal":{"uid":"668be929-995c-498f-a775-acd7d207a7b8","biId":"7239708","wAsSubmissionId":"24ef2446-866b-4808-9127-af8e42410746","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-08T13:27:05.025Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2446-866b-4808-9127-af8e42410746","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-08T13:27:06.255Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2446-866b-4808-9127-af8e42410746","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2446-866b-4808-9127-af8e42410746","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7239973 for PriceProposal 24ef2132-664b-4808-9127-af8e42410984","version":"1.4.1-qa2.43","viaxPriceProposalId":"7239973","priceProposal":{"uid":"668ced7a-ce04-41d7-80d3-90f81f1775ef","biId":"7239973","wAsSubmissionId":"24ef2132-664b-4808-9127-af8e42410984","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-07-09T07:57:46.182Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2132-664b-4808-9127-af8e42410984","edRefCode":"ACN3-2023-06-0432","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-04-15","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-07-09T07:57:46.949Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2132-664b-4808-9127-af8e42410984","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-0432","wAsSubmissionId":"24ef2132-664b-4808-9127-af8e42410984","wAsSubmissionDate":"2024-04-15","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
UI Validations added V.14
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F660940E-70E4-4008-A5C0-3A785C2A3172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87616DC5-5558-408D-B9D9-BAAD5407E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
     <sheet name="HappyFlowInputs" sheetId="2" r:id="rId2"/>
-    <sheet name="UIValidations" sheetId="3" r:id="rId3"/>
-    <sheet name="PriceProposal" sheetId="4" r:id="rId4"/>
+    <sheet name="PriceProposal" sheetId="4" r:id="rId3"/>
+    <sheet name="UIValidations" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="316">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -968,6 +968,9 @@
   </si>
   <si>
     <t>Create PP Society discount with Withdrawn</t>
+  </si>
+  <si>
+    <t>ExeEnvironment</t>
   </si>
 </sst>
 </file>
@@ -2175,14 +2178,1265 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AI24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB30" sqref="AB30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" t="s">
+        <v>261</v>
+      </c>
+      <c r="R2">
+        <v>75</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>261</v>
+      </c>
+      <c r="X2" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" t="s">
+        <v>261</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="N3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R3">
+        <v>75</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+      <c r="T3" t="s">
+        <v>261</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H4" t="s">
+        <v>261</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" t="s">
+        <v>261</v>
+      </c>
+      <c r="R4">
+        <v>75</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T4" t="s">
+        <v>261</v>
+      </c>
+      <c r="X4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" t="s">
+        <v>261</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="N5" t="s">
+        <v>261</v>
+      </c>
+      <c r="R5">
+        <v>20</v>
+      </c>
+      <c r="S5">
+        <v>90</v>
+      </c>
+      <c r="T5" t="s">
+        <v>261</v>
+      </c>
+      <c r="X5" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="H6" t="s">
+        <v>261</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N6" t="s">
+        <v>261</v>
+      </c>
+      <c r="R6">
+        <v>10</v>
+      </c>
+      <c r="S6">
+        <v>15.25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>261</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="H7" t="s">
+        <v>261</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="N7" t="s">
+        <v>261</v>
+      </c>
+      <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+      <c r="T7" t="s">
+        <v>261</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" t="s">
+        <v>261</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N8" t="s">
+        <v>261</v>
+      </c>
+      <c r="R8">
+        <v>75</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T8" t="s">
+        <v>261</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="H9" t="s">
+        <v>261</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="N9" t="s">
+        <v>261</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7">
+        <v>75</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T9" t="s">
+        <v>261</v>
+      </c>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10">
+        <v>75</v>
+      </c>
+      <c r="S10">
+        <v>20</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y10" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11">
+        <v>50</v>
+      </c>
+      <c r="S11">
+        <v>50</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H12" t="s">
+        <v>279</v>
+      </c>
+      <c r="I12" t="s">
+        <v>291</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="R12" s="15">
+        <v>75</v>
+      </c>
+      <c r="S12">
+        <v>90</v>
+      </c>
+      <c r="T12" s="15">
+        <v>50</v>
+      </c>
+      <c r="U12" s="15">
+        <v>50</v>
+      </c>
+      <c r="V12" s="15">
+        <v>5</v>
+      </c>
+      <c r="W12" s="15">
+        <v>20</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA12" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB12" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC12" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H13" t="s">
+        <v>261</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+    </row>
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>261</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15">
+        <v>75</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y15" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" t="s">
+        <v>261</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16">
+        <v>75</v>
+      </c>
+      <c r="S16" t="s">
+        <v>261</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y16" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17">
+        <v>75</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y17" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>305</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D20" t="s">
+        <v>308</v>
+      </c>
+      <c r="E20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" t="s">
+        <v>310</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D22" t="s">
+        <v>312</v>
+      </c>
+      <c r="E22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>261</v>
+      </c>
+      <c r="L23" t="s">
+        <v>161</v>
+      </c>
+      <c r="M23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N23" t="s">
+        <v>261</v>
+      </c>
+      <c r="R23">
+        <v>75</v>
+      </c>
+      <c r="S23">
+        <v>5</v>
+      </c>
+      <c r="T23" t="s">
+        <v>261</v>
+      </c>
+      <c r="X23" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>261</v>
+      </c>
+      <c r="L24" t="s">
+        <v>161</v>
+      </c>
+      <c r="M24" t="s">
+        <v>217</v>
+      </c>
+      <c r="N24" t="s">
+        <v>261</v>
+      </c>
+      <c r="R24">
+        <v>75</v>
+      </c>
+      <c r="S24">
+        <v>5</v>
+      </c>
+      <c r="T24" t="s">
+        <v>261</v>
+      </c>
+      <c r="X24" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2209,7 +3463,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -2873,1255 +4127,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AI24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R13" workbookViewId="0">
-      <selection activeCell="AB30" sqref="AB30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>261</v>
-      </c>
-      <c r="L2" t="s">
-        <v>161</v>
-      </c>
-      <c r="M2" t="s">
-        <v>217</v>
-      </c>
-      <c r="N2" t="s">
-        <v>261</v>
-      </c>
-      <c r="R2">
-        <v>75</v>
-      </c>
-      <c r="S2">
-        <v>5</v>
-      </c>
-      <c r="T2" t="s">
-        <v>261</v>
-      </c>
-      <c r="X2" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="E3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" t="s">
-        <v>261</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="N3" t="s">
-        <v>261</v>
-      </c>
-      <c r="R3">
-        <v>75</v>
-      </c>
-      <c r="S3">
-        <v>20</v>
-      </c>
-      <c r="T3" t="s">
-        <v>261</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="H4" t="s">
-        <v>261</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="N4" t="s">
-        <v>261</v>
-      </c>
-      <c r="R4">
-        <v>75</v>
-      </c>
-      <c r="S4" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T4" t="s">
-        <v>261</v>
-      </c>
-      <c r="X4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y4" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H5" t="s">
-        <v>261</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="N5" t="s">
-        <v>261</v>
-      </c>
-      <c r="R5">
-        <v>20</v>
-      </c>
-      <c r="S5">
-        <v>90</v>
-      </c>
-      <c r="T5" t="s">
-        <v>261</v>
-      </c>
-      <c r="X5" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y5" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="E6" t="s">
-        <v>274</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="H6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="N6" t="s">
-        <v>261</v>
-      </c>
-      <c r="R6">
-        <v>10</v>
-      </c>
-      <c r="S6">
-        <v>15.25</v>
-      </c>
-      <c r="T6" t="s">
-        <v>261</v>
-      </c>
-      <c r="X6" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y6" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="H7" t="s">
-        <v>261</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="N7" t="s">
-        <v>261</v>
-      </c>
-      <c r="R7">
-        <v>30</v>
-      </c>
-      <c r="S7">
-        <v>100</v>
-      </c>
-      <c r="T7" t="s">
-        <v>261</v>
-      </c>
-      <c r="X7" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y7" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H8" t="s">
-        <v>261</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="N8" t="s">
-        <v>261</v>
-      </c>
-      <c r="R8">
-        <v>75</v>
-      </c>
-      <c r="S8" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T8" t="s">
-        <v>261</v>
-      </c>
-      <c r="X8" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y8" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="H9" t="s">
-        <v>261</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="N9" t="s">
-        <v>261</v>
-      </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7">
-        <v>75</v>
-      </c>
-      <c r="S9" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T9" t="s">
-        <v>261</v>
-      </c>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-    </row>
-    <row r="10" spans="1:35">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" t="s">
-        <v>156</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10">
-        <v>75</v>
-      </c>
-      <c r="S10">
-        <v>20</v>
-      </c>
-      <c r="T10">
-        <v>5</v>
-      </c>
-      <c r="X10" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y10" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="E11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>261</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11">
-        <v>50</v>
-      </c>
-      <c r="S11">
-        <v>50</v>
-      </c>
-      <c r="T11" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y11" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z11" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-    </row>
-    <row r="12" spans="1:35">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="E12" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H12" t="s">
-        <v>279</v>
-      </c>
-      <c r="I12" t="s">
-        <v>291</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q12" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="R12" s="15">
-        <v>75</v>
-      </c>
-      <c r="S12">
-        <v>90</v>
-      </c>
-      <c r="T12" s="15">
-        <v>50</v>
-      </c>
-      <c r="U12" s="15">
-        <v>50</v>
-      </c>
-      <c r="V12" s="15">
-        <v>5</v>
-      </c>
-      <c r="W12" s="15">
-        <v>20</v>
-      </c>
-      <c r="X12" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y12" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>235</v>
-      </c>
-      <c r="AA12" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="AB12" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="AC12" s="15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H13" t="s">
-        <v>261</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="Z13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="15"/>
-    </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="N14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="S14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="Z14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-    </row>
-    <row r="15" spans="1:35">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>261</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15">
-        <v>75</v>
-      </c>
-      <c r="S15">
-        <v>5</v>
-      </c>
-      <c r="T15" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y15" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z15" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-    </row>
-    <row r="16" spans="1:35">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="E16" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="H16" t="s">
-        <v>261</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16">
-        <v>75</v>
-      </c>
-      <c r="S16" t="s">
-        <v>261</v>
-      </c>
-      <c r="T16" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y16" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z16" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
-    </row>
-    <row r="17" spans="1:29">
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="N17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17">
-        <v>75</v>
-      </c>
-      <c r="S17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="T17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y17" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="15"/>
-    </row>
-    <row r="18" spans="1:29">
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="E18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29">
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>305</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="E19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29">
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D20" t="s">
-        <v>308</v>
-      </c>
-      <c r="E20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29">
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D21" t="s">
-        <v>310</v>
-      </c>
-      <c r="E21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="D22" t="s">
-        <v>312</v>
-      </c>
-      <c r="E22" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" t="s">
-        <v>156</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" t="s">
-        <v>261</v>
-      </c>
-      <c r="L23" t="s">
-        <v>161</v>
-      </c>
-      <c r="M23" t="s">
-        <v>217</v>
-      </c>
-      <c r="N23" t="s">
-        <v>261</v>
-      </c>
-      <c r="R23">
-        <v>75</v>
-      </c>
-      <c r="S23">
-        <v>5</v>
-      </c>
-      <c r="T23" t="s">
-        <v>261</v>
-      </c>
-      <c r="X23" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" t="s">
-        <v>261</v>
-      </c>
-      <c r="L24" t="s">
-        <v>161</v>
-      </c>
-      <c r="M24" t="s">
-        <v>217</v>
-      </c>
-      <c r="N24" t="s">
-        <v>261</v>
-      </c>
-      <c r="R24">
-        <v>75</v>
-      </c>
-      <c r="S24">
-        <v>5</v>
-      </c>
-      <c r="T24" t="s">
-        <v>261</v>
-      </c>
-      <c r="X24" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
UI Validations added V.16
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87616DC5-5558-408D-B9D9-BAAD5407E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA008C4-3E8C-4222-BCE8-8DAE905CC9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
     <sheet name="HappyFlowInputs" sheetId="2" r:id="rId2"/>
-    <sheet name="PriceProposal" sheetId="4" r:id="rId3"/>
-    <sheet name="UIValidations" sheetId="3" r:id="rId4"/>
+    <sheet name="PriceProposal" sheetId="3" r:id="rId3"/>
+    <sheet name="UIValidations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="315">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -442,34 +442,328 @@
     <t>0000000135552217</t>
   </si>
   <si>
+    <t>VIAXEnvironment</t>
+  </si>
+  <si>
+    <t>ScenarioList</t>
+  </si>
+  <si>
+    <t>JSONFileName</t>
+  </si>
+  <si>
+    <t>JournalID</t>
+  </si>
+  <si>
+    <t>DiscountType1</t>
+  </si>
+  <si>
+    <t>DiscountType2</t>
+  </si>
+  <si>
+    <t>DiscountType3</t>
+  </si>
+  <si>
+    <t>DiscountType4</t>
+  </si>
+  <si>
+    <t>DiscountType5</t>
+  </si>
+  <si>
+    <t>DiscountType6</t>
+  </si>
+  <si>
+    <t>DiscountCondition1</t>
+  </si>
+  <si>
+    <t>DiscouontCondition2</t>
+  </si>
+  <si>
+    <t>DiscountCondition3</t>
+  </si>
+  <si>
+    <t>DiscountCondition4</t>
+  </si>
+  <si>
+    <t>DiscountCondition5</t>
+  </si>
+  <si>
+    <t>DiscountCondition6</t>
+  </si>
+  <si>
+    <t>DiscountPercentage1</t>
+  </si>
+  <si>
+    <t>DiscountPercentage2</t>
+  </si>
+  <si>
+    <t>DiscountPercentage3</t>
+  </si>
+  <si>
+    <t>DiscountPercentage4</t>
+  </si>
+  <si>
+    <t>DiscountPercentage5</t>
+  </si>
+  <si>
+    <t>DiscountPercentage6</t>
+  </si>
+  <si>
+    <t>AppliedYes1</t>
+  </si>
+  <si>
+    <t>AppliedYes2</t>
+  </si>
+  <si>
+    <t>AppliedYes3</t>
+  </si>
+  <si>
+    <t>AppliedYes4</t>
+  </si>
+  <si>
+    <t>AppliedYes5</t>
+  </si>
+  <si>
+    <t>AppliedYes6</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>PriceProposalStatus</t>
+  </si>
+  <si>
+    <t>ResponseStatusCode</t>
+  </si>
+  <si>
+    <t>JSONText</t>
+  </si>
+  <si>
+    <t>Create PP with Society discount</t>
+  </si>
+  <si>
+    <t>c597beef-e45f-4cc7-b34c-0df812e2ef25</t>
+  </si>
+  <si>
+    <t>ArticleType</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Research Article</t>
+  </si>
+  <si>
+    <t>JCASP</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Create PP with Promotional discount</t>
+  </si>
+  <si>
+    <t>Promotional</t>
+  </si>
+  <si>
+    <t>WileyPromoCode</t>
+  </si>
+  <si>
+    <t>PROMO50</t>
+  </si>
+  <si>
+    <t>Create PP with Institutional discount</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>E O Lawrence Berkeley National Laboratory</t>
+  </si>
+  <si>
+    <t>Create PP with Editorial discount</t>
+  </si>
+  <si>
+    <t>Editorial</t>
+  </si>
+  <si>
+    <t>EditorialDiscount</t>
+  </si>
+  <si>
+    <t>OPINION</t>
+  </si>
+  <si>
+    <t>CCCAM424</t>
+  </si>
+  <si>
+    <t>Create PP with Referral discount</t>
+  </si>
+  <si>
+    <t>Referal</t>
+  </si>
+  <si>
+    <t>e1bbb7b4-5369-4c40-a53a-aa3dc55390a6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ReferralDiscount</t>
+  </si>
+  <si>
+    <t>Create PP with Geographical discount</t>
+  </si>
+  <si>
+    <t>Geographical</t>
+  </si>
+  <si>
+    <t>b6d18dc5-3811-4b21-81f0-a01997c20001</t>
+  </si>
+  <si>
+    <t>GeographicalDiscount</t>
+  </si>
+  <si>
+    <t>MH - Marshall Islands</t>
+  </si>
+  <si>
+    <t>Create PP with Article type discount</t>
+  </si>
+  <si>
+    <t>RESEARCH ARTICLE</t>
+  </si>
+  <si>
+    <t>Create PP with Stacked Institutional discount</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>Create PP with multiple Society and Promotional discounts</t>
+  </si>
+  <si>
+    <t>SocietyPromo</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Create PP with same discount Geographical Editorial and Society discounts</t>
+  </si>
+  <si>
+    <t>GeoEditSociety</t>
+  </si>
+  <si>
+    <t>BO - Bolivia</t>
+  </si>
+  <si>
+    <t>EANM9</t>
+  </si>
+  <si>
+    <t>Create PP with Society Promotional Geographical Editorial Article type and Referral discounts</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>ReferralDiscount</t>
+  </si>
+  <si>
+    <t>PE - Peru</t>
+  </si>
+  <si>
+    <t>Create PP with Multiple Insitutional discounts</t>
+  </si>
+  <si>
+    <t>MultiInsti</t>
+  </si>
+  <si>
+    <t>Create PP with Funder details</t>
+  </si>
+  <si>
+    <t>FunderPaid</t>
+  </si>
+  <si>
+    <t>Create PP with Manual override required value as Yes</t>
+  </si>
+  <si>
+    <t>ManualOverride</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Promotional discount code</t>
+  </si>
+  <si>
+    <t>InvalidPromo</t>
+  </si>
+  <si>
+    <t>PRKMO50</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Society</t>
+  </si>
+  <si>
+    <t>InvalidSociety</t>
+  </si>
+  <si>
+    <t>EANM</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Article Type</t>
+  </si>
+  <si>
+    <t>InvalidArticleType</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Editorial</t>
+  </si>
+  <si>
+    <t>InvalidEditorial</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Referal</t>
+  </si>
+  <si>
+    <t>InvalidReferal</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid CountryCode</t>
+  </si>
+  <si>
+    <t>InvalidCountryCode</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid MailId</t>
+  </si>
+  <si>
+    <t>InvalidMailId</t>
+  </si>
+  <si>
+    <t>Create PP Society discount with Rejected</t>
+  </si>
+  <si>
+    <t>Create PP Society discount with Withdrawn</t>
+  </si>
+  <si>
     <t>HeaderCloumnName</t>
   </si>
   <si>
-    <t>FunderPaid</t>
-  </si>
-  <si>
     <t>Multiple</t>
   </si>
   <si>
-    <t>OrderID</t>
-  </si>
-  <si>
-    <t>7242085</t>
-  </si>
-  <si>
-    <t>7242086</t>
-  </si>
-  <si>
-    <t>7242087</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242085 for PriceProposal 24ef2384-235b-4808-9127-af8e42410930</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242086 for PriceProposal 24ef7710-983b-4808-9127-af8e42410367</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242087 for PriceProposal 24ef2007-947b-4808-9127-af8e42410687</t>
+    <t>ExeEnvironment</t>
+  </si>
+  <si>
+    <t>7242608</t>
+  </si>
+  <si>
+    <t>7242609</t>
+  </si>
+  <si>
+    <t>7242610</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242608 for PriceProposal 24ef3969-549b-4808-9127-af8e42410838</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242609 for PriceProposal 24ef5143-857b-4808-9127-af8e42410958</t>
+  </si>
+  <si>
+    <t>Created Viax order 7242610 for PriceProposal 24ef5787-856b-4808-9127-af8e42410444</t>
   </si>
   <si>
     <t>ResponseCode</t>
@@ -481,36 +775,12 @@
     <t>CaseName</t>
   </si>
   <si>
-    <t>Create PP with Funder details</t>
-  </si>
-  <si>
-    <t>Create PP with Society discount</t>
-  </si>
-  <si>
-    <t>Create PP with multiple Society and Promotional discounts</t>
-  </si>
-  <si>
-    <t>JournalID</t>
-  </si>
-  <si>
-    <t>c597beef-e45f-4cc7-b34c-0df812e2ef25</t>
-  </si>
-  <si>
-    <t>JSONFileName</t>
-  </si>
-  <si>
-    <t>SocietyPromo</t>
-  </si>
-  <si>
     <t>BaseArticleType</t>
   </si>
   <si>
     <t>Data Article</t>
   </si>
   <si>
-    <t>Research Article</t>
-  </si>
-  <si>
     <t>DisplayArticleType</t>
   </si>
   <si>
@@ -520,13 +790,7 @@
     <t>SubmissionDate</t>
   </si>
   <si>
-    <t>03-21-2024</t>
-  </si>
-  <si>
-    <t>04-15-2024</t>
-  </si>
-  <si>
-    <t>04-17-2024</t>
+    <t>07-16-2024</t>
   </si>
   <si>
     <t>ArticleTitle</t>
@@ -589,10 +853,13 @@
     <t>MauScriptId</t>
   </si>
   <si>
-    <t>CAM4-2024-04-1853</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-0432</t>
+    <t>CAM4-2024-04-3969</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-5143</t>
+  </si>
+  <si>
+    <t>ACN3-2023-06-5787</t>
   </si>
   <si>
     <t>SubmittedBy</t>
@@ -658,30 +925,9 @@
     <t>160.00 USD</t>
   </si>
   <si>
-    <t>DiscountType1</t>
-  </si>
-  <si>
-    <t>ArticleType</t>
-  </si>
-  <si>
-    <t>DiscountType2</t>
-  </si>
-  <si>
-    <t>WileyPromoCode</t>
-  </si>
-  <si>
-    <t>DiscountCondition1</t>
-  </si>
-  <si>
     <t>DiscountCondition2</t>
   </si>
   <si>
-    <t>JCASP</t>
-  </si>
-  <si>
-    <t>PROMO50</t>
-  </si>
-  <si>
     <t>Percentage1</t>
   </si>
   <si>
@@ -694,9 +940,6 @@
     <t>Applied1</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Applied2</t>
   </si>
   <si>
@@ -718,259 +961,13 @@
     <t>40.00 USD</t>
   </si>
   <si>
-    <t>DiscountType3</t>
-  </si>
-  <si>
-    <t>DiscountCondition3</t>
-  </si>
-  <si>
     <t>Percentage3</t>
   </si>
   <si>
     <t>Applied3</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Value3</t>
-  </si>
-  <si>
-    <t>VIAXEnvironment</t>
-  </si>
-  <si>
-    <t>ScenarioList</t>
-  </si>
-  <si>
-    <t>DiscountType4</t>
-  </si>
-  <si>
-    <t>DiscountType5</t>
-  </si>
-  <si>
-    <t>DiscountType6</t>
-  </si>
-  <si>
-    <t>DiscouontCondition2</t>
-  </si>
-  <si>
-    <t>DiscountCondition4</t>
-  </si>
-  <si>
-    <t>DiscountCondition5</t>
-  </si>
-  <si>
-    <t>DiscountCondition6</t>
-  </si>
-  <si>
-    <t>DiscountPercentage1</t>
-  </si>
-  <si>
-    <t>DiscountPercentage2</t>
-  </si>
-  <si>
-    <t>DiscountPercentage3</t>
-  </si>
-  <si>
-    <t>DiscountPercentage4</t>
-  </si>
-  <si>
-    <t>DiscountPercentage5</t>
-  </si>
-  <si>
-    <t>DiscountPercentage6</t>
-  </si>
-  <si>
-    <t>AppliedYes1</t>
-  </si>
-  <si>
-    <t>AppliedYes2</t>
-  </si>
-  <si>
-    <t>AppliedYes3</t>
-  </si>
-  <si>
-    <t>AppliedYes4</t>
-  </si>
-  <si>
-    <t>AppliedYes5</t>
-  </si>
-  <si>
-    <t>AppliedYes6</t>
-  </si>
-  <si>
-    <t>PriceProposalStatus</t>
-  </si>
-  <si>
-    <t>ResponseStatusCode</t>
-  </si>
-  <si>
-    <t>JSONText</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Create PP with Promotional discount</t>
-  </si>
-  <si>
-    <t>Promotional</t>
-  </si>
-  <si>
-    <t>Create PP with Institutional discount</t>
-  </si>
-  <si>
-    <t>Institutional</t>
-  </si>
-  <si>
-    <t>E O Lawrence Berkeley National Laboratory</t>
-  </si>
-  <si>
-    <t>Create PP with Editorial discount</t>
-  </si>
-  <si>
-    <t>Editorial</t>
-  </si>
-  <si>
-    <t>EditorialDiscount</t>
-  </si>
-  <si>
-    <t>OPINION</t>
-  </si>
-  <si>
-    <t>CCCAM424</t>
-  </si>
-  <si>
-    <t>Create PP with Referral discount</t>
-  </si>
-  <si>
-    <t>Referal</t>
-  </si>
-  <si>
-    <t>e1bbb7b4-5369-4c40-a53a-aa3dc55390a6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ReferralDiscount</t>
-  </si>
-  <si>
-    <t>Create PP with Geographical discount</t>
-  </si>
-  <si>
-    <t>Geographical</t>
-  </si>
-  <si>
-    <t>b6d18dc5-3811-4b21-81f0-a01997c20001</t>
-  </si>
-  <si>
-    <t>GeographicalDiscount</t>
-  </si>
-  <si>
-    <t>MH - Marshall Islands</t>
-  </si>
-  <si>
-    <t>Create PP with Article type discount</t>
-  </si>
-  <si>
-    <t>RESEARCH ARTICLE</t>
-  </si>
-  <si>
-    <t>Create PP with Stacked Institutional discount</t>
-  </si>
-  <si>
-    <t>Stacked</t>
-  </si>
-  <si>
-    <t>Create PP with same discount Geographical Editorial and Society discounts</t>
-  </si>
-  <si>
-    <t>GeoEditSociety</t>
-  </si>
-  <si>
-    <t>BO - Bolivia</t>
-  </si>
-  <si>
-    <t>EANM9</t>
-  </si>
-  <si>
-    <t>Create PP with Society Promotional Geographical Editorial Article type and Referral discounts</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>ReferralDiscount</t>
-  </si>
-  <si>
-    <t>PE - Peru</t>
-  </si>
-  <si>
-    <t>Create PP with Multiple Insitutional discounts</t>
-  </si>
-  <si>
-    <t>MultiInsti</t>
-  </si>
-  <si>
-    <t>Create PP with Manual override required value as Yes</t>
-  </si>
-  <si>
-    <t>ManualOverride</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid Promotional discount code</t>
-  </si>
-  <si>
-    <t>InvalidPromo</t>
-  </si>
-  <si>
-    <t>PRKMO50</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid Society</t>
-  </si>
-  <si>
-    <t>InvalidSociety</t>
-  </si>
-  <si>
-    <t>EANM</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid Article Type</t>
-  </si>
-  <si>
-    <t>InvalidArticleType</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid Editorial</t>
-  </si>
-  <si>
-    <t>InvalidEditorial</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid Referal</t>
-  </si>
-  <si>
-    <t>InvalidReferal</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid CountryCode</t>
-  </si>
-  <si>
-    <t>InvalidCountryCode</t>
-  </si>
-  <si>
-    <t>Create PP with Invalid MailId</t>
-  </si>
-  <si>
-    <t>InvalidMailId</t>
-  </si>
-  <si>
-    <t>Create PP Society discount with Rejected</t>
-  </si>
-  <si>
-    <t>Create PP Society discount with Withdrawn</t>
-  </si>
-  <si>
-    <t>ExeEnvironment</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1149,14 +1146,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2178,7 +2184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2192,103 +2198,103 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>238</v>
+        <v>140</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="U1" s="6" t="s">
-        <v>249</v>
+        <v>158</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>250</v>
+        <v>159</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>251</v>
+        <v>160</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>252</v>
+        <v>161</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>253</v>
+        <v>162</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>254</v>
+        <v>163</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>256</v>
+        <v>165</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>257</v>
+        <v>166</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>258</v>
+        <v>168</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="AI1" s="3" t="s">
         <v>70</v>
@@ -2302,31 +2308,31 @@
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="N2" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R2">
         <v>75</v>
@@ -2335,16 +2341,16 @@
         <v>5</v>
       </c>
       <c r="T2" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X2" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y2" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z2" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -2355,31 +2361,31 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>262</v>
+        <v>178</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="H3" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="N3" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R3">
         <v>75</v>
@@ -2388,16 +2394,16 @@
         <v>20</v>
       </c>
       <c r="T3" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X3" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y3" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z3" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -2408,49 +2414,49 @@
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>264</v>
+        <v>182</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>265</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>265</v>
+        <v>183</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>266</v>
+        <v>184</v>
       </c>
       <c r="N4" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R4">
         <v>75</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T4" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X4" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y4" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z4" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -2461,31 +2467,31 @@
         <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>267</v>
+        <v>185</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>268</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="N5" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R5">
         <v>20</v>
@@ -2494,16 +2500,16 @@
         <v>90</v>
       </c>
       <c r="T5" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X5" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y5" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z5" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:35">
@@ -2514,31 +2520,31 @@
         <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="E6" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="H6" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="N6" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -2547,16 +2553,16 @@
         <v>15.25</v>
       </c>
       <c r="T6" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X6" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y6" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z6" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -2567,31 +2573,31 @@
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>279</v>
+        <v>197</v>
       </c>
       <c r="H7" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>280</v>
+        <v>198</v>
       </c>
       <c r="N7" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R7">
         <v>30</v>
@@ -2600,16 +2606,16 @@
         <v>100</v>
       </c>
       <c r="T7" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X7" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y7" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z7" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -2620,49 +2626,49 @@
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>281</v>
+        <v>199</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="H8" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>282</v>
+        <v>200</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="N8" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R8">
         <v>75</v>
       </c>
       <c r="S8" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T8" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X8" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y8" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="Z8" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -2673,34 +2679,34 @@
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>283</v>
+        <v>201</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>284</v>
+        <v>202</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>265</v>
+        <v>183</v>
       </c>
       <c r="H9" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>266</v>
+        <v>184</v>
       </c>
       <c r="N9" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -2709,22 +2715,22 @@
         <v>75</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T9" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z9" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
@@ -2738,19 +2744,19 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="E10" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>23</v>
@@ -2759,13 +2765,13 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
@@ -2780,13 +2786,13 @@
         <v>5</v>
       </c>
       <c r="X10" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y10" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z10" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -2797,31 +2803,31 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>285</v>
+        <v>206</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>286</v>
+        <v>207</v>
       </c>
       <c r="E11" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>279</v>
+        <v>197</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>287</v>
+        <v>208</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
@@ -2833,19 +2839,19 @@
         <v>50</v>
       </c>
       <c r="T11" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U11" s="15"/>
       <c r="V11" s="15"/>
       <c r="W11" s="15"/>
       <c r="X11" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y11" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA11" s="15"/>
       <c r="AB11" s="15"/>
@@ -2859,46 +2865,46 @@
         <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>289</v>
+        <v>210</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>290</v>
+        <v>211</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" t="s">
+        <v>197</v>
+      </c>
+      <c r="I12" t="s">
         <v>212</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="H12" t="s">
-        <v>279</v>
-      </c>
-      <c r="I12" t="s">
-        <v>291</v>
       </c>
       <c r="J12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>282</v>
+        <v>200</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>271</v>
+        <v>189</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>292</v>
+        <v>213</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="R12" s="15">
         <v>75</v>
@@ -2919,22 +2925,22 @@
         <v>20</v>
       </c>
       <c r="X12" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y12" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z12" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="AA12" s="15" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="AB12" s="15" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="AC12" s="15" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -2945,55 +2951,55 @@
         <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>293</v>
+        <v>214</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>294</v>
+        <v>215</v>
       </c>
       <c r="E13" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="H13" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15"/>
       <c r="X13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="Y13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="Z13" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA13" s="15"/>
       <c r="AB13" s="15"/>
@@ -3007,58 +3013,58 @@
         <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>152</v>
+        <v>216</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U14" s="15"/>
       <c r="V14" s="15"/>
       <c r="W14" s="15"/>
       <c r="X14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="Y14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="Z14" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA14" s="15"/>
       <c r="AB14" s="15"/>
@@ -3069,31 +3075,31 @@
         <v>18</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>295</v>
+        <v>218</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>296</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
@@ -3105,19 +3111,19 @@
         <v>5</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U15" s="15"/>
       <c r="V15" s="15"/>
       <c r="W15" s="15"/>
       <c r="X15" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y15" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z15" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA15" s="15"/>
       <c r="AB15" s="15"/>
@@ -3131,31 +3137,31 @@
         <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>297</v>
+        <v>220</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>298</v>
+        <v>221</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>299</v>
+        <v>222</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
@@ -3164,22 +3170,22 @@
         <v>75</v>
       </c>
       <c r="S16" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T16" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U16" s="15"/>
       <c r="V16" s="15"/>
       <c r="W16" s="15"/>
       <c r="X16" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y16" s="15" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="Z16" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA16" s="15"/>
       <c r="AB16" s="15"/>
@@ -3190,34 +3196,34 @@
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>300</v>
+        <v>223</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>301</v>
+        <v>224</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M17" s="15" t="s">
-        <v>302</v>
+        <v>225</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -3226,22 +3232,22 @@
         <v>75</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="T17" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="U17" s="15"/>
       <c r="V17" s="15"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y17" s="15" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="Z17" s="15" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="AA17" s="15"/>
       <c r="AB17" s="15"/>
@@ -3252,13 +3258,13 @@
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>304</v>
+        <v>227</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:29">
@@ -3266,13 +3272,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>305</v>
+        <v>228</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>306</v>
+        <v>229</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -3280,13 +3286,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="D20" t="s">
-        <v>308</v>
+        <v>231</v>
       </c>
       <c r="E20" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:29">
@@ -3294,13 +3300,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>309</v>
+        <v>232</v>
       </c>
       <c r="D21" t="s">
-        <v>310</v>
+        <v>233</v>
       </c>
       <c r="E21" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -3308,13 +3314,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>311</v>
+        <v>234</v>
       </c>
       <c r="D22" t="s">
-        <v>312</v>
+        <v>235</v>
       </c>
       <c r="E22" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -3325,31 +3331,31 @@
         <v>18</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>313</v>
+        <v>236</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L23" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M23" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="N23" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R23">
         <v>75</v>
@@ -3358,16 +3364,16 @@
         <v>5</v>
       </c>
       <c r="T23" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X23" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y23" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z23" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -3378,31 +3384,31 @@
         <v>18</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="L24" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="M24" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="N24" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="R24">
         <v>75</v>
@@ -3411,16 +3417,16 @@
         <v>5</v>
       </c>
       <c r="T24" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="X24" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Y24" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="Z24" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3429,14 +3435,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3449,681 +3455,686 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
-        <v>139</v>
+        <v>238</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" t="s">
-        <v>145</v>
+        <v>167</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" t="s">
-        <v>148</v>
+      <c r="B4" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" t="s">
-        <v>150</v>
+        <v>247</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>154</v>
+        <v>249</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>158</v>
+      <c r="D8" s="20" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>161</v>
+        <v>250</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" t="s">
-        <v>163</v>
+        <v>252</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>167</v>
+        <v>254</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D12" t="s">
-        <v>169</v>
+        <v>256</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" t="s">
-        <v>170</v>
+      <c r="B13" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" t="s">
-        <v>171</v>
+      <c r="B14" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" t="s">
-        <v>173</v>
+        <v>260</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>176</v>
+        <v>262</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" t="s">
-        <v>178</v>
+        <v>265</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B18" s="14">
+        <v>267</v>
+      </c>
+      <c r="B18" s="21">
         <v>2221</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>180</v>
+      <c r="C18" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>181</v>
+      <c r="B19" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" t="s">
-        <v>183</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>184</v>
+        <v>270</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C21" t="s">
-        <v>186</v>
-      </c>
-      <c r="D21" t="s">
-        <v>186</v>
+        <v>273</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>189</v>
+        <v>275</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" t="s">
-        <v>173</v>
+        <v>279</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>193</v>
+        <v>280</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D25" t="s">
-        <v>193</v>
+        <v>283</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B26" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>197</v>
+        <v>285</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>199</v>
+        <v>287</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>202</v>
+        <v>289</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B29" t="s">
-        <v>204</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>205</v>
+        <v>292</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B30" t="s">
-        <v>201</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>201</v>
+        <v>295</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B31" t="s">
-        <v>201</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>201</v>
+        <v>296</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
-        <v>204</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>204</v>
+      <c r="B32" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B33" t="s">
-        <v>201</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>210</v>
+        <v>297</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>212</v>
+        <v>143</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="B35" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>161</v>
+        <v>149</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>218</v>
+        <v>300</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>220</v>
+        <v>301</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>205</v>
+        <v>303</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>223</v>
+        <v>304</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>223</v>
+        <v>305</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>227</v>
+        <v>306</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>230</v>
+        <v>309</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D44" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>217</v>
+        <v>151</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>226</v>
+        <v>312</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>235</v>
+        <v>313</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>229</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="19"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI Validations added V.23
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA008C4-3E8C-4222-BCE8-8DAE905CC9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F4B490-E015-4AD9-BEBF-B46B26BE6462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
     <sheet name="HappyFlowInputs" sheetId="2" r:id="rId2"/>
     <sheet name="PriceProposal" sheetId="3" r:id="rId3"/>
     <sheet name="UIValidations" sheetId="4" r:id="rId4"/>
+    <sheet name="OrderCreationCases" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="340">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -739,6 +740,12 @@
     <t>Create PP Society discount with Withdrawn</t>
   </si>
   <si>
+    <t>Verify UI Change Data Correction to Price Determined</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
     <t>HeaderCloumnName</t>
   </si>
   <si>
@@ -769,9 +776,6 @@
     <t>ResponseCode</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>CaseName</t>
   </si>
   <si>
@@ -968,13 +972,92 @@
   </si>
   <si>
     <t>Value3</t>
+  </si>
+  <si>
+    <t>TesctCaseName</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>ExecutionDate</t>
+  </si>
+  <si>
+    <t>Trigger Invoice Order with New Customer</t>
+  </si>
+  <si>
+    <t>UnPaidNewCustomer</t>
+  </si>
+  <si>
+    <t>3213528</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213528 for AS order 20240724115240</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using soldTo : 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using billTo: 0d523810-099a-4e82-bd65-0a0c16c03cb8","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213528 for AS order 20240724115240","version":"1.3.3-qa2.92","biId":"3213528"}}'}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115240 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-24\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f32600759\" title: \"Secrets of nature\" dhId: \"e0c7047c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" email: \"20240724115240@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240724115240@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" } } ] } }\t) { status data\t}}"
+}
+</t>
+  </si>
+  <si>
+    <t>2024-07-24 11:52:40.035</t>
+  </si>
+  <si>
+    <t>Trigger CreditCard Order with New Customer</t>
+  </si>
+  <si>
+    <t>CreditCardNewCustomer</t>
+  </si>
+  <si>
+    <t>3213529</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213529 for AS order 20240724115242</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using soldTo : cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using billTo: cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213529 for AS order 20240724115242","version":"1.3.3-qa2.92","biId":"3213529"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115242 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f23495525\" title: \"Secrets of volcano\" dhId: \"e0c2068c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" email: \"20240724115242@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-24T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240724115242@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-07-24 11:52:42.471</t>
+  </si>
+  <si>
+    <t>Trigger Alipay Order with New Customer</t>
+  </si>
+  <si>
+    <t>AlipayNewCustomer</t>
+  </si>
+  <si>
+    <t>3213530</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213530 for AS order 20240724115245</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using soldTo : cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using billTo: cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213530 for AS order 20240724115245","version":"1.3.3-qa2.92","biId":"3213530"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115245 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f73332373\" title: \"Secrets of nature\" dhId: \"e0c2581c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" email: \"20240724115245@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240724115245@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-07-24 11:52:45.100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,14 +1093,13 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF871094"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1078,6 +1160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1117,7 +1205,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1143,27 +1231,20 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1452,11 +1533,11 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.90625" bestFit="1" customWidth="1"/>
@@ -1472,7 +1553,7 @@
     <col min="18" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +1653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1616,7 +1697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1688,7 +1769,7 @@
       <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
@@ -1716,7 +1797,7 @@
     <col min="29" max="29" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -1811,7 +1892,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1888,7 +1969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1959,7 +2040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2012,7 +2093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2065,7 +2146,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2121,7 +2202,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2185,15 +2266,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AI24"/>
+  <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB30" sqref="AB30"/>
+    <sheetView tabSelected="1" topLeftCell="P21" workbookViewId="0">
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -2300,7 +2385,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2316,10 +2401,10 @@
       <c r="E2" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
@@ -2353,7 +2438,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2406,7 +2491,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2459,7 +2544,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2512,7 +2597,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2565,7 +2650,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2618,7 +2703,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2671,7 +2756,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2736,7 +2821,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2795,7 +2880,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2857,7 +2942,7 @@
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2943,7 +3028,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3005,7 +3090,7 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3070,7 +3155,7 @@
       <c r="AB14" s="15"/>
       <c r="AC14" s="15"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -3129,7 +3214,7 @@
       <c r="AB15" s="15"/>
       <c r="AC15" s="15"/>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3191,7 +3276,7 @@
       <c r="AB16" s="15"/>
       <c r="AC16" s="15"/>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -3253,7 +3338,7 @@
       <c r="AB17" s="15"/>
       <c r="AC17" s="15"/>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -3267,7 +3352,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -3281,7 +3366,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -3295,7 +3380,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3309,7 +3394,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -3323,7 +3408,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -3339,10 +3424,10 @@
       <c r="E23" t="s">
         <v>172</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" t="s">
         <v>173</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="H23" t="s">
@@ -3376,7 +3461,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3392,10 +3477,10 @@
       <c r="E24" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" t="s">
         <v>173</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" t="s">
         <v>23</v>
       </c>
       <c r="H24" t="s">
@@ -3428,6 +3513,69 @@
       <c r="Z24" t="s">
         <v>174</v>
       </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="22">
+        <v>75</v>
+      </c>
+      <c r="S25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="T25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y25" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3439,13 +3587,13 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.7265625" customWidth="1"/>
@@ -3453,682 +3601,677 @@
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="B3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="B4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="C4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B6" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" t="s">
         <v>216</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" t="s">
         <v>217</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="B11" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B12" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="B15" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="B16" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="C16" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B17" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="B18" s="21">
+        <v>268</v>
+      </c>
+      <c r="B18" s="14">
         <v>2221</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="C18" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="B20" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="B20" t="s">
         <v>272</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="C20" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B21" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="B21" t="s">
+        <v>275</v>
+      </c>
+      <c r="C21" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="B22" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="B22" t="s">
         <v>277</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="C22" s="14" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>280</v>
+      </c>
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="B24" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="B24" t="s">
         <v>282</v>
       </c>
-      <c r="D24" s="21" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="C24" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="B26" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="B26" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B27" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="B27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="B28" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="B28" t="s">
         <v>291</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="C28" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>293</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="C30" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>297</v>
+      </c>
+      <c r="B31" t="s">
+        <v>291</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>293</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="B32" t="s">
+        <v>294</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C33" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="B33" t="s">
+        <v>291</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="14" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C35" s="21" t="s">
+      <c r="B35" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C36" s="21" t="s">
+      <c r="B36" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C37" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C38" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="B38" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>304</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C41" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C42" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="B42" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C42" s="20" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C43" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="B43" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="D43" s="14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D44" s="21" t="s">
+      <c r="B44" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D45" s="21" t="s">
+      <c r="B45" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>313</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D47" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="19"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="19"/>
+        <v>315</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>311</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4138,4 +4281,156 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H3" t="s">
+        <v>330</v>
+      </c>
+      <c r="I3" t="s">
+        <v>331</v>
+      </c>
+      <c r="J3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" t="s">
+        <v>336</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" t="s">
+        <v>338</v>
+      </c>
+      <c r="J4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UI Validations added V.30
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F4B490-E015-4AD9-BEBF-B46B26BE6462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6285F448-0FF9-43F8-8AAD-AAF9A0ADD6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HappyFlowData" sheetId="1" r:id="rId1"/>
     <sheet name="HappyFlowInputs" sheetId="2" r:id="rId2"/>
     <sheet name="PriceProposal" sheetId="3" r:id="rId3"/>
-    <sheet name="UIValidations" sheetId="4" r:id="rId4"/>
-    <sheet name="OrderCreationCases" sheetId="5" r:id="rId5"/>
+    <sheet name="OrderCreationCases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="300">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -743,268 +742,49 @@
     <t>Verify UI Change Data Correction to Price Determined</t>
   </si>
   <si>
+    <t>TesctCaseName</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>ExecutionDate</t>
+  </si>
+  <si>
+    <t>Trigger Invoice Order with New Customer</t>
+  </si>
+  <si>
+    <t>UnPaidNewCustomer</t>
+  </si>
+  <si>
+    <t>20240725124413Test</t>
+  </si>
+  <si>
+    <t>20240725124413Auto</t>
+  </si>
+  <si>
+    <t>20240725124413@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213549</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213549 for AS order 20240725124413</t>
+  </si>
+  <si>
     <t>200</t>
   </si>
   <si>
-    <t>HeaderCloumnName</t>
-  </si>
-  <si>
-    <t>Multiple</t>
-  </si>
-  <si>
-    <t>ExeEnvironment</t>
-  </si>
-  <si>
-    <t>7242608</t>
-  </si>
-  <si>
-    <t>7242609</t>
-  </si>
-  <si>
-    <t>7242610</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242608 for PriceProposal 24ef3969-549b-4808-9127-af8e42410838</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242609 for PriceProposal 24ef5143-857b-4808-9127-af8e42410958</t>
-  </si>
-  <si>
-    <t>Created Viax order 7242610 for PriceProposal 24ef5787-856b-4808-9127-af8e42410444</t>
-  </si>
-  <si>
-    <t>ResponseCode</t>
-  </si>
-  <si>
-    <t>CaseName</t>
-  </si>
-  <si>
-    <t>BaseArticleType</t>
-  </si>
-  <si>
-    <t>Data Article</t>
-  </si>
-  <si>
-    <t>DisplayArticleType</t>
-  </si>
-  <si>
-    <t>Research Article (ABC)</t>
-  </si>
-  <si>
-    <t>SubmissionDate</t>
-  </si>
-  <si>
-    <t>07-16-2024</t>
-  </si>
-  <si>
-    <t>ArticleTitle</t>
-  </si>
-  <si>
-    <t>Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>TESSON</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Jim TESSON</t>
-  </si>
-  <si>
-    <t>EmailID</t>
-  </si>
-  <si>
-    <t>TestAuto@wiley.com</t>
-  </si>
-  <si>
-    <t>TestAutomation@Wiley.com</t>
-  </si>
-  <si>
-    <t>InstitutionIdType</t>
-  </si>
-  <si>
-    <t>Ringgold</t>
-  </si>
-  <si>
-    <t>InstitutionId</t>
-  </si>
-  <si>
-    <t>N.A</t>
-  </si>
-  <si>
-    <t>US - United States</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>Universidad Nacional De Ingenieria</t>
-  </si>
-  <si>
-    <t>Grant Institute</t>
-  </si>
-  <si>
-    <t>PublishedIn</t>
-  </si>
-  <si>
-    <t>Cancer Medicine</t>
-  </si>
-  <si>
-    <t>MauScriptId</t>
-  </si>
-  <si>
-    <t>CAM4-2024-04-3969</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-5143</t>
-  </si>
-  <si>
-    <t>ACN3-2023-06-5787</t>
-  </si>
-  <si>
-    <t>SubmittedBy</t>
-  </si>
-  <si>
-    <t>FunderName</t>
-  </si>
-  <si>
-    <t>ARC of the Piedmont (The Arc)</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>FunderId</t>
-  </si>
-  <si>
-    <t>10.13039/100006467</t>
-  </si>
-  <si>
-    <t>EditorialStatus</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>JournalGroupCode</t>
-  </si>
-  <si>
-    <t>CAM4</t>
-  </si>
-  <si>
-    <t>BaseAPCPrice</t>
-  </si>
-  <si>
-    <t>800.00 USD</t>
-  </si>
-  <si>
-    <t>200.00 USD</t>
-  </si>
-  <si>
-    <t>BaseArticleTypeDiscount</t>
-  </si>
-  <si>
-    <t>0.00 USD</t>
-  </si>
-  <si>
-    <t>600.00 USD</t>
-  </si>
-  <si>
-    <t>BaseAPCCharge</t>
-  </si>
-  <si>
-    <t>FinalNetPrice</t>
-  </si>
-  <si>
-    <t>TotalCharge</t>
-  </si>
-  <si>
-    <t>190.00 USD</t>
-  </si>
-  <si>
-    <t>160.00 USD</t>
-  </si>
-  <si>
-    <t>DiscountCondition2</t>
-  </si>
-  <si>
-    <t>Percentage1</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Applied1</t>
-  </si>
-  <si>
-    <t>Applied2</t>
-  </si>
-  <si>
-    <t>Percentage2</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
-    <t>10.00 USD</t>
-  </si>
-  <si>
-    <t>40.00 USD</t>
-  </si>
-  <si>
-    <t>Percentage3</t>
-  </si>
-  <si>
-    <t>Applied3</t>
-  </si>
-  <si>
-    <t>Value3</t>
-  </si>
-  <si>
-    <t>TesctCaseName</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>ExecutionDate</t>
-  </si>
-  <si>
-    <t>Trigger Invoice Order with New Customer</t>
-  </si>
-  <si>
-    <t>UnPaidNewCustomer</t>
-  </si>
-  <si>
-    <t>3213528</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213528 for AS order 20240724115240</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using soldTo : 0d523810-099a-4e82-bd65-0a0c16c03cb8","Using billTo: 0d523810-099a-4e82-bd65-0a0c16c03cb8","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213528 for AS order 20240724115240","version":"1.3.3-qa2.92","biId":"3213528"}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Using soldTo : 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Using billTo: 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213549 for AS order 20240725124413","version":"1.3.3-qa2.92","biId":"3213549"}}'}}}</t>
   </si>
   <si>
     <t xml:space="preserve">{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115240 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-24\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f32600759\" title: \"Secrets of nature\" dhId: \"e0c7047c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" email: \"20240724115240@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240724115240Test\" lastName: \"20240724115240Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240724115240@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e754a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e611a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124413 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-25\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f84363986\" title: \"Secrets of nature\" dhId: \"e0c3500c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240725124413Test\" lastName: \"20240725124413Auto\" email: \"20240725124413@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240725124413Test\" lastName: \"20240725124413Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240725124413@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e611a\" } } ] } }\t) { status data\t}}"
 }
 </t>
   </si>
   <si>
-    <t>2024-07-24 11:52:40.035</t>
+    <t>2024-07-25 12:44:13.240</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with New Customer</t>
@@ -1013,21 +793,30 @@
     <t>CreditCardNewCustomer</t>
   </si>
   <si>
-    <t>3213529</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213529 for AS order 20240724115242</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using soldTo : cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Using billTo: cb12cb1e-fba2-49b9-970f-ba42ff2cc8af","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213529 for AS order 20240724115242","version":"1.3.3-qa2.92","biId":"3213529"}}'}}}</t>
+    <t>20240725124414Test</t>
+  </si>
+  <si>
+    <t>20240725124414Auto</t>
+  </si>
+  <si>
+    <t>20240725124414@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213550</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213550 for AS order 20240725124414</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Using soldTo : 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Using billTo: 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213550 for AS order 20240725124414","version":"1.3.3-qa2.92","biId":"3213550"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115242 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f23495525\" title: \"Secrets of volcano\" dhId: \"e0c2068c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" email: \"20240724115242@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-24T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240724115242Test\" lastName: \"20240724115242Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240724115242@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e823a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e444a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124414 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f77072811\" title: \"Secrets of volcano\" dhId: \"e0c5454c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725124414Test\" lastName: \"20240725124414Auto\" email: \"20240725124414@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-25T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240725124414Test\" lastName: \"20240725124414Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240725124414@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e444a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-07-24 11:52:42.471</t>
+    <t>2024-07-25 12:44:14.800</t>
   </si>
   <si>
     <t>Trigger Alipay Order with New Customer</t>
@@ -1036,28 +825,125 @@
     <t>AlipayNewCustomer</t>
   </si>
   <si>
-    <t>3213530</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213530 for AS order 20240724115245</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using soldTo : cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Using billTo: cfbd48fd-2e75-4ab1-a222-18a20241e8f3","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213530 for AS order 20240724115245","version":"1.3.3-qa2.92","biId":"3213530"}}'}}}</t>
+    <t>20240725124417Test</t>
+  </si>
+  <si>
+    <t>20240725124417Auto</t>
+  </si>
+  <si>
+    <t>20240725124417@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213551</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213551 for AS order 20240725124417</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP a518b16b-f6a9-4bf6-896f-64498fd5582f","Using soldTo : a518b16b-f6a9-4bf6-896f-64498fd5582f","Using billTo: a518b16b-f6a9-4bf6-896f-64498fd5582f","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213551 for AS order 20240725124417","version":"1.3.3-qa2.92","biId":"3213551"}}'}}}</t>
   </si>
   <si>
     <t>{
-	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240724115245 submittedDate: \"2024-07-24T15:00:14-05\" createdDate: \"2024-07-24T15:00:14-05\" cancelDate: \"2024-07-24T15:00:14-05\" paymentDate: \"2024-07-24T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-24T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f73332373\" title: \"Secrets of nature\" dhId: \"e0c2581c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" email: \"20240724115245@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240724115245Test\" lastName: \"20240724115245Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240724115245@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
+	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e384a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124417 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f69105972\" title: \"Secrets of nature\" dhId: \"e0c3874c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725124417Test\" lastName: \"20240725124417Auto\" email: \"20240725124417@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240725124417Test\" lastName: \"20240725124417Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240725124417@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e384a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-07-24 11:52:45.100</t>
+    <t>2024-07-25 12:44:17.023</t>
+  </si>
+  <si>
+    <t>Trigger Invoice Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>20240725122330Test</t>
+  </si>
+  <si>
+    <t>20240725122330Auto</t>
+  </si>
+  <si>
+    <t>20240725122330@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213554</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213554 for AS order 20240725124428</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 01293557-6002-473a-8703-9b00d7c74746","Using billTo: 01293557-6002-473a-8703-9b00d7c74746","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213554 for AS order 20240725124428","version":"1.3.3-qa2.92","biId":"3213554"}}'}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e478a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124428 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-25\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f68616279\" title: \"Secrets of nature\" dhId: \"e0c4085c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" email: \"20240725122330@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240725122330@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e478a\" } } ] } }\t) { status data\t}}"
+}
+</t>
+  </si>
+  <si>
+    <t>2024-07-25 12:44:28.437</t>
+  </si>
+  <si>
+    <t>Trigger CreditCard Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>20240725122331Test</t>
+  </si>
+  <si>
+    <t>20240725122331Auto</t>
+  </si>
+  <si>
+    <t>20240725122331@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213553</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213553 for AS order 20240725124423</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 33a93dba-b930-4819-99f3-9b0c7cdf3177","Using billTo: 33a93dba-b930-4819-99f3-9b0c7cdf3177","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213553 for AS order 20240725124423","version":"1.3.3-qa2.92","biId":"3213553"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e323a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124423 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f48910586\" title: \"Secrets of volcano\" dhId: \"e0c4141c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" email: \"20240725122331@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-25T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240725122331@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e323a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-07-25 12:44:23.004</t>
+  </si>
+  <si>
+    <t>Trigger Alipay Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>20240725122333Test</t>
+  </si>
+  <si>
+    <t>20240725122333Auto</t>
+  </si>
+  <si>
+    <t>20240725122333@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213552</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213552 for AS order 20240725124421</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 98a00db8-47be-4f1e-9218-872a83a124aa","Using billTo: 98a00db8-47be-4f1e-9218-872a83a124aa","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213552 for AS order 20240725124421","version":"1.3.3-qa2.92","biId":"3213552"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e586a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124421 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62930726\" title: \"Secrets of nature\" dhId: \"e0c2896c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" email: \"20240725122333@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240725122333@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e586a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-07-25 12:44:21.072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1080,13 +966,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF39373E"/>
       <name val="Arial"/>
@@ -1099,7 +978,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,18 +1023,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1167,27 +1034,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1200,12 +1052,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1221,34 +1072,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1766,7 +1600,7 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2268,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P21" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2401,10 +2235,10 @@
       <c r="E2" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H2" t="s">
@@ -2454,19 +2288,19 @@
       <c r="E3" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>180</v>
       </c>
       <c r="H3" t="s">
         <v>174</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="11" t="s">
         <v>181</v>
       </c>
       <c r="N3" t="s">
@@ -2481,10 +2315,10 @@
       <c r="T3" t="s">
         <v>174</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z3" t="s">
@@ -2507,19 +2341,19 @@
       <c r="E4" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>183</v>
       </c>
       <c r="H4" t="s">
         <v>174</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="11" t="s">
         <v>184</v>
       </c>
       <c r="N4" t="s">
@@ -2528,16 +2362,16 @@
       <c r="R4">
         <v>75</v>
       </c>
-      <c r="S4" s="15" t="s">
+      <c r="S4" s="11" t="s">
         <v>174</v>
       </c>
       <c r="T4" t="s">
         <v>174</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="X4" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y4" s="15" t="s">
+      <c r="Y4" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z4" t="s">
@@ -2560,19 +2394,19 @@
       <c r="E5" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>187</v>
       </c>
       <c r="H5" t="s">
         <v>174</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="11" t="s">
         <v>189</v>
       </c>
       <c r="N5" t="s">
@@ -2587,10 +2421,10 @@
       <c r="T5" t="s">
         <v>174</v>
       </c>
-      <c r="X5" s="15" t="s">
+      <c r="X5" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z5" t="s">
@@ -2613,19 +2447,19 @@
       <c r="E6" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>193</v>
       </c>
       <c r="H6" t="s">
         <v>174</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="11" t="s">
         <v>174</v>
       </c>
       <c r="N6" t="s">
@@ -2640,10 +2474,10 @@
       <c r="T6" t="s">
         <v>174</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="X6" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z6" t="s">
@@ -2666,19 +2500,19 @@
       <c r="E7" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="11" t="s">
         <v>197</v>
       </c>
       <c r="H7" t="s">
         <v>174</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="11" t="s">
         <v>198</v>
       </c>
       <c r="N7" t="s">
@@ -2693,10 +2527,10 @@
       <c r="T7" t="s">
         <v>174</v>
       </c>
-      <c r="X7" s="15" t="s">
+      <c r="X7" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y7" s="15" t="s">
+      <c r="Y7" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z7" t="s">
@@ -2719,19 +2553,19 @@
       <c r="E8" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="11" t="s">
         <v>174</v>
       </c>
       <c r="H8" t="s">
         <v>174</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="11" t="s">
         <v>174</v>
       </c>
       <c r="N8" t="s">
@@ -2740,16 +2574,16 @@
       <c r="R8">
         <v>75</v>
       </c>
-      <c r="S8" s="15" t="s">
+      <c r="S8" s="11" t="s">
         <v>174</v>
       </c>
       <c r="T8" t="s">
         <v>174</v>
       </c>
-      <c r="X8" s="15" t="s">
+      <c r="X8" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y8" s="15" t="s">
+      <c r="Y8" s="11" t="s">
         <v>174</v>
       </c>
       <c r="Z8" t="s">
@@ -2772,10 +2606,10 @@
       <c r="E9" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="11" t="s">
         <v>183</v>
       </c>
       <c r="H9" t="s">
@@ -2784,10 +2618,10 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="11" t="s">
         <v>184</v>
       </c>
       <c r="N9" t="s">
@@ -2799,7 +2633,7 @@
       <c r="R9" s="7">
         <v>75</v>
       </c>
-      <c r="S9" s="15" t="s">
+      <c r="S9" s="11" t="s">
         <v>174</v>
       </c>
       <c r="T9" t="s">
@@ -2837,30 +2671,30 @@
       <c r="E10" t="s">
         <v>172</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15" t="s">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
       <c r="R10">
         <v>75</v>
       </c>
@@ -2870,10 +2704,10 @@
       <c r="T10">
         <v>5</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="X10" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y10" s="15" t="s">
+      <c r="Y10" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z10" t="s">
@@ -2896,51 +2730,51 @@
       <c r="E11" t="s">
         <v>172</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H11" t="s">
         <v>174</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="N11" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
+      <c r="N11" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
       <c r="R11">
         <v>50</v>
       </c>
       <c r="S11">
         <v>50</v>
       </c>
-      <c r="T11" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15" t="s">
+      <c r="T11" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y11" s="15" t="s">
+      <c r="Y11" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Z11" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
+      <c r="Z11" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -2958,10 +2792,10 @@
       <c r="E12" t="s">
         <v>172</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="11" t="s">
         <v>187</v>
       </c>
       <c r="H12" t="s">
@@ -2970,61 +2804,61 @@
       <c r="I12" t="s">
         <v>212</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="Q12" s="15" t="s">
+      <c r="Q12" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="11">
         <v>75</v>
       </c>
       <c r="S12">
         <v>90</v>
       </c>
-      <c r="T12" s="15">
+      <c r="T12" s="11">
         <v>50</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U12" s="11">
         <v>50</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V12" s="11">
         <v>5</v>
       </c>
-      <c r="W12" s="15">
+      <c r="W12" s="11">
         <v>20</v>
       </c>
-      <c r="X12" s="15" t="s">
+      <c r="X12" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y12" s="15" t="s">
+      <c r="Y12" s="11" t="s">
         <v>177</v>
       </c>
       <c r="Z12" t="s">
         <v>205</v>
       </c>
-      <c r="AA12" s="15" t="s">
+      <c r="AA12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="AB12" s="15" t="s">
+      <c r="AB12" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="AC12" s="15" t="s">
+      <c r="AC12" s="11" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3044,51 +2878,51 @@
       <c r="E13" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>174</v>
       </c>
       <c r="H13" t="s">
         <v>174</v>
       </c>
-      <c r="L13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="T13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="Z13" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="15"/>
+      <c r="L13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
     </row>
     <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
@@ -3106,54 +2940,54 @@
       <c r="E14" t="s">
         <v>172</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="N14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="S14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="T14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="Z14" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
+      <c r="F14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
@@ -3168,51 +3002,51 @@
       <c r="E15" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>174</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="N15" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
+      <c r="N15" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
       <c r="R15">
         <v>75</v>
       </c>
       <c r="S15">
         <v>5</v>
       </c>
-      <c r="T15" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15" t="s">
+      <c r="T15" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y15" s="15" t="s">
+      <c r="Y15" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Z15" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
+      <c r="Z15" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -3230,51 +3064,51 @@
       <c r="E16" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="11" t="s">
         <v>180</v>
       </c>
       <c r="H16" t="s">
         <v>174</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="N16" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
+      <c r="N16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
       <c r="R16">
         <v>75</v>
       </c>
       <c r="S16" t="s">
         <v>174</v>
       </c>
-      <c r="T16" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15" t="s">
+      <c r="T16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y16" s="15" t="s">
+      <c r="Y16" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="Z16" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
+      <c r="Z16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -3289,54 +3123,54 @@
       <c r="E17" t="s">
         <v>172</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15" t="s">
+      <c r="H17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="N17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
+      <c r="N17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
       <c r="R17">
         <v>75</v>
       </c>
-      <c r="S17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="T17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15" t="s">
+      <c r="S17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y17" s="15" t="s">
+      <c r="Y17" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="Z17" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="15"/>
+      <c r="Z17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
@@ -3515,17 +3349,17 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="13" t="s">
         <v>172</v>
       </c>
       <c r="F25" t="s">
@@ -3534,48 +3368,48 @@
       <c r="G25" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15" t="s">
+      <c r="H25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="N25" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="22">
+      <c r="N25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="13">
         <v>75</v>
       </c>
-      <c r="S25" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="T25" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15" t="s">
+      <c r="S25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="T25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="Y25" s="15" t="s">
+      <c r="Y25" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="Z25" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
+      <c r="Z25" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3584,850 +3418,310 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7265625" customWidth="1"/>
-    <col min="3" max="3" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C13" t="s">
-        <v>259</v>
-      </c>
-      <c r="D13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>260</v>
-      </c>
-      <c r="C14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D14" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="B15" t="s">
-        <v>262</v>
-      </c>
-      <c r="C15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="B17" t="s">
-        <v>267</v>
-      </c>
-      <c r="C17" t="s">
-        <v>267</v>
-      </c>
-      <c r="D17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="B18" s="14">
-        <v>2221</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>270</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="B20" t="s">
-        <v>272</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B21" t="s">
-        <v>275</v>
-      </c>
-      <c r="C21" t="s">
-        <v>275</v>
-      </c>
-      <c r="D21" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="B22" t="s">
-        <v>277</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="B23" t="s">
-        <v>262</v>
-      </c>
-      <c r="C23" t="s">
-        <v>262</v>
-      </c>
-      <c r="D23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B24" t="s">
-        <v>282</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B25" t="s">
-        <v>285</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D25" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="B26" t="s">
-        <v>287</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="B27" t="s">
-        <v>289</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="B28" t="s">
-        <v>291</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="B29" t="s">
-        <v>294</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B30" t="s">
-        <v>291</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B31" t="s">
-        <v>291</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>294</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="B33" t="s">
-        <v>291</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="D16" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.81640625" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>316</v>
+        <v>239</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>317</v>
+        <v>240</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M1" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>320</v>
+        <v>243</v>
       </c>
       <c r="E2" t="s">
-        <v>321</v>
+        <v>244</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>239</v>
+        <v>245</v>
+      </c>
+      <c r="G2" t="s">
+        <v>246</v>
       </c>
       <c r="H2" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c r="I2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2" t="s">
+        <v>250</v>
+      </c>
+      <c r="L2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>254</v>
       </c>
       <c r="E3" t="s">
-        <v>328</v>
+        <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>329</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>239</v>
+        <v>256</v>
+      </c>
+      <c r="G3" t="s">
+        <v>257</v>
       </c>
       <c r="H3" t="s">
-        <v>330</v>
+        <v>258</v>
       </c>
       <c r="I3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L3" t="s">
+        <v>261</v>
+      </c>
+      <c r="M3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>264</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>265</v>
       </c>
       <c r="F4" t="s">
-        <v>336</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>239</v>
+        <v>266</v>
+      </c>
+      <c r="G4" t="s">
+        <v>267</v>
       </c>
       <c r="H4" t="s">
-        <v>337</v>
+        <v>268</v>
       </c>
       <c r="I4" t="s">
-        <v>338</v>
-      </c>
-      <c r="J4" t="s">
-        <v>339</v>
+        <v>269</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" t="s">
+        <v>270</v>
+      </c>
+      <c r="L4" t="s">
+        <v>271</v>
+      </c>
+      <c r="M4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H5" t="s">
+        <v>277</v>
+      </c>
+      <c r="I5" t="s">
+        <v>278</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K5" t="s">
+        <v>279</v>
+      </c>
+      <c r="L5" t="s">
+        <v>280</v>
+      </c>
+      <c r="M5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I6" t="s">
+        <v>287</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K6" t="s">
+        <v>288</v>
+      </c>
+      <c r="L6" t="s">
+        <v>289</v>
+      </c>
+      <c r="M6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" t="s">
+        <v>292</v>
+      </c>
+      <c r="F7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G7" t="s">
+        <v>294</v>
+      </c>
+      <c r="H7" t="s">
+        <v>295</v>
+      </c>
+      <c r="I7" t="s">
+        <v>296</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K7" t="s">
+        <v>297</v>
+      </c>
+      <c r="L7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M7" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.35
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\TestSuites\UploadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6285F448-0FF9-43F8-8AAD-AAF9A0ADD6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A1F1C-D01B-4DDB-B8DC-5CD7CF171B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="314">
   <si>
     <t>ExecutionEnvironment</t>
   </si>
@@ -757,34 +757,34 @@
     <t>UnPaidNewCustomer</t>
   </si>
   <si>
-    <t>20240725124413Test</t>
-  </si>
-  <si>
-    <t>20240725124413Auto</t>
-  </si>
-  <si>
-    <t>20240725124413@Wiley.com</t>
-  </si>
-  <si>
-    <t>3213549</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213549 for AS order 20240725124413</t>
+    <t>20240729155518Test</t>
+  </si>
+  <si>
+    <t>20240729155518Auto</t>
+  </si>
+  <si>
+    <t>20240729155518@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213591</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213591 for AS order 20240729155518</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Using soldTo : 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Using billTo: 13cfdfc9-f6db-4cd9-9dd4-8480f22a6841","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213549 for AS order 20240725124413","version":"1.3.3-qa2.92","biId":"3213549"}}'}}}</t>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 2b869c74-80fe-42f3-a730-058107236e8b","Using soldTo : 2b869c74-80fe-42f3-a730-058107236e8b","Using billTo: 2b869c74-80fe-42f3-a730-058107236e8b","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213591 for AS order 20240729155518","version":"1.3.3-qa2.92","biId":"3213591"}}'}}}</t>
   </si>
   <si>
     <t xml:space="preserve">{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e611a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124413 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-25\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f84363986\" title: \"Secrets of nature\" dhId: \"e0c3500c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240725124413Test\" lastName: \"20240725124413Auto\" email: \"20240725124413@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240725124413Test\" lastName: \"20240725124413Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240725124413@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e611a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e762a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155518 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-29\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f75816419\" title: \"Secrets of nature\" dhId: \"e0c7405c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240729155518Test\" lastName: \"20240729155518Auto\" email: \"20240729155518@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240729155518Test\" lastName: \"20240729155518Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240729155518@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e762a\" } } ] } }\t) { status data\t}}"
 }
 </t>
   </si>
   <si>
-    <t>2024-07-25 12:44:13.240</t>
+    <t>2024-07-29 15:55:18.655</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with New Customer</t>
@@ -793,92 +793,122 @@
     <t>CreditCardNewCustomer</t>
   </si>
   <si>
-    <t>20240725124414Test</t>
-  </si>
-  <si>
-    <t>20240725124414Auto</t>
-  </si>
-  <si>
-    <t>20240725124414@Wiley.com</t>
-  </si>
-  <si>
-    <t>3213550</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213550 for AS order 20240725124414</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Using soldTo : 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Using billTo: 7e8494cc-fd0e-4db4-b07b-36abf27e31ee","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213550 for AS order 20240725124414","version":"1.3.3-qa2.92","biId":"3213550"}}'}}}</t>
+    <t>20240729155520Test</t>
+  </si>
+  <si>
+    <t>20240729155520Auto</t>
+  </si>
+  <si>
+    <t>20240729155520@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213592</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213592 for AS order 20240729155520</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP e52281e6-208d-45b2-abda-49002d3de769","Using soldTo : e52281e6-208d-45b2-abda-49002d3de769","Using billTo: e52281e6-208d-45b2-abda-49002d3de769","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213592 for AS order 20240729155520","version":"1.3.3-qa2.92","biId":"3213592"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e444a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124414 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f77072811\" title: \"Secrets of volcano\" dhId: \"e0c5454c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725124414Test\" lastName: \"20240725124414Auto\" email: \"20240725124414@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-25T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240725124414Test\" lastName: \"20240725124414Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240725124414@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e444a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e276a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155520 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f72283919\" title: \"Secrets of volcano\" dhId: \"e0c9824c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240729155520Test\" lastName: \"20240729155520Auto\" email: \"20240729155520@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-29T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240729155520Test\" lastName: \"20240729155520Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240729155520@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e276a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-07-25 12:44:14.800</t>
-  </si>
-  <si>
-    <t>Trigger Alipay Order with New Customer</t>
-  </si>
-  <si>
-    <t>AlipayNewCustomer</t>
-  </si>
-  <si>
-    <t>20240725124417Test</t>
-  </si>
-  <si>
-    <t>20240725124417Auto</t>
-  </si>
-  <si>
-    <t>20240725124417@Wiley.com</t>
-  </si>
-  <si>
-    <t>3213551</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213551 for AS order 20240725124417</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP a518b16b-f6a9-4bf6-896f-64498fd5582f","Using soldTo : a518b16b-f6a9-4bf6-896f-64498fd5582f","Using billTo: a518b16b-f6a9-4bf6-896f-64498fd5582f","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213551 for AS order 20240725124417","version":"1.3.3-qa2.92","biId":"3213551"}}'}}}</t>
-  </si>
-  <si>
-    <t>{
-	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e384a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124417 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f69105972\" title: \"Secrets of nature\" dhId: \"e0c3874c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725124417Test\" lastName: \"20240725124417Auto\" email: \"20240725124417@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240725124417Test\" lastName: \"20240725124417Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240725124417@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e384a\" } } ] } }\t) { status data\t}}"
-}</t>
-  </si>
-  <si>
-    <t>2024-07-25 12:44:17.023</t>
-  </si>
-  <si>
-    <t>Trigger Invoice Order with Existing Customer</t>
-  </si>
-  <si>
-    <t>20240725122330Test</t>
-  </si>
-  <si>
-    <t>20240725122330Auto</t>
-  </si>
-  <si>
-    <t>20240725122330@Wiley.com</t>
-  </si>
-  <si>
-    <t>3213554</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213554 for AS order 20240725124428</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 01293557-6002-473a-8703-9b00d7c74746","Using billTo: 01293557-6002-473a-8703-9b00d7c74746","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213554 for AS order 20240725124428","version":"1.3.3-qa2.92","biId":"3213554"}}'}}}</t>
+    <t>2024-07-29 15:55:20.578</t>
+  </si>
+  <si>
+    <t>Trigger Proforma Order with New Customer</t>
+  </si>
+  <si>
+    <t>Proforma</t>
+  </si>
+  <si>
+    <t>20240729155541Test</t>
+  </si>
+  <si>
+    <t>20240729155541Auto</t>
+  </si>
+  <si>
+    <t>20240729155541@Wiley.com</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213597 for AS order 20240729155541</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 45ed1df4-925b-4f04-b9e1-6d1ac150e613","Using soldTo : 45ed1df4-925b-4f04-b9e1-6d1ac150e613","Using billTo: 45ed1df4-925b-4f04-b9e1-6d1ac150e613","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213597 for AS order 20240729155541","version":"1.3.3-qa2.92","biId":"3213597"}}'}}}</t>
   </si>
   <si>
     <t xml:space="preserve">{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e478a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124428 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-25\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f68616279\" title: \"Secrets of nature\" dhId: \"e0c4085c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" email: \"20240725122330@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240725122330@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e478a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e543a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155541 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 0.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-29\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f80753492\" title: \"Secrets of nature\" dhId: \"e0c2871c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240729155541Test\" lastName: \"20240729155541Auto\" email: \"20240729155541@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240729155541Test\" lastName: \"20240729155541Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240729155541@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e543a\" } } ] } }\t) { status data\t}}"
 }
 </t>
   </si>
   <si>
-    <t>2024-07-25 12:44:28.437</t>
+    <t>2024-07-29 15:55:41.629</t>
+  </si>
+  <si>
+    <t>Trigger Alipay Order with New Customer</t>
+  </si>
+  <si>
+    <t>AlipayNewCustomer</t>
+  </si>
+  <si>
+    <t>20240729155523Test</t>
+  </si>
+  <si>
+    <t>20240729155523Auto</t>
+  </si>
+  <si>
+    <t>20240729155523@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213593</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213593 for AS order 20240729155523</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 994255c4-70f7-43c3-8cf5-05b5bffe0a16","Using soldTo : 994255c4-70f7-43c3-8cf5-05b5bffe0a16","Using billTo: 994255c4-70f7-43c3-8cf5-05b5bffe0a16","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213593 for AS order 20240729155523","version":"1.3.3-qa2.92","biId":"3213593"}}'}}}</t>
+  </si>
+  <si>
+    <t>{
+	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e880a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155523 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f80456028\" title: \"Secrets of nature\" dhId: \"e0c7965c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240729155523Test\" lastName: \"20240729155523Auto\" email: \"20240729155523@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240729155523Test\" lastName: \"20240729155523Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240729155523@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e880a\" } } ] } }\t) { status data\t}}"
+}</t>
+  </si>
+  <si>
+    <t>2024-07-29 15:55:23.441</t>
+  </si>
+  <si>
+    <t>Trigger Invoice Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>20240725122330Test</t>
+  </si>
+  <si>
+    <t>20240725122330Auto</t>
+  </si>
+  <si>
+    <t>20240725122330@Wiley.com</t>
+  </si>
+  <si>
+    <t>3213596</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213596 for AS order 20240729155536</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 01293557-6002-473a-8703-9b00d7c74746","Using billTo: 01293557-6002-473a-8703-9b00d7c74746","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213596 for AS order 20240729155536","version":"1.3.3-qa2.92","biId":"3213596"}}'}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e413a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155536 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-29\" vatIdNumber: \"\" countryCode: \"IS\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f29938860\" title: \"Secrets of nature\" dhId: \"e0c5108c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/ibi.38363\" } soldToDetails: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" email: \"20240725122330@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1080.00, billingAddress: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" streetAddress: [\"Lindarbraut 5\"] addressLocality: \"Laugarvatn\" addressRegion: \"8\" countryCode: \"IS\" postalCode: \"840\" phoneNumber: \"003545254000\" email: \"20240725122330@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e413a\" } } ] } }\t) { status data\t}}"
+}
+</t>
+  </si>
+  <si>
+    <t>2024-07-29 15:55:36.582</t>
   </si>
   <si>
     <t>Trigger CreditCard Order with Existing Customer</t>
@@ -893,21 +923,21 @@
     <t>20240725122331@Wiley.com</t>
   </si>
   <si>
-    <t>3213553</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213553 for AS order 20240725124423</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 33a93dba-b930-4819-99f3-9b0c7cdf3177","Using billTo: 33a93dba-b930-4819-99f3-9b0c7cdf3177","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213553 for AS order 20240725124423","version":"1.3.3-qa2.92","biId":"3213553"}}'}}}</t>
+    <t>3213595</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213595 for AS order 20240729155530</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 33a93dba-b930-4819-99f3-9b0c7cdf3177","Using billTo: 33a93dba-b930-4819-99f3-9b0c7cdf3177","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213595 for AS order 20240729155530","version":"1.3.3-qa2.92","biId":"3213595"}}'}}}</t>
   </si>
   <si>
     <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e323a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124423 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f48910586\" title: \"Secrets of volcano\" dhId: \"e0c4141c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" email: \"20240725122331@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-25T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240725122331@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e323a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e484a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-10-10T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155530 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CC order &lt;&lt;CURRENCY&gt;&gt; form validation\" apc: 1100.00 appliedDiscount: 200.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 180.00 totalChargedAmount: 1080.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"GB564291137\" countryCode: \"GB\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f19860090\" title: \"Secrets of volcano\" dhId: \"e0c7293c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" email: \"20240725122331@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 1080.00 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2024-07-29T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240725122331Test\" lastName: \"20240725122331Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"260 Edison Park\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"+44 1793 528342\" email: \"20240725122331@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e484a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-07-25 12:44:23.004</t>
+    <t>2024-07-29 15:55:30.147</t>
   </si>
   <si>
     <t>Trigger Alipay Order with Existing Customer</t>
@@ -922,21 +952,39 @@
     <t>20240725122333@Wiley.com</t>
   </si>
   <si>
-    <t>3213552</t>
-  </si>
-  <si>
-    <t>Created Viax order 3213552 for AS order 20240725124421</t>
-  </si>
-  <si>
-    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 98a00db8-47be-4f1e-9218-872a83a124aa","Using billTo: 98a00db8-47be-4f1e-9218-872a83a124aa","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213552 for AS order 20240725124421","version":"1.3.3-qa2.92","biId":"3213552"}}'}}}</t>
+    <t>3213594</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213594 for AS order 20240729155528</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 98a00db8-47be-4f1e-9218-872a83a124aa","Using billTo: 98a00db8-47be-4f1e-9218-872a83a124aa","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213594 for AS order 20240729155528","version":"1.3.3-qa2.92","biId":"3213594"}}'}}}</t>
   </si>
   <si>
     <t>{
-	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e586a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240725124421 submittedDate: \"2024-07-25T15:00:14-05\" createdDate: \"2024-07-25T15:00:14-05\" cancelDate: \"2024-07-25T15:00:14-05\" paymentDate: \"2024-07-25T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-25T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62930726\" title: \"Secrets of nature\" dhId: \"e0c2896c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" email: \"20240725122333@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240725122333@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e586a\" } } ] } }\t) { status data\t}}"
+	"query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e460a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155528 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 1000.00 appliedDiscount: 0 discountType: \"Society\" estimatedTax: 0 totalChargedAmount: 1080.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f12061860\" title: \"Secrets of nature\" dhId: \"e0c1102c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" email: \"20240725122333@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 1080.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2039-06-29 08:00:00\" } billingAddress: { firstName: \"20240725122333Test\" lastName: \"20240725122333Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"257 Sanxiang Road\"] addressLocality: \"SHenchou - Futian District\" addressRegion: \"GD\" countryCode: \"CN\" postalCode: \"1234435\" phoneNumber: \"0703503263\" email: \"20240725122333@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e460a\" } } ] } }\t) { status data\t}}"
 }</t>
   </si>
   <si>
-    <t>2024-07-25 12:44:21.072</t>
+    <t>2024-07-29 15:55:28.526</t>
+  </si>
+  <si>
+    <t>Trigger Proforma Order with Existing Customer</t>
+  </si>
+  <si>
+    <t>Created Viax order 3213598 for AS order 20240729155543</t>
+  </si>
+  <si>
+    <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP b8094fa3-e18c-4ab6-a495-0c8ea8a70f8b","Using soldTo : b8094fa3-e18c-4ab6-a495-0c8ea8a70f8b","Using billTo: b8094fa3-e18c-4ab6-a495-0c8ea8a70f8b","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213598 for AS order 20240729155543","version":"1.3.3-qa2.92","biId":"3213598"}}'}}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e879a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240729155543 submittedDate: \"2024-07-29T15:00:14-05\" createdDate: \"2024-07-29T15:00:14-05\" cancelDate: \"2024-07-29T15:00:14-05\" paymentDate: \"2024-07-29T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-07-29T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 0.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-07-29\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f23156004\" title: \"Secrets of nature\" dhId: \"e0c9533c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" email: \"20240725122330@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240725122330Test\" lastName: \"20240725122330Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240725122330@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e879a\" } } ] } }\t) { status data\t}}"
+}
+</t>
+  </si>
+  <si>
+    <t>2024-07-29 15:55:43.110</t>
   </si>
 </sst>
 </file>
@@ -3418,10 +3466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3568,7 +3616,7 @@
         <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>264</v>
@@ -3582,23 +3630,23 @@
       <c r="G4" t="s">
         <v>267</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>3213597</v>
+      </c>
+      <c r="I4" t="s">
         <v>268</v>
-      </c>
-      <c r="I4" t="s">
-        <v>269</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>249</v>
       </c>
       <c r="K4" t="s">
+        <v>269</v>
+      </c>
+      <c r="L4" t="s">
         <v>270</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>271</v>
-      </c>
-      <c r="M4" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -3606,13 +3654,13 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
         <v>273</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>243</v>
       </c>
       <c r="E5" t="s">
         <v>274</v>
@@ -3650,10 +3698,10 @@
         <v>282</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="E6" t="s">
         <v>283</v>
@@ -3691,10 +3739,10 @@
         <v>291</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E7" t="s">
         <v>292</v>
@@ -3722,6 +3770,88 @@
       </c>
       <c r="M7" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" t="s">
+        <v>301</v>
+      </c>
+      <c r="F8" t="s">
+        <v>302</v>
+      </c>
+      <c r="G8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" t="s">
+        <v>304</v>
+      </c>
+      <c r="I8" t="s">
+        <v>305</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K8" t="s">
+        <v>306</v>
+      </c>
+      <c r="L8" t="s">
+        <v>307</v>
+      </c>
+      <c r="M8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" t="s">
+        <v>285</v>
+      </c>
+      <c r="H9">
+        <v>3213598</v>
+      </c>
+      <c r="I9" t="s">
+        <v>310</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K9" t="s">
+        <v>311</v>
+      </c>
+      <c r="L9" t="s">
+        <v>312</v>
+      </c>
+      <c r="M9" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI Validations added V.48
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_Inputs.xlsx
+++ b/TestSuites/UploadExcel/TD_Inputs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HappyFlowData" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,7 +54,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -121,6 +121,12 @@
         <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -144,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -171,6 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1681,8 +1688,8 @@
   </sheetPr>
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView topLeftCell="R13" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1957,15 +1964,15 @@
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Created Viax order 7260078 for PriceProposal 24ef5195-847b-4808-9127-af8e42410548</t>
+          <t>Created Viax order 7266602 for PriceProposal 24ef3995-177b-4808-9127-af8e42410543</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>24ef5195-847b-4808-9127-af8e42410548</t>
-        </is>
-      </c>
-      <c r="AF2" s="17" t="inlineStr">
+          <t>7266602</t>
+        </is>
+      </c>
+      <c r="AF2" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
@@ -1982,14 +1989,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef5195-847b-4808-9127-af8e42410548",
-      "edRefCode": "ACN3-2023-06-5195",
+      "submissionId": "24ef3995-177b-4808-9127-af8e42410543",
+      "edRefCode": "ACN3-2023-06-3995",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-10",
+      "submissionDate": "2024-09-03",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2040,7 +2047,7 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7260078 for PriceProposal 24ef5195-847b-4808-9127-af8e42410548","version":"1.4.4-qa2.51","viaxPriceProposalId":"7260078","priceProposal":{"uid":"66b69c33-3a0c-4097-8502-f44ce94aa14e","biId":"7260078","wAsSubmissionId":"24ef5195-847b-4808-9127-af8e42410548","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-09T22:46:11.373Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef5195-847b-4808-9127-af8e42410548","edRefCode":"ACN3-2023-06-5195","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-10","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-09T22:46:11.900Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5195-847b-4808-9127-af8e42410548","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5195","wAsSubmissionId":"24ef5195-847b-4808-9127-af8e42410548","wAsSubmissionDate":"2024-08-10","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266602 for PriceProposal 24ef3995-177b-4808-9127-af8e42410543","version":"1.4.7-qa2.56","viaxPriceProposalId":"7266602","priceProposal":{"uid":"66d6f5de-ab0c-441f-b4f5-18329ff2fbae","biId":"7266602","wAsSubmissionId":"24ef3995-177b-4808-9127-af8e42410543","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-09-03T11:41:18.911Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef3995-177b-4808-9127-af8e42410543","edRefCode":"ACN3-2023-06-3995","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-09-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-09-03T11:41:24.246Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'JCASP\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"JCASP"},{"errorCode":"500","errorMessage":"Cannot read properties of undefined (reading \'data\')","fieldPath":"","fieldValue":""}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3995-177b-4808-9127-af8e42410543","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3995","wAsSubmissionId":"24ef3995-177b-4808-9127-af8e42410543","wAsSubmissionDate":"2024-09-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2128,20 +2135,20 @@
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Created Viax order 7256064 for PriceProposal 24ef3531-304b-4808-9127-af8e42410422</t>
+          <t>Created Viax order 7266603 for PriceProposal 24ef7976-372b-4808-9127-af8e42410856</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>7256064</t>
-        </is>
-      </c>
-      <c r="AF3" s="15" t="inlineStr">
-        <is>
-          <t>PriceDetermined</t>
-        </is>
-      </c>
-      <c r="AH3" s="15" t="inlineStr">
+          <t>7266603</t>
+        </is>
+      </c>
+      <c r="AF3" s="18" t="inlineStr">
+        <is>
+          <t>DataCorrectionRequired</t>
+        </is>
+      </c>
+      <c r="AH3" s="17" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2153,14 +2160,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef3531-304b-4808-9127-af8e42410422",
-      "edRefCode": "ACN3-2023-06-3531",
+      "submissionId": "24ef7976-372b-4808-9127-af8e42410856",
+      "edRefCode": "ACN3-2023-06-7976",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-09-03",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2211,7 +2218,7 @@
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256064 for PriceProposal 24ef3531-304b-4808-9127-af8e42410422","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256064","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef3531-304b-4808-9127-af8e42410422","version":"1.6.6-qa2.75","submissionId":"24ef3531-304b-4808-9127-af8e42410422","priceProposal":{"uid":"66ac3f4c-0655-4e45-a427-cc11f656672d","biId":"7256064","wAsSubmissionId":"24ef3531-304b-4808-9127-af8e42410422","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:07:08.820Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef3531-304b-4808-9127-af8e42410422","edRefCode":"ACN3-2023-06-3531","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:07:09.452Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3531-304b-4808-9127-af8e42410422","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3531","wAsSubmissionId":"24ef3531-304b-4808-9127-af8e42410422","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266603 for PriceProposal 24ef7976-372b-4808-9127-af8e42410856","version":"1.4.7-qa2.56","viaxPriceProposalId":"7266603","priceProposal":{"uid":"66d6f5f4-af15-422b-b524-8ae23a77b25b","biId":"7266603","wAsSubmissionId":"24ef7976-372b-4808-9127-af8e42410856","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-09-03T11:41:40.694Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7976-372b-4808-9127-af8e42410856","edRefCode":"ACN3-2023-06-7976","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-09-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-09-03T11:41:45.115Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PROMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PROMO50"},{"errorCode":"500","errorMessage":"Cannot read properties of undefined (reading \'data\')","fieldPath":"","fieldValue":""}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7976-372b-4808-9127-af8e42410856","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7976","wAsSubmissionId":"24ef7976-372b-4808-9127-af8e42410856","wAsSubmissionDate":"2024-09-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2301,20 +2308,20 @@
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Created Viax order 7256065 for PriceProposal 24ef5609-371b-4808-9127-af8e42410508</t>
+          <t>Created Viax order 7266604 for PriceProposal 24ef9892-977b-4808-9127-af8e42410833</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>7256065</t>
-        </is>
-      </c>
-      <c r="AF4" s="15" t="inlineStr">
-        <is>
-          <t>PriceDetermined</t>
-        </is>
-      </c>
-      <c r="AH4" s="15" t="inlineStr">
+          <t>7266604</t>
+        </is>
+      </c>
+      <c r="AF4" s="18" t="inlineStr">
+        <is>
+          <t>DataCorrectionRequired</t>
+        </is>
+      </c>
+      <c r="AH4" s="17" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2326,14 +2333,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef5609-371b-4808-9127-af8e42410508",
-      "edRefCode": "ACN3-2023-06-5609",
+      "submissionId": "24ef9892-977b-4808-9127-af8e42410833",
+      "edRefCode": "ACN3-2023-06-9892",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-09-03",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2382,7 +2389,7 @@
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256065 for PriceProposal 24ef5609-371b-4808-9127-af8e42410508","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256065","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5609-371b-4808-9127-af8e42410508","version":"1.6.6-qa2.75","submissionId":"24ef5609-371b-4808-9127-af8e42410508","priceProposal":{"uid":"66ac3fc0-40d1-4ff5-ac8c-3187a8427aaf","biId":"7256065","wAsSubmissionId":"24ef5609-371b-4808-9127-af8e42410508","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:09:04.593Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5609-371b-4808-9127-af8e42410508","edRefCode":"ACN3-2023-06-5609","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:09:05.628Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":800,"price":200,"subtotal":0,"tax":0,"total":0,"discountAmount":200,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":200,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5609-371b-4808-9127-af8e42410508","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5609","wAsSubmissionId":"24ef5609-371b-4808-9127-af8e42410508","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266604 for PriceProposal 24ef9892-977b-4808-9127-af8e42410833","version":"1.4.7-qa2.56","viaxPriceProposalId":"7266604","priceProposal":{"uid":"66d6f60a-d99a-4e3f-8912-b71c8961b90e","biId":"7266604","wAsSubmissionId":"24ef9892-977b-4808-9127-af8e42410833","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-09-03T11:42:02.005Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef9892-977b-4808-9127-af8e42410833","edRefCode":"ACN3-2023-06-9892","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-09-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-09-03T11:42:06.393Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"500","errorMessage":"Cannot read properties of undefined (reading \'data\')","fieldPath":"","fieldValue":""}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9892-977b-4808-9127-af8e42410833","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-9892","wAsSubmissionId":"24ef9892-977b-4808-9127-af8e42410833","wAsSubmissionDate":"2024-09-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2470,20 +2477,20 @@
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>Created Viax order 7256066 for PriceProposal 24ef8753-169b-4808-9127-af8e42410833</t>
+          <t>Created Viax order 7266605 for PriceProposal 24ef5258-336b-4808-9127-af8e42410267</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>7256066</t>
-        </is>
-      </c>
-      <c r="AF5" s="15" t="inlineStr">
-        <is>
-          <t>PriceDetermined</t>
-        </is>
-      </c>
-      <c r="AH5" s="15" t="inlineStr">
+          <t>7266605</t>
+        </is>
+      </c>
+      <c r="AF5" s="18" t="inlineStr">
+        <is>
+          <t>DataCorrectionRequired</t>
+        </is>
+      </c>
+      <c r="AH5" s="17" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2495,14 +2502,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef8753-169b-4808-9127-af8e42410833",
-      "edRefCode": "ACN3-2023-06-8753",
+      "submissionId": "24ef5258-336b-4808-9127-af8e42410267",
+      "edRefCode": "ACN3-2023-06-5258",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "OPINION",
       "displayArticleType": "OPINION",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-09-03",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2552,7 +2559,7 @@
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256066 for PriceProposal 24ef8753-169b-4808-9127-af8e42410833","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256066","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef8753-169b-4808-9127-af8e42410833","version":"1.6.6-qa2.75","submissionId":"24ef8753-169b-4808-9127-af8e42410833","priceProposal":{"uid":"66ac4033-2374-4754-b2b4-bada0bdf8570","biId":"7256066","wAsSubmissionId":"24ef8753-169b-4808-9127-af8e42410833","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:10:59.905Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8753-169b-4808-9127-af8e42410833","edRefCode":"ACN3-2023-06-8753","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:11:00.635Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":64,"tax":0,"total":64,"discountAmount":576,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":576,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef8753-169b-4808-9127-af8e42410833","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8753","wAsSubmissionId":"24ef8753-169b-4808-9127-af8e42410833","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266605 for PriceProposal 24ef5258-336b-4808-9127-af8e42410267","version":"1.4.7-qa2.56","viaxPriceProposalId":"7266605","priceProposal":{"uid":"66d6f61b-3283-44aa-a21f-08c70ae1025b","biId":"7266605","wAsSubmissionId":"24ef5258-336b-4808-9127-af8e42410267","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-09-03T11:42:19.447Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5258-336b-4808-9127-af8e42410267","edRefCode":"ACN3-2023-06-5258","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"OPINION","submissionDate":"2024-09-03","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CCCAM424","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-09-03T11:42:23.826Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P000","errorMessage":"{}","fieldPath":"","fieldValue":""},{"errorCode":"500","errorMessage":"Cannot read properties of undefined (reading \'data\')","fieldPath":"","fieldValue":""}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef5258-336b-4808-9127-af8e42410267","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5258","wAsSubmissionId":"24ef5258-336b-4808-9127-af8e42410267","wAsSubmissionDate":"2024-09-03","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"OPINION","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2640,20 +2647,20 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Created Viax order 7256067 for PriceProposal 24ef6431-765b-4808-9127-af8e42410118</t>
+          <t>Created Viax order 7266465 for PriceProposal 24ef4824-428b-4808-9127-af8e42410318</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>7256067</t>
-        </is>
-      </c>
-      <c r="AF6" s="15" t="inlineStr">
+          <t>7266465</t>
+        </is>
+      </c>
+      <c r="AF6" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH6" s="15" t="inlineStr">
+      <c r="AH6" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2665,14 +2672,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef6431-765b-4808-9127-af8e42410118",
-      "edRefCode": "ACN3-2023-06-6431",
+      "submissionId": "24ef4824-428b-4808-9127-af8e42410318",
+      "edRefCode": "ACN3-2023-06-4824",
       "articleDOI": "",
       "journalId": "e1bbb7b4-5369-4c40-a53a-aa3dc55390a6",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2024-02-10",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2722,7 +2729,7 @@
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256067 for PriceProposal 24ef6431-765b-4808-9127-af8e42410118","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256067","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6431-765b-4808-9127-af8e42410118","version":"1.6.6-qa2.75","submissionId":"24ef6431-765b-4808-9127-af8e42410118","priceProposal":{"uid":"66ac40a9-caee-4ba5-a2c3-a10b6c265687","biId":"7256067","wAsSubmissionId":"24ef6431-765b-4808-9127-af8e42410118","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:12:57.417Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6431-765b-4808-9127-af8e42410118","edRefCode":"ACN3-2023-06-6431","articleDOI":"","journalId":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Hi","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:12:57.960Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":1000,"price":900,"subtotal":762.75,"tax":0,"total":762.75,"discountAmount":137.25,"discountPercentage":15.25,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Hi","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6431-765b-4808-9127-af8e42410118","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6431","wAsSubmissionId":"24ef6431-765b-4808-9127-af8e42410118","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"JCSM","maName":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalUuid":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"21906009x","wAsFlipDate":null,"wAsJournalTitle":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalGroupCode":"JCSM","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"JCSM1@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266465 for PriceProposal 24ef4824-428b-4808-9127-af8e42410318","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266465","priceProposal":{"uid":"66d02726-2045-4472-bf99-8c9c7e72ddf9","biId":"7266465","wAsSubmissionId":"24ef4824-428b-4808-9127-af8e42410318","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:45:42.201Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4824-428b-4808-9127-af8e42410318","edRefCode":"ACN3-2023-06-4824","articleDOI":"","journalId":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2024-02-10","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"Hi","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"anagarajan@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"AixenProvence","countryCode":"IN","country":"IN","institution":"GrantInstitute","department":"SchoolofGeoSciences","stateProvince":"AndhraPradesh","postalCode":"500072","streetAddress":["1832ColvinAve"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:45:42.704Z"}},"wAsCountryCode":"IN","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":1000,"price":900,"subtotal":762.75,"tax":0,"total":762.75,"discountAmount":137.25,"discountPercentage":15.25,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","attribute":"wAsJournalUuid"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":100,"discountPercentage":10,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":137.25,"discountPercentage":15.25,"discountDescription":"","sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"Hi","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"anagarajan@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"GrantInstitute","countryCode":"IN","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4824-428b-4808-9127-af8e42410318","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4824","wAsSubmissionId":"24ef4824-428b-4808-9127-af8e42410318","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2024-02-10","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"JCSM","maName":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalUuid":"e1bbb7b4-5369-4c40-a53a-aa3dc55390a6","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"21906009x","wAsFlipDate":null,"wAsJournalTitle":"Journal of Cachexia, Sarcopenia and Muscle","wAsJournalGroupCode":"JCSM","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"JCSM1@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2810,20 +2817,20 @@
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Created Viax order 7256068 for PriceProposal 24ef4678-427b-4808-9127-af8e42410478</t>
+          <t>Created Viax order 7266466 for PriceProposal 24ef6694-229b-4808-9127-af8e42410362</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>7256068</t>
-        </is>
-      </c>
-      <c r="AF7" s="15" t="inlineStr">
+          <t>7266466</t>
+        </is>
+      </c>
+      <c r="AF7" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH7" s="15" t="inlineStr">
+      <c r="AH7" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2835,14 +2842,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef4678-427b-4808-9127-af8e42410478",
-      "edRefCode": "ACN3-2023-06-4678",
+      "submissionId": "24ef6694-229b-4808-9127-af8e42410362",
+      "edRefCode": "ACN3-2023-06-6694",
       "articleDOI": "",
       "journalId": "b6d18dc5-3811-4b21-81f0-a01997c20001",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -2891,7 +2898,7 @@
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256068 for PriceProposal 24ef4678-427b-4808-9127-af8e42410478","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256068","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4678-427b-4808-9127-af8e42410478","version":"1.6.6-qa2.75","submissionId":"24ef4678-427b-4808-9127-af8e42410478","priceProposal":{"uid":"66ac4117-e784-4aac-b77e-f34fd981e4ab","biId":"7256068","wAsSubmissionId":"24ef4678-427b-4808-9127-af8e42410478","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:14:47.699Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4678-427b-4808-9127-af8e42410478","edRefCode":"ACN3-2023-06-4678","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:14:48.943Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":210,"subtotal":0,"tax":0,"total":0,"discountAmount":210,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4678-427b-4808-9127-af8e42410478","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4678","wAsSubmissionId":"24ef4678-427b-4808-9127-af8e42410478","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266466 for PriceProposal 24ef6694-229b-4808-9127-af8e42410362","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266466","priceProposal":{"uid":"66d02796-f2ec-4b57-9e2d-26a3697f169b","biId":"7266466","wAsSubmissionId":"24ef6694-229b-4808-9127-af8e42410362","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:47:34.185Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6694-229b-4808-9127-af8e42410362","edRefCode":"ACN3-2023-06-6694","articleDOI":"","journalId":"b6d18dc5-3811-4b21-81f0-a01997c20001","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"MH","country":"MH","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:47:34.845Z"}},"wAsCountryCode":"MH","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":300,"price":210,"subtotal":0,"tax":0,"total":0,"discountAmount":210,"discountPercentage":100,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"b6d18dc5-3811-4b21-81f0-a01997c20001","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"MH","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":210,"discountPercentage":100,"discountDescription":"","sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":90,"discountPercentage":30,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"MH","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6694-229b-4808-9127-af8e42410362","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6694","wAsSubmissionId":"24ef6694-229b-4808-9127-af8e42410362","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article","ibrProduct":{"maId":"CCR3","maName":"Clinical Case Reports","wAsJournalUuid":"b6d18dc5-3811-4b21-81f0-a01997c20001","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20500904","wAsFlipDate":null,"wAsJournalTitle":"Clinical Case Reports","wAsJournalGroupCode":"CCR3","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"clinicalcases@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -2981,20 +2988,20 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>Created Viax order 7256069 for PriceProposal 24ef5134-691b-4808-9127-af8e42410536</t>
+          <t>Created Viax order 7266467 for PriceProposal 24ef8184-907b-4808-9127-af8e42410253</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>7256069</t>
-        </is>
-      </c>
-      <c r="AF8" s="15" t="inlineStr">
+          <t>7266467</t>
+        </is>
+      </c>
+      <c r="AF8" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH8" s="15" t="inlineStr">
+      <c r="AH8" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3006,14 +3013,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef5134-691b-4808-9127-af8e42410536",
-      "edRefCode": "ACN3-2023-06-5134",
+      "submissionId": "24ef8184-907b-4808-9127-af8e42410253",
+      "edRefCode": "ACN3-2023-06-8184",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "RESEARCH ARTICLE",
       "displayArticleType": "RESEARCH ARTICLE",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -3062,7 +3069,7 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256069 for PriceProposal 24ef5134-691b-4808-9127-af8e42410536","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256069","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5134-691b-4808-9127-af8e42410536","version":"1.6.6-qa2.75","submissionId":"24ef5134-691b-4808-9127-af8e42410536","priceProposal":{"uid":"66ac418c-22ca-4269-97a2-d9b302041348","biId":"7256069","wAsSubmissionId":"24ef5134-691b-4808-9127-af8e42410536","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:16:44.642Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5134-691b-4808-9127-af8e42410536","edRefCode":"ACN3-2023-06-5134","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:16:45.302Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5134-691b-4808-9127-af8e42410536","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5134","wAsSubmissionId":"24ef5134-691b-4808-9127-af8e42410536","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266467 for PriceProposal 24ef8184-907b-4808-9127-af8e42410253","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266467","priceProposal":{"uid":"66d0280e-81b1-44a5-9472-077d0de709ad","biId":"7266467","wAsSubmissionId":"24ef8184-907b-4808-9127-af8e42410253","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:49:34.473Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8184-907b-4808-9127-af8e42410253","edRefCode":"ACN3-2023-06-8184","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:49:35.686Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":500,"tax":0,"total":500,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8184-907b-4808-9127-af8e42410253","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8184","wAsSubmissionId":"24ef8184-907b-4808-9127-af8e42410253","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -3164,20 +3171,20 @@
       <c r="AC9" s="7" t="n"/>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>Created Viax order 7256070 for PriceProposal 24ef3341-758b-4808-9127-af8e42410499</t>
+          <t>Created Viax order 7266468 for PriceProposal 24ef4223-662b-4808-9127-af8e42410809</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>7256070</t>
-        </is>
-      </c>
-      <c r="AF9" s="15" t="inlineStr">
+          <t>7266468</t>
+        </is>
+      </c>
+      <c r="AF9" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH9" s="15" t="inlineStr">
+      <c r="AH9" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3189,14 +3196,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef3341-758b-4808-9127-af8e42410499",
-      "edRefCode": "ACN3-2023-06-3341",
+      "submissionId": "24ef4223-662b-4808-9127-af8e42410809",
+      "edRefCode": "ACN3-2023-06-4223",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -3245,7 +3252,7 @@
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256070 for PriceProposal 24ef3341-758b-4808-9127-af8e42410499","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256070","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef3341-758b-4808-9127-af8e42410499","version":"1.6.6-qa2.75","submissionId":"24ef3341-758b-4808-9127-af8e42410499","priceProposal":{"uid":"66ac41dc-69e1-410c-99aa-607728c1558d","biId":"7256070","wAsSubmissionId":"24ef3341-758b-4808-9127-af8e42410499","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:18:04.508Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef3341-758b-4808-9127-af8e42410499","edRefCode":"ACN3-2023-06-3341","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:18:05.323Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":2471,"price":617.75,"subtotal":0,"tax":0,"total":0,"discountAmount":617.75,"discountPercentage":100,"currencyCode":"GBP","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":617.75,"discountPercentage":33.535511938486444,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1853.25,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":617.75,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3341-758b-4808-9127-af8e42410499","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3341","wAsSubmissionId":"24ef3341-758b-4808-9127-af8e42410499","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266468 for PriceProposal 24ef4223-662b-4808-9127-af8e42410809","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266468","priceProposal":{"uid":"66d02861-da83-44b7-8326-3543854f87fe","biId":"7266468","wAsSubmissionId":"24ef4223-662b-4808-9127-af8e42410809","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:50:57.354Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef4223-662b-4808-9127-af8e42410809","edRefCode":"ACN3-2023-06-4223","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"GB","country":"UK","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:50:58.222Z"}},"wAsCountryCode":"GB","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":{"institutionId":"1666","institutionName":"E O Lawrence Berkeley National Laboratory","institutionIdType":"Ringgold","woaCode":null,"consortiumCode":"CDL"},"prices":[{"basePrice":1472,"price":368,"subtotal":0,"tax":0,"total":0,"discountAmount":368,"discountPercentage":100,"currencyCode":"GBP","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1104,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":368,"discountPercentage":53.75,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"E O Lawrence Berkeley National Laboratory","discountType":"Institutional","discountAmount":368,"discountPercentage":100,"discountDescription":"Institutional Discounts Group","sapDiscountTableCode":"ZIV1","isPercentageDiscount":false,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":1104,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"1666","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"GB","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4223-662b-4808-9127-af8e42410809","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4223","wAsSubmissionId":"24ef4223-662b-4808-9127-af8e42410809","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -3337,20 +3344,20 @@
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>Created Viax order 7256071 for PriceProposal 24ef9346-203b-4808-9127-af8e42410605</t>
+          <t>Created Viax order 7266469 for PriceProposal 24ef8763-683b-4808-9127-af8e42410236</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>7256071</t>
-        </is>
-      </c>
-      <c r="AF10" s="15" t="inlineStr">
+          <t>7266469</t>
+        </is>
+      </c>
+      <c r="AF10" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH10" s="15" t="inlineStr">
+      <c r="AH10" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3362,14 +3369,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef9346-203b-4808-9127-af8e42410605",
-      "edRefCode": "ACN3-2023-06-9346",
+      "submissionId": "24ef8763-683b-4808-9127-af8e42410236",
+      "edRefCode": "ACN3-2023-06-8763",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -3422,7 +3429,7 @@
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256071 for PriceProposal 24ef9346-203b-4808-9127-af8e42410605","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256071","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef9346-203b-4808-9127-af8e42410605","version":"1.6.6-qa2.75","submissionId":"24ef9346-203b-4808-9127-af8e42410605","priceProposal":{"uid":"66ac4251-5dab-4f92-a264-7d164d3c3f78","biId":"7256071","wAsSubmissionId":"24ef9346-203b-4808-9127-af8e42410605","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:20:01.494Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9346-203b-4808-9127-af8e42410605","edRefCode":"ACN3-2023-06-9346","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:20:02.035Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":160,"tax":0,"total":160,"discountAmount":40,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9346-203b-4808-9127-af8e42410605","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-9346","wAsSubmissionId":"24ef9346-203b-4808-9127-af8e42410605","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266469 for PriceProposal 24ef8763-683b-4808-9127-af8e42410236","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266469","priceProposal":{"uid":"66d028d8-ea51-458a-a0d6-90cbd38201cd","biId":"7266469","wAsSubmissionId":"24ef8763-683b-4808-9127-af8e42410236","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:52:56.948Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8763-683b-4808-9127-af8e42410236","edRefCode":"ACN3-2023-06-8763","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":100,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:52:57.572Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":400,"tax":0,"total":400,"discountAmount":100,"discountPercentage":20,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":100,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":100,"discountPercentage":20,"discountDescription":"UPDATED VALID TO DATE","sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8763-683b-4808-9127-af8e42410236","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8763","wAsSubmissionId":"24ef8763-683b-4808-9127-af8e42410236","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -3519,20 +3526,20 @@
       <c r="AC11" s="11" t="n"/>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>Created Viax order 7256072 for PriceProposal 24ef5278-339b-4808-9127-af8e42410612</t>
+          <t>Created Viax order 7266470 for PriceProposal 24ef6899-237b-4808-9127-af8e42410785</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>7256072</t>
-        </is>
-      </c>
-      <c r="AF11" s="15" t="inlineStr">
+          <t>7266470</t>
+        </is>
+      </c>
+      <c r="AF11" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH11" s="15" t="inlineStr">
+      <c r="AH11" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3544,14 +3551,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef5278-339b-4808-9127-af8e42410612",
-      "edRefCode": "ACN3-2023-06-5278",
+      "submissionId": "24ef6899-237b-4808-9127-af8e42410785",
+      "edRefCode": "ACN3-2023-06-6899",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "EDUCATION",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -3602,7 +3609,7 @@
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256072 for PriceProposal 24ef5278-339b-4808-9127-af8e42410612","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256072","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5278-339b-4808-9127-af8e42410612","version":"1.6.6-qa2.75","submissionId":"24ef5278-339b-4808-9127-af8e42410612","priceProposal":{"uid":"66ac42de-bb66-48b9-9016-2fde7c04d7d6","biId":"7256072","wAsSubmissionId":"24ef5278-339b-4808-9127-af8e42410612","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:22:22.172Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef5278-339b-4808-9127-af8e42410612","edRefCode":"ACN3-2023-06-5278","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM9"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"BO","country":"BO","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:22:22.725Z"}},"wAsCountryCode":"BO","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":400,"tax":0,"total":400,"discountAmount":400,"discountPercentage":50,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM9","discountType":"Society","discountAmount":400,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"BO","attribute":"wAsCountryCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":400,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"BO","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5278-339b-4808-9127-af8e42410612","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5278","wAsSubmissionId":"24ef5278-339b-4808-9127-af8e42410612","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266470 for PriceProposal 24ef6899-237b-4808-9127-af8e42410785","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266470","priceProposal":{"uid":"66d02969-3ef2-4c4f-b3f2-60579c419c66","biId":"7266470","wAsSubmissionId":"24ef6899-237b-4808-9127-af8e42410785","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:55:21.741Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef6899-237b-4808-9127-af8e42410785","edRefCode":"ACN3-2023-06-6899","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM9"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"BO","country":"BO","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"EANM9","discountType":"Society","discountAmount":1000,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:55:22.288Z"}},"wAsCountryCode":"BO","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":2000,"subtotal":1000,"tax":0,"total":1000,"discountAmount":1000,"discountPercentage":50,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":1000,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"BO","attribute":"wAsCountryCode"}]},{"discountCode":"EANM9","discountType":"Society","discountAmount":1000,"discountPercentage":50,"discountDescription":"SOCIETY","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"EANM9","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":1000,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"BO","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6899-237b-4808-9127-af8e42410785","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6899","wAsSubmissionId":"24ef6899-237b-4808-9127-af8e42410785","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -3737,20 +3744,20 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>Created Viax order 7256081 for PriceProposal 24ef6602-438b-4808-9127-af8e42410743</t>
+          <t>Created Viax order 7266471 for PriceProposal 24ef8422-154b-4808-9127-af8e42410556</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>7256081</t>
-        </is>
-      </c>
-      <c r="AF12" s="15" t="inlineStr">
+          <t>7266471</t>
+        </is>
+      </c>
+      <c r="AF12" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH12" s="15" t="inlineStr">
+      <c r="AH12" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3762,14 +3769,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef6602-438b-4808-9127-af8e42410743",
-      "edRefCode": "ACN3-2023-06-6602",
+      "submissionId": "24ef8422-154b-4808-9127-af8e42410556",
+      "edRefCode": "ACN3-2023-06-8422",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "RESEARCH ARTICLE",
       "displayArticleType": "RESEARCH ARTICLE",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -3824,7 +3831,7 @@
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256081 for PriceProposal 24ef6602-438b-4808-9127-af8e42410743","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256081","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6602-438b-4808-9127-af8e42410743","version":"1.6.6-qa2.75","submissionId":"24ef6602-438b-4808-9127-af8e42410743","priceProposal":{"uid":"66ac4897-22b2-4cb6-89a8-7074970f6b57","biId":"7256081","wAsSubmissionId":"24ef6602-438b-4808-9127-af8e42410743","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:46:47.195Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef6602-438b-4808-9127-af8e42410743","edRefCode":"ACN3-2023-06-6602","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:46:48.589Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":20,"tax":0,"total":20,"discountAmount":180,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":100,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":40,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":180,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef6602-438b-4808-9127-af8e42410743","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6602","wAsSubmissionId":"24ef6602-438b-4808-9127-af8e42410743","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266471 for PriceProposal 24ef8422-154b-4808-9127-af8e42410556","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266471","priceProposal":{"uid":"66d029e9-eb15-475f-b7ee-1da631f2ce33","biId":"7266471","wAsSubmissionId":"24ef8422-154b-4808-9127-af8e42410556","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T07:57:29.520Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8422-154b-4808-9127-af8e42410556","edRefCode":"ACN3-2023-06-8422","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"RESEARCH ARTICLE","displayArticleType":"RESEARCH ARTICLE","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":["PROMO50"],"discountCodes":[],"editorialDiscountCode":"CCCAM424","referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"PE","country":"PE","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":100,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T07:57:30.079Z"}},"wAsCountryCode":"PE","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsReferringJournalRef":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalStatus":"Yes","wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalEISSN":"20457634","wAsEditorialOfficeEmail":"cancermed@wiley.com"},"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":50,"tax":0,"total":50,"discountAmount":450,"discountPercentage":90,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"GeographicalDiscount","discountAmount":250,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZGPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PE","attribute":"wAsCountryCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"","discountType":"ReferralDiscount","discountAmount":250,"discountPercentage":50,"discountDescription":null,"sapDiscountTableCode":"ZRPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsReferringJournal"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":null,"sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":450,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"CCCAM424","attribute":"wAsEditorialDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"PROMO50","discountType":"WileyPromoCode","discountAmount":100,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZPP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"PROMO50","attribute":"wAsSelectedPromotionPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"CCCAM424","discountType":"EditorialDiscount","discountAmount":450,"discountPercentage":90,"discountDescription":"","sapDiscountTableCode":"ZEPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"PE","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CCCAM424","biiSalable":{"maId":"24ef8422-154b-4808-9127-af8e42410556","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8422","wAsSubmissionId":"24ef8422-154b-4808-9127-af8e42410556","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"RESEARCH ARTICLE","wAsDisplayArticleType":"RESEARCH ARTICLE","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -3925,20 +3932,20 @@
       <c r="AC13" s="11" t="n"/>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>Created Viax order 7256082 for PriceProposal 24ef5088-168b-4808-9127-af8e42410890</t>
+          <t>Created Viax order 7266507 for PriceProposal 24ef8459-626b-4808-9127-af8e42410984</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>7256082</t>
-        </is>
-      </c>
-      <c r="AF13" s="15" t="inlineStr">
+          <t>7266507</t>
+        </is>
+      </c>
+      <c r="AF13" s="17" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH13" s="15" t="inlineStr">
+      <c r="AH13" s="17" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -3950,14 +3957,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d02-8c68-fe0b8c46172a",
-      "submissionId": "24ef5088-168b-4808-9127-af8e42410890",
-      "edRefCode": "ACN3-2023-06-5088",
+      "submissionId": "24ef8459-626b-4808-9127-af8e42410984",
+      "edRefCode": "ACN3-2023-06-8459",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4008,7 +4015,7 @@
       </c>
       <c r="AJ13" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256082 for PriceProposal 24ef5088-168b-4808-9127-af8e42410890","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256082","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5088-168b-4808-9127-af8e42410890","version":"1.6.6-qa2.75","submissionId":"24ef5088-168b-4808-9127-af8e42410890","priceProposal":{"uid":"66ac4967-edaa-4f83-940e-380229b4cc07","biId":"7256082","wAsSubmissionId":"24ef5088-168b-4808-9127-af8e42410890","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:50:15.638Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef5088-168b-4808-9127-af8e42410890","edRefCode":"ACN3-2023-06-5088","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:50:16.393Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5088-168b-4808-9127-af8e42410890","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5088","wAsSubmissionId":"24ef5088-168b-4808-9127-af8e42410890","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266507 for PriceProposal 24ef8459-626b-4808-9127-af8e42410984","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266507","priceProposal":{"uid":"66d0403c-3cff-4986-b59a-8f5ddb6519ef","biId":"7266507","wAsSubmissionId":"24ef8459-626b-4808-9127-af8e42410984","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T09:32:43.978Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d02-8c68-fe0b8c46172a","submissionId":"24ef8459-626b-4808-9127-af8e42410984","edRefCode":"ACN3-2023-06-8459","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"PhD","orcId":"0000-0003-4043-3196","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"addressLocality":"Stavnger","countryCode":"US","country":"France","institution":"Ardrossan Area School","department":"School of GeoSciences","stateProvince":"Rogaland Fylke","postalCode":"4036","streetAddress":["Po Box 2554"]}]}],"funders":[]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T09:32:45.364Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":500,"tax":0,"total":500,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":"0000-0003-4043-3196","firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"PhD","affiliations":[{"affiliationIds":[{"institutionId":"131661","institutionIdType":"Ringgold"}],"affiliationName":"Ardrossan Area School","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8459-626b-4808-9127-af8e42410984","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8459","wAsSubmissionId":"24ef8459-626b-4808-9127-af8e42410984","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4112,20 +4119,20 @@
       <c r="AC14" s="11" t="n"/>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>Created Viax order 7256083 for PriceProposal 24ef5554-787b-4808-9127-af8e42410953</t>
+          <t>Created Viax order 7266473 for PriceProposal 24ef7069-360b-4808-9127-af8e42410537</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>7256083</t>
-        </is>
-      </c>
-      <c r="AF14" s="15" t="inlineStr">
+          <t>7266473</t>
+        </is>
+      </c>
+      <c r="AF14" s="16" t="inlineStr">
         <is>
           <t>PriceDetermined</t>
         </is>
       </c>
-      <c r="AH14" s="15" t="inlineStr">
+      <c r="AH14" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4137,14 +4144,14 @@
   "variables": {
     "data": {
       "requestId": "4a48d9c8-6b6d-4583-b9ac-1836890cb988",
-      "submissionId": "24ef5554-787b-4808-9127-af8e42410953",
-      "edRefCode": "CAM4-2024-04-5554",
+      "submissionId": "24ef7069-360b-4808-9127-af8e42410537",
+      "edRefCode": "CAM4-2024-04-7069",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Data Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4207,7 +4214,7 @@
       </c>
       <c r="AJ14" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256083 for PriceProposal 24ef5554-787b-4808-9127-af8e42410953","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256083","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5554-787b-4808-9127-af8e42410953","version":"1.6.6-qa2.75","submissionId":"24ef5554-787b-4808-9127-af8e42410953","priceProposal":{"uid":"66ac499f-a4d0-4065-8cae-14fadece6c21","biId":"7256083","wAsSubmissionId":"24ef5554-787b-4808-9127-af8e42410953","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T02:51:11.552Z","wAsPaymentType":"FunderPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef5554-787b-4808-9127-af8e42410953","edRefCode":"CAM4-2024-04-5554","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:51:12.598Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":true,"woadInstitution":{"institutionId":"2221","institutionName":"Commonwealth Scientific and Industrial Research Organisation","institutionIdType":"Ringgold","woaCode":"CSIR","consortiumCode":""},"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5554-787b-4808-9127-af8e42410953","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-5554","wAsSubmissionId":"24ef5554-787b-4808-9127-af8e42410953","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266473 for PriceProposal 24ef7069-360b-4808-9127-af8e42410537","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266473","priceProposal":{"uid":"66d02af7-bfdf-4c64-b610-e2d1ba46b357","biId":"7266473","wAsSubmissionId":"24ef7069-360b-4808-9127-af8e42410537","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T08:01:59.095Z","wAsPaymentType":"FunderPaid","wAsPriceProposalPayload":{"requestId":"4a48d9c8-6b6d-4583-b9ac-1836890cb988","submissionId":"24ef7069-360b-4808-9127-af8e42410537","edRefCode":"CAM4-2024-04-7069","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Data Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"wAsManualDiscountAmount":0,"authors":[{"role":"CorrespondingAuthor","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","email":"TestAuto@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"orcId":"0000-0003-0888-1984","addressLocality":"Stavnger","countryCode":"US","country":"USA","institution":"Universidad Nacional De Ingenieria","department":"SchoolofGeoSciences","stateProvince":"RogalandFylke","postalCode":"4036","streetAddress":["PoBox2554"]}]}],"funders":[{"name":"ARC of the Piedmont (The Arc)","funderId":"10.13039/100006467","grants":[{"grantNumber":"124566AA","grantRecipient":["PhilipJ.Cameron-Smith"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:02:00.287Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":true,"woadInstitution":{"institutionId":"2221","institutionName":"Commonwealth Scientific and Industrial Research Organisation","institutionIdType":"Ringgold","woaCode":"CSIR","consortiumCode":""},"prices":[{"basePrice":2000,"price":2000,"subtotal":2000,"tax":0,"total":2000,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAuto@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":null,"honorificSuffix":null,"affiliations":[{"affiliationIds":[{"institutionId":"2221","institutionIdType":"Ringgold"}],"affiliationName":"Universidad Nacional De Ingenieria","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[{"funderId":"10.13039/100006467","name":"ARC of the Piedmont (The Arc)","researchGrants":[{"grantNumber":"124566AA","grantRecipients":["PhilipJ.Cameron-Smith"]}]}],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7069-360b-4808-9127-af8e42410537","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"CAM4-2024-04-7069","wAsSubmissionId":"24ef7069-360b-4808-9127-af8e42410537","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Data Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4299,20 +4306,20 @@
       <c r="AC15" s="11" t="n"/>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>Created Viax order 7256085 for PriceProposal 24ef8559-588b-4808-9127-af8e42410290</t>
+          <t>Created Viax order 7266475 for PriceProposal 24ef8460-826b-4808-9127-af8e42410920</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>7256085</t>
-        </is>
-      </c>
-      <c r="AF15" s="15" t="inlineStr">
+          <t>7266475</t>
+        </is>
+      </c>
+      <c r="AF15" s="16" t="inlineStr">
         <is>
           <t>ManualOverrideRequired</t>
         </is>
       </c>
-      <c r="AH15" s="15" t="inlineStr">
+      <c r="AH15" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4324,14 +4331,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef8559-588b-4808-9127-af8e42410290",
-      "edRefCode": "ACN3-2023-06-8559",
+      "submissionId": "24ef8460-826b-4808-9127-af8e42410920",
+      "edRefCode": "ACN3-2023-06-8460",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4382,7 +4389,7 @@
       </c>
       <c r="AJ15" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256085 for PriceProposal 24ef8559-588b-4808-9127-af8e42410290","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256085","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef8559-588b-4808-9127-af8e42410290","version":"1.6.6-qa2.75","submissionId":"24ef8559-588b-4808-9127-af8e42410290","priceProposal":{"uid":"66ac4a4c-0e3f-4d90-9349-e892ad2945df","biId":"7256085","wAsSubmissionId":"24ef8559-588b-4808-9127-af8e42410290","bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-08-02T02:54:04.137Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8559-588b-4808-9127-af8e42410290","edRefCode":"ACN3-2023-06-8559","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:54:04.706Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8559-588b-4808-9127-af8e42410290","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8559","wAsSubmissionId":"24ef8559-588b-4808-9127-af8e42410290","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266475 for PriceProposal 24ef8460-826b-4808-9127-af8e42410920","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266475","priceProposal":{"uid":"66d02baa-51bf-49f0-9694-f9ee5f6d9092","biId":"7266475","wAsSubmissionId":"24ef8460-826b-4808-9127-af8e42410920","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"ManualOverrideRequired"},"biCreatedAt":"2024-08-29T08:04:58.434Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8460-826b-4808-9127-af8e42410920","edRefCode":"ACN3-2023-06-8460","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":true,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:04:59.035Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":475,"tax":0,"total":475,"discountAmount":25,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":true,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8460-826b-4808-9127-af8e42410920","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8460","wAsSubmissionId":"24ef8460-826b-4808-9127-af8e42410920","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4481,20 +4488,20 @@
       <c r="AC16" s="11" t="n"/>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>Created Viax order 7256084 for PriceProposal 24ef7677-712b-4808-9127-af8e42410611</t>
+          <t>Created Viax order 7266474 for PriceProposal 24ef2431-427b-4808-9127-af8e42410638</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>7256084</t>
-        </is>
-      </c>
-      <c r="AF16" s="15" t="inlineStr">
+          <t>7266474</t>
+        </is>
+      </c>
+      <c r="AF16" s="16" t="inlineStr">
         <is>
           <t>DataCorrectionRequired</t>
         </is>
       </c>
-      <c r="AH16" s="15" t="inlineStr">
+      <c r="AH16" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4506,14 +4513,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef7677-712b-4808-9127-af8e42410611",
-      "edRefCode": "ACN3-2023-06-7677",
+      "submissionId": "24ef2431-427b-4808-9127-af8e42410638",
+      "edRefCode": "ACN3-2023-06-2431",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4564,7 +4571,7 @@
       </c>
       <c r="AJ16" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256084 for PriceProposal 24ef7677-712b-4808-9127-af8e42410611","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256084","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef7677-712b-4808-9127-af8e42410611","version":"1.6.6-qa2.75","submissionId":"24ef7677-712b-4808-9127-af8e42410611","priceProposal":{"uid":"66ac49d8-dcd7-4328-9e15-794550032924","biId":"7256084","wAsSubmissionId":"24ef7677-712b-4808-9127-af8e42410611","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:52:07.986Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef7677-712b-4808-9127-af8e42410611","edRefCode":"ACN3-2023-06-7677","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:52:08.571Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7677-712b-4808-9127-af8e42410611","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7677","wAsSubmissionId":"24ef7677-712b-4808-9127-af8e42410611","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266474 for PriceProposal 24ef2431-427b-4808-9127-af8e42410638","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266474","priceProposal":{"uid":"66d02b31-5496-400c-9c4a-8a7c70894c88","biId":"7266474","wAsSubmissionId":"24ef2431-427b-4808-9127-af8e42410638","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-29T08:02:57.604Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2431-427b-4808-9127-af8e42410638","edRefCode":"ACN3-2023-06-2431","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":["PRKMO50"],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:02:58.094Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'PRKMO50\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"PRKMO50"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":500,"tax":0,"total":500,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]},{"discountCode":"PRKMO50","discountType":"WileyPromoCode","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2431-427b-4808-9127-af8e42410638","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-2431","wAsSubmissionId":"24ef2431-427b-4808-9127-af8e42410638","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4661,20 +4668,20 @@
       <c r="AC17" s="11" t="n"/>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>Created Viax order 7256086 for PriceProposal 24ef6216-261b-4808-9127-af8e42410557</t>
+          <t>Created Viax order 7266476 for PriceProposal 24ef4203-871b-4808-9127-af8e42410273</t>
         </is>
       </c>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>7256086</t>
-        </is>
-      </c>
-      <c r="AF17" s="15" t="inlineStr">
+          <t>7266476</t>
+        </is>
+      </c>
+      <c r="AF17" s="16" t="inlineStr">
         <is>
           <t>DataCorrectionRequired</t>
         </is>
       </c>
-      <c r="AH17" s="15" t="inlineStr">
+      <c r="AH17" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4686,14 +4693,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef6216-261b-4808-9127-af8e42410557",
-      "edRefCode": "ACN3-2023-06-6216",
+      "submissionId": "24ef4203-871b-4808-9127-af8e42410273",
+      "edRefCode": "ACN3-2023-06-4203",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4744,7 +4751,7 @@
       </c>
       <c r="AJ17" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256086 for PriceProposal 24ef6216-261b-4808-9127-af8e42410557","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256086","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6216-261b-4808-9127-af8e42410557","version":"1.6.6-qa2.75","submissionId":"24ef6216-261b-4808-9127-af8e42410557","priceProposal":{"uid":"66ac4aae-0b1d-4144-b5f0-a802f3222584","biId":"7256086","wAsSubmissionId":"24ef6216-261b-4808-9127-af8e42410557","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:55:42.292Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6216-261b-4808-9127-af8e42410557","edRefCode":"ACN3-2023-06-6216","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:55:42.852Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6216-261b-4808-9127-af8e42410557","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6216","wAsSubmissionId":"24ef6216-261b-4808-9127-af8e42410557","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266476 for PriceProposal 24ef4203-871b-4808-9127-af8e42410273","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266476","priceProposal":{"uid":"66d02bfd-102d-45e6-a84c-1f0e98794ce8","biId":"7266476","wAsSubmissionId":"24ef4203-871b-4808-9127-af8e42410273","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-29T08:06:21.357Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef4203-871b-4808-9127-af8e42410273","edRefCode":"ACN3-2023-06-4203","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:06:21.890Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":500,"tax":0,"total":500,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4203-871b-4808-9127-af8e42410273","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4203","wAsSubmissionId":"24ef4203-871b-4808-9127-af8e42410273","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4771,20 +4778,20 @@
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>Created Viax order 7256087 for PriceProposal 24ef4466-307b-4808-9127-af8e42410713</t>
+          <t>Created Viax order 7266477 for PriceProposal 24ef4089-344b-4808-9127-af8e42410404</t>
         </is>
       </c>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>7256087</t>
-        </is>
-      </c>
-      <c r="AF18" s="15" t="inlineStr">
+          <t>7266477</t>
+        </is>
+      </c>
+      <c r="AF18" s="16" t="inlineStr">
         <is>
           <t>DataCorrectionRequired</t>
         </is>
       </c>
-      <c r="AH18" s="15" t="inlineStr">
+      <c r="AH18" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4796,14 +4803,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef4466-307b-4808-9127-af8e42410713",
-      "edRefCode": "ACN3-2023-06-4466",
+      "submissionId": "24ef4089-344b-4808-9127-af8e42410404",
+      "edRefCode": "ACN3-2023-06-4089",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "EDUCATIO",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4852,7 +4859,7 @@
       </c>
       <c r="AJ18" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256087 for PriceProposal 24ef4466-307b-4808-9127-af8e42410713","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256087","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4466-307b-4808-9127-af8e42410713","version":"1.6.6-qa2.75","submissionId":"24ef4466-307b-4808-9127-af8e42410713","priceProposal":{"uid":"66ac4af5-0a0b-476f-967d-876367f5cbe5","biId":"7256087","wAsSubmissionId":"24ef4466-307b-4808-9127-af8e42410713","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:56:52.995Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4466-307b-4808-9127-af8e42410713","edRefCode":"ACN3-2023-06-4466","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATIO","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:56:54.429Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P005","errorMessage":"Base Article Type not defined.","fieldPath":"priceProposal.hiConsistsOf[0].biiSalable.wAsBaseArticleType","fieldValue":"EDUCATIO"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4466-307b-4808-9127-af8e42410713","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4466","wAsSubmissionId":"24ef4466-307b-4808-9127-af8e42410713","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATIO","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266477 for PriceProposal 24ef4089-344b-4808-9127-af8e42410404","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266477","priceProposal":{"uid":"66d02c37-4d62-4885-be1f-2a2fdd145722","biId":"7266477","wAsSubmissionId":"24ef4089-344b-4808-9127-af8e42410404","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-29T08:07:19.333Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4089-344b-4808-9127-af8e42410404","edRefCode":"ACN3-2023-06-4089","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATIO","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:07:19.878Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P005","errorMessage":"Base Article Type not defined.","fieldPath":"priceProposal.hiConsistsOf[0].biiSalable.wAsBaseArticleType","fieldValue":"EDUCATIO"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":2000,"subtotal":2000,"tax":0,"total":2000,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4089-344b-4808-9127-af8e42410404","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4089","wAsSubmissionId":"24ef4089-344b-4808-9127-af8e42410404","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATIO","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4879,20 +4886,20 @@
       </c>
       <c r="AD19" t="inlineStr">
         <is>
-          <t>Created Viax order 7256088 for PriceProposal 24ef6320-470b-4808-9127-af8e42410858</t>
+          <t>Created Viax order 7266478 for PriceProposal 24ef1650-510b-4808-9127-af8e42410857</t>
         </is>
       </c>
       <c r="AE19" t="inlineStr">
         <is>
-          <t>7256088</t>
-        </is>
-      </c>
-      <c r="AF19" s="15" t="inlineStr">
+          <t>7266478</t>
+        </is>
+      </c>
+      <c r="AF19" s="16" t="inlineStr">
         <is>
           <t>DataCorrectionRequired</t>
         </is>
       </c>
-      <c r="AH19" s="15" t="inlineStr">
+      <c r="AH19" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -4904,14 +4911,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef6320-470b-4808-9127-af8e42410858",
-      "edRefCode": "ACN3-2023-06-6320",
+      "submissionId": "24ef1650-510b-4808-9127-af8e42410857",
+      "edRefCode": "ACN3-2023-06-1650",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "EDUCATION",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -4961,7 +4968,7 @@
       </c>
       <c r="AJ19" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256088 for PriceProposal 24ef6320-470b-4808-9127-af8e42410858","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256088","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6320-470b-4808-9127-af8e42410858","version":"1.6.6-qa2.75","submissionId":"24ef6320-470b-4808-9127-af8e42410858","priceProposal":{"uid":"66ac4b2f-8684-4409-9b28-52c6e74c297f","biId":"7256088","wAsSubmissionId":"24ef6320-470b-4808-9127-af8e42410858","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T02:57:51.040Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef6320-470b-4808-9127-af8e42410858","edRefCode":"ACN3-2023-06-6320","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CWECE3","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:57:51.652Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P007","errorMessage":"Editorial code \'CWECE3\' does not exist for the journal","fieldPath":"hiConsistsOf[0].wAsEditorialDiscountCode","fieldValue":"CWECE3"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":800,"subtotal":800,"tax":0,"total":800,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"CWECE3","discountType":"EditorialDiscount","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CWECE3","biiSalable":{"maId":"24ef6320-470b-4808-9127-af8e42410858","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6320","wAsSubmissionId":"24ef6320-470b-4808-9127-af8e42410858","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266478 for PriceProposal 24ef1650-510b-4808-9127-af8e42410857","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266478","priceProposal":{"uid":"66d02c71-1590-481b-9166-f46704552f8a","biId":"7266478","wAsSubmissionId":"24ef1650-510b-4808-9127-af8e42410857","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-29T08:08:17.474Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef1650-510b-4808-9127-af8e42410857","edRefCode":"ACN3-2023-06-1650","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"EDUCATION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"editorialDiscountCode":"CWECE3","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:08:18.097Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P007","errorMessage":"Editorial code \'CWECE3\' does not exist for the journal","fieldPath":"hiConsistsOf[0].wAsEditorialDiscountCode","fieldValue":"CWECE3"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":2000,"subtotal":2000,"tax":0,"total":2000,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"CWECE3","discountType":"EditorialDiscount","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":"CWECE3","biiSalable":{"maId":"24ef1650-510b-4808-9127-af8e42410857","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-1650","wAsSubmissionId":"24ef1650-510b-4808-9127-af8e42410857","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"EDUCATION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -4988,20 +4995,20 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>Created Viax order 7256089 for PriceProposal 24ef5372-595b-4808-9127-af8e42410195</t>
+          <t>Created Viax order 7266479 for PriceProposal 24ef3755-972b-4808-9127-af8e42410658</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>7256089</t>
-        </is>
-      </c>
-      <c r="AF20" s="15" t="inlineStr">
+          <t>7266479</t>
+        </is>
+      </c>
+      <c r="AF20" s="16" t="inlineStr">
         <is>
           <t>ReSend</t>
         </is>
       </c>
-      <c r="AH20" s="15" t="inlineStr">
+      <c r="AH20" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5013,14 +5020,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef5372-595b-4808-9127-af8e42410195",
-      "edRefCode": "ACN3-2023-06-5372",
+      "submissionId": "24ef3755-972b-4808-9127-af8e42410658",
+      "edRefCode": "ACN3-2023-06-3755",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "OPINION",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5070,7 +5077,7 @@
       </c>
       <c r="AJ20" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256089 for PriceProposal 24ef5372-595b-4808-9127-af8e42410195","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256089","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef5372-595b-4808-9127-af8e42410195","version":"1.6.6-qa2.75","submissionId":"24ef5372-595b-4808-9127-af8e42410195","priceProposal":{"uid":"66ac4b66-7a54-46f1-8506-9d7a2930d7fc","biId":"7256089","wAsSubmissionId":"24ef5372-595b-4808-9127-af8e42410195","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T02:58:46.980Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef5372-595b-4808-9127-af8e42410195","edRefCode":"ACN3-2023-06-5372","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef21","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:58:47.527Z"}},"wAsCountryCode":"US","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef21","wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P004","errorMessage":"Unable to locate the referring journal from STIBO.","fieldPath":"priceProposal.wAsReferringJournalRef.wAsJournalUuid","fieldValue":""}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":640,"tax":0,"total":640,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5372-595b-4808-9127-af8e42410195","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5372","wAsSubmissionId":"24ef5372-595b-4808-9127-af8e42410195","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266479 for PriceProposal 24ef3755-972b-4808-9127-af8e42410658","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266479","priceProposal":{"uid":"66d02cad-3623-49af-8a2a-5eacc86159b2","biId":"7266479","wAsSubmissionId":"24ef3755-972b-4808-9127-af8e42410658","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-29T08:09:17.454Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef3755-972b-4808-9127-af8e42410658","edRefCode":"ACN3-2023-06-3755","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"referringJournalId":"c597beef-e45f-4cc7-b34c-0df812e2ef21","authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:09:18.240Z"}},"wAsCountryCode":"US","wAsReferringJournal":"c597beef-e45f-4cc7-b34c-0df812e2ef21","wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P004","errorMessage":"Unable to locate the referring journal from STIBO.","fieldPath":"priceProposal.wAsReferringJournalRef.wAsJournalUuid","fieldValue":""}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":1600,"subtotal":1600,"tax":0,"total":1600,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":400,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":400,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef3755-972b-4808-9127-af8e42410658","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-3755","wAsSubmissionId":"24ef3755-972b-4808-9127-af8e42410658","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5097,20 +5104,20 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>Created Viax order 7256090 for PriceProposal 24ef7904-293b-4808-9127-af8e42410597</t>
+          <t>Created Viax order 7266480 for PriceProposal 24ef4967-441b-4808-9127-af8e42410460</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>7256090</t>
-        </is>
-      </c>
-      <c r="AF21" s="15" t="inlineStr">
+          <t>7266480</t>
+        </is>
+      </c>
+      <c r="AF21" s="16" t="inlineStr">
         <is>
           <t>ReSend</t>
         </is>
       </c>
-      <c r="AH21" s="15" t="inlineStr">
+      <c r="AH21" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5122,14 +5129,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef7904-293b-4808-9127-af8e42410597",
-      "edRefCode": "ACN3-2023-06-7904",
+      "submissionId": "24ef4967-441b-4808-9127-af8e42410460",
+      "edRefCode": "ACN3-2023-06-4967",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "OPINION",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5178,7 +5185,7 @@
       </c>
       <c r="AJ21" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256090 for PriceProposal 24ef7904-293b-4808-9127-af8e42410597","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256090","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef7904-293b-4808-9127-af8e42410597","version":"1.6.6-qa2.75","submissionId":"24ef7904-293b-4808-9127-af8e42410597","priceProposal":{"uid":"66ac4b9f-1480-4739-b5b1-77405a83bcd1","biId":"7256090","wAsSubmissionId":"24ef7904-293b-4808-9127-af8e42410597","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T02:59:43.598Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef7904-293b-4808-9127-af8e42410597","edRefCode":"ACN3-2023-06-7904","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"ZZ","country":"ZZ","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T02:59:44.129Z"}},"wAsCountryCode":"ZZ","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"500","errorMessage":"Price calculation error. {}","fieldPath":"","fieldValue":""},{"errorCode":"P006","errorMessage":"Country Code Not Defined","fieldPath":"priceProposal.wAsCorrespondingAuthor.affiliations?.[0].countryCode","fieldValue":"ZZ"}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"ZZ","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef7904-293b-4808-9127-af8e42410597","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-7904","wAsSubmissionId":"24ef7904-293b-4808-9127-af8e42410597","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266480 for PriceProposal 24ef4967-441b-4808-9127-af8e42410460","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266480","priceProposal":{"uid":"66d02ce7-5866-4686-9dc6-6def32238edc","biId":"7266480","wAsSubmissionId":"24ef4967-441b-4808-9127-af8e42410460","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-29T08:10:15.763Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4967-441b-4808-9127-af8e42410460","edRefCode":"ACN3-2023-06-4967","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny@wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"ZZ","country":"ZZ","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:10:16.326Z"}},"wAsCountryCode":"ZZ","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P003","errorMessage":"Failed to find a price for wAsSalesArea = null, wAsMediaType = Digital, wAsJournalUuid = c597beef-e45f-4cc7-b34c-0df812e2ef25","fieldPath":"","fieldValue":""},{"errorCode":"P006","errorMessage":"Country Code Not Defined","fieldPath":"priceProposal.wAsCorrespondingAuthor.affiliations?.[0].countryCode","fieldValue":"ZZ"}],"wAsPricing":null,"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny@wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"ZZ","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4967-441b-4808-9127-af8e42410460","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4967","wAsSubmissionId":"24ef4967-441b-4808-9127-af8e42410460","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5205,20 +5212,20 @@
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>Created Viax order 7256091 for PriceProposal 24ef4190-617b-4808-9127-af8e42410397</t>
+          <t>Created Viax order 7266481 for PriceProposal 24ef6380-501b-4808-9127-af8e42410996</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>7256091</t>
-        </is>
-      </c>
-      <c r="AF22" s="15" t="inlineStr">
+          <t>7266481</t>
+        </is>
+      </c>
+      <c r="AF22" s="16" t="inlineStr">
         <is>
           <t>ReSend</t>
         </is>
       </c>
-      <c r="AH22" s="15" t="inlineStr">
+      <c r="AH22" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5230,14 +5237,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c69-fe0b8c44002a",
-      "submissionId": "24ef4190-617b-4808-9127-af8e42410397",
-      "edRefCode": "ACN3-2023-06-4190",
+      "submissionId": "24ef6380-501b-4808-9127-af8e42410996",
+      "edRefCode": "ACN3-2023-06-6380",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "OPINION",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5286,7 +5293,7 @@
       </c>
       <c r="AJ22" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256091 for PriceProposal 24ef4190-617b-4808-9127-af8e42410397","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256091","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef4190-617b-4808-9127-af8e42410397","version":"1.6.6-qa2.75","submissionId":"24ef4190-617b-4808-9127-af8e42410397","priceProposal":{"uid":"66ac4bda-af04-4c02-996d-4d90bf2155c4","biId":"7256091","wAsSubmissionId":"24ef4190-617b-4808-9127-af8e42410397","bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-02T03:00:42.565Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef4190-617b-4808-9127-af8e42410397","edRefCode":"ACN3-2023-06-4190","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny.wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:00:43.046Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P021","errorMessage":"Email address has invalid format","fieldPath":"priceProposal.wAsCorrespondingAuthor.email","fieldValue":"rbenny.wiley.com"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":640,"subtotal":640,"tax":0,"total":640,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":160,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny.wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef4190-617b-4808-9127-af8e42410397","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-4190","wAsSubmissionId":"24ef4190-617b-4808-9127-af8e42410397","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266481 for PriceProposal 24ef6380-501b-4808-9127-af8e42410996","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266481","priceProposal":{"uid":"66d02d21-d4d7-4b21-98d3-0a81b40a478a","biId":"7266481","wAsSubmissionId":"24ef6380-501b-4808-9127-af8e42410996","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"ReSend"},"biCreatedAt":"2024-08-29T08:11:13.695Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c69-fe0b8c44002a","submissionId":"24ef6380-501b-4808-9127-af8e42410996","edRefCode":"ACN3-2023-06-6380","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"OPINION","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"rbenny.wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:11:14.987Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P021","errorMessage":"Email address has invalid format","fieldPath":"priceProposal.wAsCorrespondingAuthor.email","fieldValue":"rbenny.wiley.com"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":1600,"subtotal":1600,"tax":0,"total":1600,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":400,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"OPINION","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":400,"discountPercentage":20,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"rbenny.wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6380-501b-4808-9127-af8e42410996","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6380","wAsSubmissionId":"24ef6380-501b-4808-9127-af8e42410996","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"OPINION","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5374,20 +5381,20 @@
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>Created Viax order 7256092 for PriceProposal 24ef6993-663b-4808-9127-af8e42410585</t>
+          <t>Created Viax order 7266482 for PriceProposal 24ef2982-630b-4808-9127-af8e42410396</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>7256092</t>
-        </is>
-      </c>
-      <c r="AF23" s="15" t="inlineStr">
+          <t>7266482</t>
+        </is>
+      </c>
+      <c r="AF23" s="16" t="inlineStr">
         <is>
           <t>REJECTED</t>
         </is>
       </c>
-      <c r="AH23" s="15" t="inlineStr">
+      <c r="AH23" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5399,14 +5406,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef6993-663b-4808-9127-af8e42410585",
-      "edRefCode": "ACN3-2023-06-6993",
+      "submissionId": "24ef2982-630b-4808-9127-af8e42410396",
+      "edRefCode": "ACN3-2023-06-2982",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5457,7 +5464,7 @@
       </c>
       <c r="AJ23" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256092 for PriceProposal 24ef6993-663b-4808-9127-af8e42410585","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256092","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef6993-663b-4808-9127-af8e42410585","version":"1.6.6-qa2.75","submissionId":"24ef6993-663b-4808-9127-af8e42410585","priceProposal":{"uid":"66ac4c14-81fc-4c71-a08b-3a5608bc9e3d","biId":"7256092","wAsSubmissionId":"24ef6993-663b-4808-9127-af8e42410585","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T03:01:39.984Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6993-663b-4808-9127-af8e42410585","edRefCode":"ACN3-2023-06-6993","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:01:40.627Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6993-663b-4808-9127-af8e42410585","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6993","wAsSubmissionId":"24ef6993-663b-4808-9127-af8e42410585","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266482 for PriceProposal 24ef2982-630b-4808-9127-af8e42410396","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266482","priceProposal":{"uid":"66d02d5c-a97b-4db3-99a8-d3fb3a307d62","biId":"7266482","wAsSubmissionId":"24ef2982-630b-4808-9127-af8e42410396","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T08:12:12.176Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2982-630b-4808-9127-af8e42410396","edRefCode":"ACN3-2023-06-2982","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:12:12.762Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":475,"tax":0,"total":475,"discountAmount":25,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2982-630b-4808-9127-af8e42410396","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-2982","wAsSubmissionId":"24ef2982-630b-4808-9127-af8e42410396","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5545,20 +5552,20 @@
       </c>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>Created Viax order 7256093 for PriceProposal 24ef9397-207b-4808-9127-af8e42410272</t>
+          <t>Created Viax order 7266483 for PriceProposal 24ef6802-160b-4808-9127-af8e42410776</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>7256093</t>
-        </is>
-      </c>
-      <c r="AF24" s="15" t="inlineStr">
+          <t>7266483</t>
+        </is>
+      </c>
+      <c r="AF24" s="16" t="inlineStr">
         <is>
           <t>WITHDRAWN</t>
         </is>
       </c>
-      <c r="AH24" s="15" t="inlineStr">
+      <c r="AH24" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5570,14 +5577,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef9397-207b-4808-9127-af8e42410272",
-      "edRefCode": "ACN3-2023-06-9397",
+      "submissionId": "24ef6802-160b-4808-9127-af8e42410776",
+      "edRefCode": "ACN3-2023-06-6802",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5628,7 +5635,7 @@
       </c>
       <c r="AJ24" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256093 for PriceProposal 24ef9397-207b-4808-9127-af8e42410272","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256093","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef9397-207b-4808-9127-af8e42410272","version":"1.6.6-qa2.75","submissionId":"24ef9397-207b-4808-9127-af8e42410272","priceProposal":{"uid":"66ac4c7a-59b5-42a8-8389-8d785f1736a5","biId":"7256093","wAsSubmissionId":"24ef9397-207b-4808-9127-af8e42410272","bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-02T03:03:22.407Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef9397-207b-4808-9127-af8e42410272","edRefCode":"ACN3-2023-06-9397","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:03:22.986Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":190,"tax":0,"total":190,"discountAmount":10,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":10,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef9397-207b-4808-9127-af8e42410272","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-9397","wAsSubmissionId":"24ef9397-207b-4808-9127-af8e42410272","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266483 for PriceProposal 24ef6802-160b-4808-9127-af8e42410776","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266483","priceProposal":{"uid":"66d02dc5-11fa-4ff9-ab24-3c79093df25d","biId":"7266483","wAsSubmissionId":"24ef6802-160b-4808-9127-af8e42410776","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-08-29T08:13:57.024Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6802-160b-4808-9127-af8e42410776","edRefCode":"ACN3-2023-06-6802","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["JCASP"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":false,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"}]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:13:57.608Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":475,"tax":0,"total":475,"discountAmount":25,"discountPercentage":5,"currencyCode":"USD","allDiscounts":[{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"JCASP","attribute":"wAsSelectedSocietyPercentageDiscountCode"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null},{"discountCode":"JCASP","discountType":"Society","discountAmount":25,"discountPercentage":5,"discountDescription":"BULK LOAD EQ2 - QA ON 12/19/2023","sapDiscountTableCode":"ZSP1","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6802-160b-4808-9127-af8e42410776","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6802","wAsSubmissionId":"24ef6802-160b-4808-9127-af8e42410776","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5726,20 +5733,20 @@
       <c r="AC25" s="11" t="n"/>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>Created Viax order 7256094 for PriceProposal 24ef2328-240b-4808-9127-af8e42410877</t>
+          <t>Created Viax order 7266484 for PriceProposal 24ef6100-368b-4808-9127-af8e42410867</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>7256094</t>
-        </is>
-      </c>
-      <c r="AF25" s="15" t="inlineStr">
+          <t>7266484</t>
+        </is>
+      </c>
+      <c r="AF25" s="16" t="inlineStr">
         <is>
           <t>DATA CORRECTION REQUIRED::PRICE DETERMINED</t>
         </is>
       </c>
-      <c r="AH25" s="15" t="inlineStr">
+      <c r="AH25" s="16" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -5751,14 +5758,14 @@
   "variables": {
     "data": {
       "requestId": "e5a1358c-2f36-4d12-8c68-fe0b8c46172a",
-      "submissionId": "24ef2328-240b-4808-9127-af8e42410877",
-      "edRefCode": "ACN3-2023-06-2328",
+      "submissionId": "24ef6100-368b-4808-9127-af8e42410867",
+      "edRefCode": "ACN3-2023-06-6100",
       "articleDOI": "",
       "journalId": "c597beef-e45f-4cc7-b34c-0df812e2ef25",
       "sourceSystem": "EM",
       "baseArticleType": "Research Article",
       "displayArticleType": "Research Article (ABC)",
-      "submissionDate": "2024-08-02",
+      "submissionDate": "2024-08-29",
       "articleAcceptedDate": "2015-09-29",
       "editorialStatus": "TBC",
       "articleTitle": "Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.",
@@ -5809,7 +5816,7 @@
       </c>
       <c r="AJ25" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7256094 for PriceProposal 24ef2328-240b-4808-9127-af8e42410877","version":"1.4.3-qa2.49","viaxPriceProposalId":"7256094","priceProposal":{"status":"SUCCESS","message":"Updated PriceProposal 24ef2328-240b-4808-9127-af8e42410877","version":"1.6.6-qa2.75","submissionId":"24ef2328-240b-4808-9127-af8e42410877","priceProposal":{"uid":"66ac4ce0-bd45-4a41-8c14-05bf7eefe876","biId":"7256094","wAsSubmissionId":"24ef2328-240b-4808-9127-af8e42410877","bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-02T03:05:04.971Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef2328-240b-4808-9127-af8e42410877","edRefCode":"ACN3-2023-06-2328","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-02","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":null,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-02T03:05:05.586Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":800,"price":200,"subtotal":200,"tax":0,"total":200,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"},{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"}]},{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":600,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef2328-240b-4808-9127-af8e42410877","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-2328","wAsSubmissionId":"24ef2328-240b-4808-9127-af8e42410877","wAsSubmissionDate":"2024-08-02","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7266484 for PriceProposal 24ef6100-368b-4808-9127-af8e42410867","version":"1.4.7-qa2.55","viaxPriceProposalId":"7266484","priceProposal":{"uid":"66d02e2d-e5e6-45fa-aa1e-1461451c7192","biId":"7266484","wAsSubmissionId":"24ef6100-368b-4808-9127-af8e42410867","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":null,"wAsReopenDateTime":null,"bpStatus":{"code":"DataCorrectionRequired"},"biCreatedAt":"2024-08-29T08:15:41.133Z","wAsPaymentType":"Undefined","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef6100-368b-4808-9127-af8e42410867","edRefCode":"ACN3-2023-06-6100","articleDOI":"","journalId":"c597beef-e45f-4cc7-b34c-0df812e2ef25","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article (ABC)","submissionDate":"2024-08-29","articleAcceptedDate":"2015-09-29","editorialStatus":"TBC","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":["EANM"],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"90210","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"discountContext":[]}],"auAudit":{"updatedAt":{"dateTime":"2024-08-29T08:15:41.856Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[{"errorCode":"P030","errorMessage":"The discount code \'EANM\' does not exist.","fieldPath":"wAsDiscountCodes[0].discountCode","fieldValue":"EANM"}],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":2000,"price":500,"subtotal":500,"tax":0,"total":500,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[{"discountCode":"EANM","discountType":"Society","discountAmount":null,"discountPercentage":null,"discountDescription":null,"sapDiscountTableCode":null,"isPercentageDiscount":null,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[]},{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null,"discountContext":[{"value":"c597beef-e45f-4cc7-b34c-0df812e2ef25","attribute":"wAsJournalUuid"},{"value":"RESEARCH ARTICLE","attribute":"wAsBaseArticleType"}]}],"appliedDiscounts":[{"discountCode":"","discountType":"ArticleType","discountAmount":1500,"discountPercentage":75,"discountDescription":null,"sapDiscountTableCode":"ZAPA","isPercentageDiscount":true,"isStackedDiscount":null,"institutionId":null,"institutionName":null,"institutionIdType":null,"woaCode":null,"consortiumCode":null}]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef6100-368b-4808-9127-af8e42410867","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-6100","wAsSubmissionId":"24ef6100-368b-4808-9127-af8e42410867","wAsSubmissionDate":"2024-08-29","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"TBC","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article (ABC)","ibrProduct":{"maId":"CAM4","maName":"Cancer Medicine","wAsJournalUuid":"c597beef-e45f-4cc7-b34c-0df812e2ef25","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20457634","wAsFlipDate":null,"wAsJournalTitle":"Cancer Medicine","wAsJournalGroupCode":"CAM4","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"cancermed@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
     </row>
@@ -5826,7 +5833,7 @@
   </sheetPr>
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -6026,54 +6033,54 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>20240809182435Test</t>
+          <t>20240816190247Test</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>20240809182435Auto</t>
+          <t>20240816190247Auto</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>20240809182435@Wiley.com</t>
+          <t>20240816190247@Wiley.com</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f11732200</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f84775519</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>3213807</t>
+          <t>3213873</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Created Viax order 3213807 for AS order 20240809182435</t>
-        </is>
-      </c>
-      <c r="S2" s="16" t="inlineStr">
+          <t>Created Viax order 3213873 for AS order 20240816190247</t>
+        </is>
+      </c>
+      <c r="S2" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 03b77b24-24e1-40f0-ad8a-83c8e1fb3723","Using soldTo : 03b77b24-24e1-40f0-ad8a-83c8e1fb3723","Using billTo: 03b77b24-24e1-40f0-ad8a-83c8e1fb3723","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213807 for AS order 20240809182435","version":"1.3.3-qa2.92","biId":"3213807"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 9ca90171-81f4-4d1b-9528-8a34490d50be","Using soldTo : 9ca90171-81f4-4d1b-9528-8a34490d50be","Using billTo: 9ca90171-81f4-4d1b-9528-8a34490d50be","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213873 for AS order 20240816190247","version":"1.3.5-qa2.94","biId":"3213873"}}'}}}</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e297a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182435 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-09T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f11732200\" title: \"Secrets of nature\" dhId: \"e0c3394c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809182435Test\" lastName: \"20240809182435Auto\" email: \"20240809182435@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809182435Test\" lastName: \"20240809182435Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809182435@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e297a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190247 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f84775519\" title: \"Secrets of nature\" dhId: \"e0c4569c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" email: \"20240816190247@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240816190247Test\" lastName: \"20240816190247Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240816190247@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e198a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:35.582</t>
+          <t>2024-08-16 19:02:47.871</t>
         </is>
       </c>
     </row>
@@ -6140,54 +6147,54 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>20240809182437Test</t>
+          <t>20240816190249Test</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>20240809182437Auto</t>
+          <t>20240816190249Auto</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>20240809182437@Wiley.com</t>
+          <t>20240816190249@Wiley.com</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f85309375</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f82547776</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>3213808</t>
+          <t>3213874</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Created Viax order 3213808 for AS order 20240809182437</t>
-        </is>
-      </c>
-      <c r="S3" s="16" t="inlineStr">
+          <t>Created Viax order 3213874 for AS order 20240816190249</t>
+        </is>
+      </c>
+      <c r="S3" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP 93ea3a0b-44ec-4268-aeb7-e0b5e3f46f8b","Using soldTo : 93ea3a0b-44ec-4268-aeb7-e0b5e3f46f8b","Using billTo: 93ea3a0b-44ec-4268-aeb7-e0b5e3f46f8b","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213808 for AS order 20240809182437","version":"1.3.3-qa2.92","biId":"3213808"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using soldTo : db7230bc-e352-4a3c-a64b-56d3a5bf268c","Using billTo: db7230bc-e352-4a3c-a64b-56d3a5bf268c","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213874 for AS order 20240816190249","version":"1.3.5-qa2.94","biId":"3213874"}}'}}}</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e415a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-09T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182437 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f85309375\" title: \"Secrets of volcano\" dhId: \"e0c2088c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809182437Test\" lastName: \"20240809182437Auto\" email: \"20240809182437@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809182437Test\" lastName:\"20240809182437Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809182437@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e415a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190249 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f82547776\" title: \"Secrets of volcano\" dhId: \"e0c3220c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240816190249Test\" lastName: \"20240816190249Auto\" email: \"20240816190249@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240816190249Test\" lastName:\"20240816190249Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240816190249@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e527a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:37.239</t>
+          <t>2024-08-16 19:02:49.665</t>
         </is>
       </c>
     </row>
@@ -6254,54 +6261,54 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>20240809182438Test</t>
+          <t>20240816190251Test</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>20240809182438Auto</t>
+          <t>20240816190251Auto</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>20240809182438@Wiley.com</t>
+          <t>20240816190251@Wiley.com</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f76633514</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f51045539</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>3213809</t>
+          <t>3213875</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Created Viax order 3213809 for AS order 20240809182438</t>
-        </is>
-      </c>
-      <c r="S4" s="16" t="inlineStr">
+          <t>Created Viax order 3213875 for AS order 20240816190251</t>
+        </is>
+      </c>
+      <c r="S4" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP defb4fc8-9aa5-4534-9b32-c6267fce219b","Using soldTo : defb4fc8-9aa5-4534-9b32-c6267fce219b","Using billTo: defb4fc8-9aa5-4534-9b32-c6267fce219b","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213809 for AS order 20240809182438","version":"1.3.3-qa2.92","biId":"3213809"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP c56044fa-84e5-4134-b919-d954b8524a7e","Using soldTo : c56044fa-84e5-4134-b919-d954b8524a7e","Using billTo: c56044fa-84e5-4134-b919-d954b8524a7e","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213875 for AS order 20240816190251","version":"1.3.5-qa2.94","biId":"3213875"}}'}}}</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e445a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182438 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f76633514\" title: \"Secrets of nature\" dhId: \"e0c4445c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809182438Test\" lastName: \"20240809182438Auto\" email: \"20240809182438@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-09 08:00:00\" } billingAddress: { firstName: \"20240809182438Test\" lastName: \"20240809182438Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809182438@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e445a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190251 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51045539\" title: \"Secrets of nature\" dhId: \"e0c1151c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" email: \"20240816190251@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240816190251Test\" lastName: \"20240816190251Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240816190251@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e873a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:38.836</t>
+          <t>2024-08-16 19:02:51.200</t>
         </is>
       </c>
     </row>
@@ -6368,54 +6375,54 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>20240809182444Test</t>
+          <t>20240816190256Test</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>20240809182444Auto</t>
+          <t>20240816190256Auto</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>20240809182444@Wiley.com</t>
+          <t>20240816190256@Wiley.com</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f74756097</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f27834654</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>3213813</t>
+          <t>3213879</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Created Viax order 3213813 for AS order 20240809182444</t>
-        </is>
-      </c>
-      <c r="S5" s="16" t="inlineStr">
+          <t>Created Viax order 3213879 for AS order 20240816190256</t>
+        </is>
+      </c>
+      <c r="S5" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP b69c81b3-ee37-4a50-b9f9-b86ab679020e","Using soldTo : b69c81b3-ee37-4a50-b9f9-b86ab679020e","Using billTo: b69c81b3-ee37-4a50-b9f9-b86ab679020e","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213813 for AS order 20240809182444","version":"1.3.3-qa2.92","biId":"3213813"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Creating BillTo","Sending BillTo to SAP db9caa52-3038-4d87-8158-9f847e8c63d4","Using soldTo : db9caa52-3038-4d87-8158-9f847e8c63d4","Using billTo: db9caa52-3038-4d87-8158-9f847e8c63d4","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213879 for AS order 20240816190256","version":"1.3.5-qa2.94","biId":"3213879"}}'}}}</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e142a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182444 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-09T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-09\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f74756097\" title: \"Secrets of nature\" dhId: \"e0c7293c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809182444Test\" lastName: \"20240809182444Auto\" email: \"20240809182444@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809182444Test\" lastName: \"20240809182444Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809182444@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e142a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190256 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f27834654\" title: \"Secrets of nature\" dhId: \"e0c3582c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" email: \"20240816190256@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240816190256Test\" lastName: \"20240816190256Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240816190256@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e366a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:44.577</t>
+          <t>2024-08-16 19:02:56.916</t>
         </is>
       </c>
     </row>
@@ -6497,39 +6504,39 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f86588840</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f62879150</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>3213812</t>
+          <t>3213878</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Created Viax order 3213812 for AS order 20240809182443</t>
-        </is>
-      </c>
-      <c r="S6" s="16" t="inlineStr">
+          <t>Created Viax order 3213878 for AS order 20240816190255</t>
+        </is>
+      </c>
+      <c r="S6" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Using billTo: 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213812 for AS order 20240809182443","version":"1.3.3-qa2.92","biId":"3213812"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Using billTo: 3f7431cb-eef3-49fa-bdfc-5d16128c6fd5","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213878 for AS order 20240816190255","version":"1.3.5-qa2.94","biId":"3213878"}}'}}}</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e459a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182443 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-09T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f86588840\" title: \"Secrets of nature\" dhId: \"e0c4479c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" email: \"20240809175918@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809175918@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e459a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2023-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190255 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Invoice\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"GBP\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2023-12-31\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f62879150\" title: \"Secrets of nature\" dhId: \"e0c7856c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"RRO39999\" jpcmsArticleIdentifier: \"RRO.39999.ART\" articleDOI: \"10.1111/RRO.39999\" } soldToDetails: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" email: \"20240809175918@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1180.00, billingAddress: { firstName: \"20240809175918Test\" lastName: \"20240809175918Auto\" streetAddress: [\"389 Nepean Hwy\"] addressLocality:\"Edison\" addressRegion: \"NJ\" countryCode: \"GB\" postalCode: \"08817\" phoneNumber: \"06667778888\" email: \"20240809175918@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e572a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:43.265</t>
+          <t>2024-08-16 19:02:55.481</t>
         </is>
       </c>
     </row>
@@ -6611,39 +6618,39 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f73092863</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f16859253</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>3213811</t>
+          <t>3213877</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Created Viax order 3213811 for AS order 20240809182441</t>
-        </is>
-      </c>
-      <c r="S7" s="16" t="inlineStr">
+          <t>Created Viax order 3213877 for AS order 20240816190254</t>
+        </is>
+      </c>
+      <c r="S7" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 9be953a5-d4ea-4149-a439-801fe3371d6a","Using billTo: 9be953a5-d4ea-4149-a439-801fe3371d6a","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213811 for AS order 20240809182441","version":"1.3.3-qa2.92","biId":"3213811"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 9be953a5-d4ea-4149-a439-801fe3371d6a","Using billTo: 9be953a5-d4ea-4149-a439-801fe3371d6a","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213877 for AS order 20240816190254","version":"1.3.5-qa2.94","biId":"3213877"}}'}}}</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e434a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-09T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182441 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f73092863\" title: \"Secrets of volcano\" dhId: \"e0c9982c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809175920Test\" lastName: \"20240809175920Auto\" email: \"20240809175920@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809175920Test\" lastName:\"20240809175920Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809175920@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e434a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2024-08-16T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190254 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"CreditCard\" upfrontPaymentDate: \"2023-01-26T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" poNumber: \"CC order form\" specialNotes: \"CH CC order form validation\" apc: 2300.25 appliedDiscount: 0.00 discountType: \"Institutional\" estimatedTax: 0.00 totalChargedAmount: 2300.25 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CH\" journalId: \"9c9a4e6b-fef6-4a2f-9ed4-804e944dd14d\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f16859253\" title: \"Secrets of volcano\" dhId: \"e0c3651c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"TJP38363\" jpcmsArticleIdentifier: \"TJP.38363.ART\" articleDOI: \"10.1111/tjp.38363\" } soldToDetails: { firstName: \"20240809175920Test\" lastName: \"20240809175920Auto\" email: \"20240809175920@Wiley.com\" userId: \"ALM-eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\", participantId:\"eb1b9579-2b3c-4c4c-8a45-cca0bbb747e7\" } billToDetails: [ { chargedAmount: 2300.25 creditCard: { creditCardToken: \"S5555555718124449\", creditCardTypeID: \"M\", creditCardType: \"masTercarD\", partialCardNumber: \"555555xxxxxx4449\", expirationDate: \"1234\", bankId: \"U\", bankName: \"UNKNOWN\", authCode: \"bxERe4\", creditCardAuthDate: \"2023-07-03T15:04:06.000+00:00\" }, billingAddress: { firstName: \"20240809175920Test\" lastName:\"20240809175920Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"Dufourstrasse 40a\"] addressLocality: \"St. Gallen\" addressRegion: \"SG\" countryCode: \"CH\" postalCode: \"9000\" phoneNumber: \"8299729725\" email: \"20240809175920@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e832a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:41.935</t>
+          <t>2024-08-16 19:02:54.193</t>
         </is>
       </c>
     </row>
@@ -6725,39 +6732,39 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f54572045</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f55866607</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>3213810</t>
+          <t>3213876</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>Created Viax order 3213810 for AS order 20240809182440</t>
-        </is>
-      </c>
-      <c r="S8" s="16" t="inlineStr">
+          <t>Created Viax order 3213876 for AS order 20240816190252</t>
+        </is>
+      </c>
+      <c r="S8" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 58af0986-6542-4f02-84c5-faff2f9041c7","Using billTo: 58af0986-6542-4f02-84c5-faff2f9041c7","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213810 for AS order 20240809182440","version":"1.3.3-qa2.92","biId":"3213810"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 58af0986-6542-4f02-84c5-faff2f9041c7","Using billTo: 58af0986-6542-4f02-84c5-faff2f9041c7","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213876 for AS order 20240816190252","version":"1.3.5-qa2.94","biId":"3213876"}}'}}}</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e743a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182440 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f54572045\" title: \"Secrets of nature\" dhId: \"e0c6429c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" email: \"20240809175921@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-09 08:00:00\" } billingAddress: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809175921@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e743a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\"eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-09-12T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190252 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2023-09-12T15:00:14-05\" paymentDate: \"2023-09-12T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Alipay\" upfrontPaymentDate: \"2023-09-12T15:00:14-05\" upfrontPaymentStatus: \"Paid\" onesourceTaxCode: \"sAPC\" apc: 900.00 appliedDiscount: 0.00 estimatedTax: 0.00 totalChargedAmount: 900.00 currency: \"USD\" taxExceptionNumber: \"40180089023\" taxExceptionExpirationDate: \"2024-10-26\" vatIdNumber: \"\" countryCode: \"CN\" journalId: \"c597beef-e45f-4cc7-b34c-0df812e2ef25\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f55866607\" title: \"Secrets of nature\" dhId: \"e0c4870c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"CAM448363\" jpcmsArticleIdentifier: \"CAM4.48363.ART\" articleDOI: \"10.1111/CAM4.48363\" } soldToDetails: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" email: \"20240809175921@Wiley.com\" userId: \"ALM-77d825fc-4df8-47b4-b941-029ff74bfc2b\" participantId: \"77d825fc-4df8-47b4-b941-029ff74bfc2b\" } billToDetails: [ { chargedAmount: 900.00 AlipayDetails: { alipayOrderNumber: \"23154811\", alipayPaymentNumber: \"87540622\", alipayPaymentDate:\"2024-08-16 08:00:00\" } billingAddress: { firstName: \"20240809175921Test\" lastName: \"20240809175921Auto\" organization: \"University of Edinburgh\" department: \"School of GeoSciences\" institution: \"Grant Institute\" streetAddress: [\"No. 1 Xikang Road\"] addressLocality: \"Harbin\" addressRegion: \"100\" countryCode: \"CN\" postalCode: \"210024\" phoneNumber: \"0703503263\" email: \"20240809175921@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e617a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:40.558</t>
+          <t>2024-08-16 19:02:52.820</t>
         </is>
       </c>
     </row>
@@ -6839,39 +6846,39 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>11ca99f1-8a00-4cb3-123e-222f94681782</t>
+          <t>11ca99f1-8a00-4cb3-123e-222f51013723</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>3213814</t>
+          <t>3213880</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Created Viax order 3213814 for AS order 20240809182446</t>
-        </is>
-      </c>
-      <c r="S9" s="16" t="inlineStr">
+          <t>Created Viax order 3213880 for AS order 20240816190258</t>
+        </is>
+      </c>
+      <c r="S9" s="15" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 19d4ae48-402a-46e7-be58-753966fbec09","Using billTo: 19d4ae48-402a-46e7-be58-753966fbec09","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213814 for AS order 20240809182446","version":"1.3.3-qa2.92","biId":"3213814"}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":["Both sold-to and bill-to exist inside Viax.","Using soldTo : 19d4ae48-402a-46e7-be58-753966fbec09","Using billTo: 19d4ae48-402a-46e7-be58-753966fbec09","Creating the viax order"],"result":{"status":"SUCCESS","message":"Created Viax order 3213880 for AS order 20240816190258","version":"1.3.5-qa2.94","biId":"3213880"}}'}}}</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
           <t>{
-  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e729a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240809182446 submittedDate: \"2024-08-09T15:00:14-05\" createdDate: \"2024-08-09T15:00:14-05\" cancelDate: \"2024-08-09T15:00:14-05\" paymentDate: \"2024-08-09T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-09T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-09\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f94681782\" title: \"Secrets of nature\" dhId: \"e0c5736c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" email: \"20240809181925@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809181925@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e729a\" } } ] } }\t) { status data\t}}"
+  "query": "mutation placeOrder {\ttestFunction( input: { name: \"receive-event-from-kafka\" data: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" eventType: \"order.submitted\" source: \"as-order-service\" specVersion: \"1.0\" eventDate: \"2022-11-01T12:08:56.235-0700\" dataContentType: \"application/json\" orderUniqueId: 20240816190258 submittedDate: \"2024-08-16T15:00:14-05\" createdDate: \"2024-08-16T15:00:14-05\" cancelDate: \"2024-08-16T15:00:14-05\" paymentDate: \"2024-08-16T15:00:14-05\" revenueModel: \"OA\" type: \"AuthorPaid\" paymentMethod: \"Proforma\" upfrontPaymentDate: \"2024-08-16T15:00:14-05\" upfrontPaymentStatus: \"Unpaid\" onesourceTaxCode: \"sAPC\" apc: 1180.00 appliedDiscount: 100.00 discountType: \"Society\" discountCode: \"ZSV1\" estimatedTax: 236.00 totalChargedAmount: 1416.00 currency: \"EUR\" taxExceptionNumber: \"\" taxExceptionExpirationDate: \"2024-08-16\" vatIdNumber: \"\" countryCode: \"GB\" journalId: \"1b28a8b9-067b-4ce9-b981-e8eabe16e0a7\" article: { submissionId: \"11ca99f1-8a00-4cb3-123e-222f51013723\" title: \"Secrets of nature\" dhId: \"e0c8024c-ba2c-401d-b2a6-3fb3a59b3c00\" jpcmsAID: \"AND38363\" jpcmsArticleIdentifier: \"AND.38363.ART\" articleDOI: \"10.1111/AND.38363\" } soldToDetails: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" email: \"20240809181925@Wiley.com\" userId: \"ALM-6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" participantId: \"6b045551-a5fc-4fdb-9a43-ae56ece8f82a\" } billToDetails: [ { chargedAmount: 1416.00, billingAddress: { firstName: \"20240809181925Test\" lastName: \"20240809181925Auto\" streetAddress: [\"university of edinburgh\"] addressLocality: \"Swindon\" addressRegion: \"WIL\" countryCode: \"GB\" postalCode: \"SN4 3FR\" phoneNumber: \"8299729729\" email: \"20240809181925@Wiley.com\" } organization: { id: \"df1e950b-a1d7-45bf-acab-42f7ed3e705a\" } } ] } }\t) { status data\t}}"
 }</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>2024-08-09 18:24:46.159</t>
+          <t>2024-08-16 19:02:58.389</t>
         </is>
       </c>
     </row>

</xml_diff>